<commit_message>
Automatic update of 16/05/2024 at 04:03
</commit_message>
<xml_diff>
--- a/Indicadores OPI-CETG rev 28.04.24 v3.xlsx
+++ b/Indicadores OPI-CETG rev 28.04.24 v3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\03. Job\05. CONSULTORIAS\13. MEF\FIDT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\03. Job\05. CONSULTORIAS\13. MEF\FIDT_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EA9354-6B2B-435E-AA09-025587A802E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EF7F54-0504-4114-83F4-0E3279C67362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{A4291CEF-37A6-4732-90F4-77F55B4FD4D0}"/>
   </bookViews>
@@ -63,7 +63,7 @@
     <definedName name="_ftnref4" localSheetId="4">Indicadores_v3!#REF!</definedName>
     <definedName name="_ftnref4" localSheetId="2">Indicadores_v4!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="292">
   <si>
     <t>SERVICIOS</t>
   </si>
@@ -1083,9 +1083,6 @@
     <t>Porcentaje de población con alguna dificultad permanente</t>
   </si>
   <si>
-    <t xml:space="preserve">Porcentaje Población que no tiene seguro de salud </t>
-  </si>
-  <si>
     <t>Porcentaje de desnutrición crónica en niños menores de 5 años</t>
   </si>
   <si>
@@ -1204,13 +1201,22 @@
   </si>
   <si>
     <t>¿Lo desagrego por urbano/rural?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Porcentaje de población que no tiene seguro de salud </t>
+  </si>
+  <si>
+    <t>Años promedios de escolaridad de 3 a 17 años</t>
+  </si>
+  <si>
+    <t>VF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1343,6 +1349,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1383,7 +1411,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1493,7 +1521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -1766,15 +1794,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1784,18 +1803,36 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1823,21 +1860,6 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1847,15 +1869,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1865,12 +1896,6 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1881,6 +1906,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2257,8 +2312,8 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="117"/>
-      <c r="B3" s="114" t="s">
+      <c r="A3" s="106"/>
+      <c r="B3" s="103" t="s">
         <v>99</v>
       </c>
       <c r="C3" s="31"/>
@@ -2275,8 +2330,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="114"/>
+      <c r="A4" s="106"/>
+      <c r="B4" s="103"/>
       <c r="C4" s="31"/>
       <c r="D4" s="23" t="s">
         <v>65</v>
@@ -2288,8 +2343,8 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="117"/>
-      <c r="B5" s="114"/>
+      <c r="A5" s="106"/>
+      <c r="B5" s="103"/>
       <c r="C5" s="31">
         <v>1.1000000000000001</v>
       </c>
@@ -2307,8 +2362,8 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="117"/>
-      <c r="B6" s="114" t="s">
+      <c r="A6" s="106"/>
+      <c r="B6" s="103" t="s">
         <v>68</v>
       </c>
       <c r="C6" s="31">
@@ -2326,8 +2381,8 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="117"/>
-      <c r="B7" s="114"/>
+      <c r="A7" s="106"/>
+      <c r="B7" s="103"/>
       <c r="C7" s="31">
         <v>2.2000000000000002</v>
       </c>
@@ -2343,8 +2398,8 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="117"/>
-      <c r="B8" s="114" t="s">
+      <c r="A8" s="106"/>
+      <c r="B8" s="103" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="31">
@@ -2364,8 +2419,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="117"/>
-      <c r="B9" s="114"/>
+      <c r="A9" s="106"/>
+      <c r="B9" s="103"/>
       <c r="C9" s="31"/>
       <c r="D9" s="23" t="s">
         <v>117</v>
@@ -2380,8 +2435,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="117"/>
-      <c r="B10" s="114"/>
+      <c r="A10" s="106"/>
+      <c r="B10" s="103"/>
       <c r="C10" s="31"/>
       <c r="D10" s="23" t="s">
         <v>105</v>
@@ -2391,13 +2446,13 @@
       </c>
       <c r="F10" s="56"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="115" t="s">
+      <c r="H10" s="104" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="117"/>
-      <c r="B11" s="114"/>
+      <c r="A11" s="106"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="31"/>
       <c r="D11" s="23" t="s">
         <v>50</v>
@@ -2407,11 +2462,11 @@
       </c>
       <c r="F11" s="56"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="115"/>
+      <c r="H11" s="104"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="117"/>
-      <c r="B12" s="114"/>
+      <c r="A12" s="106"/>
+      <c r="B12" s="103"/>
       <c r="C12" s="31">
         <v>3.2</v>
       </c>
@@ -2429,8 +2484,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="117"/>
-      <c r="B13" s="114"/>
+      <c r="A13" s="106"/>
+      <c r="B13" s="103"/>
       <c r="C13" s="31">
         <v>12.1</v>
       </c>
@@ -2446,8 +2501,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="117"/>
-      <c r="B14" s="114"/>
+      <c r="A14" s="106"/>
+      <c r="B14" s="103"/>
       <c r="C14" s="31">
         <v>12.2</v>
       </c>
@@ -2463,8 +2518,8 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="117"/>
-      <c r="B15" s="114"/>
+      <c r="A15" s="106"/>
+      <c r="B15" s="103"/>
       <c r="C15" s="31">
         <v>12.3</v>
       </c>
@@ -2480,8 +2535,8 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="117"/>
-      <c r="B16" s="114" t="s">
+      <c r="A16" s="106"/>
+      <c r="B16" s="103" t="s">
         <v>67</v>
       </c>
       <c r="C16" s="31"/>
@@ -2495,8 +2550,8 @@
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="117"/>
-      <c r="B17" s="114"/>
+      <c r="A17" s="106"/>
+      <c r="B17" s="103"/>
       <c r="C17" s="31"/>
       <c r="D17" s="23" t="s">
         <v>108</v>
@@ -2508,8 +2563,8 @@
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="117"/>
-      <c r="B18" s="114"/>
+      <c r="A18" s="106"/>
+      <c r="B18" s="103"/>
       <c r="C18" s="31"/>
       <c r="D18" s="23" t="s">
         <v>109</v>
@@ -2521,8 +2576,8 @@
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="117"/>
-      <c r="B19" s="114"/>
+      <c r="A19" s="106"/>
+      <c r="B19" s="103"/>
       <c r="C19" s="31"/>
       <c r="D19" s="23" t="s">
         <v>110</v>
@@ -2534,8 +2589,8 @@
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="117"/>
-      <c r="B20" s="114"/>
+      <c r="A20" s="106"/>
+      <c r="B20" s="103"/>
       <c r="C20" s="31"/>
       <c r="D20" s="23" t="s">
         <v>111</v>
@@ -2547,8 +2602,8 @@
       <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="117"/>
-      <c r="B21" s="114"/>
+      <c r="A21" s="106"/>
+      <c r="B21" s="103"/>
       <c r="C21" s="31"/>
       <c r="D21" s="23" t="s">
         <v>112</v>
@@ -2563,8 +2618,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="117"/>
-      <c r="B22" s="114" t="s">
+      <c r="A22" s="106"/>
+      <c r="B22" s="103" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="35">
@@ -2587,8 +2642,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="117"/>
-      <c r="B23" s="114"/>
+      <c r="A23" s="106"/>
+      <c r="B23" s="103"/>
       <c r="C23" s="35">
         <v>5.2</v>
       </c>
@@ -2609,8 +2664,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="117"/>
-      <c r="B24" s="114"/>
+      <c r="A24" s="106"/>
+      <c r="B24" s="103"/>
       <c r="C24" s="31">
         <v>5.3</v>
       </c>
@@ -2628,8 +2683,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="117"/>
-      <c r="B25" s="114"/>
+      <c r="A25" s="106"/>
+      <c r="B25" s="103"/>
       <c r="C25" s="35">
         <v>5.4</v>
       </c>
@@ -2650,8 +2705,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="117"/>
-      <c r="B26" s="114"/>
+      <c r="A26" s="106"/>
+      <c r="B26" s="103"/>
       <c r="C26" s="35"/>
       <c r="D26" s="41" t="s">
         <v>53</v>
@@ -2666,8 +2721,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="117"/>
-      <c r="B27" s="114"/>
+      <c r="A27" s="106"/>
+      <c r="B27" s="103"/>
       <c r="C27" s="35"/>
       <c r="D27" s="41" t="s">
         <v>54</v>
@@ -2682,8 +2737,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="117"/>
-      <c r="B28" s="114" t="s">
+      <c r="A28" s="106"/>
+      <c r="B28" s="103" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="35">
@@ -2706,8 +2761,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="117"/>
-      <c r="B29" s="114"/>
+      <c r="A29" s="106"/>
+      <c r="B29" s="103"/>
       <c r="C29" s="31"/>
       <c r="D29" s="41" t="s">
         <v>51</v>
@@ -2722,8 +2777,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="117"/>
-      <c r="B30" s="114"/>
+      <c r="A30" s="106"/>
+      <c r="B30" s="103"/>
       <c r="C30" s="31"/>
       <c r="D30" s="41" t="s">
         <v>52</v>
@@ -2738,8 +2793,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="117"/>
-      <c r="B31" s="114" t="s">
+      <c r="A31" s="106"/>
+      <c r="B31" s="103" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="31">
@@ -2757,8 +2812,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="117"/>
-      <c r="B32" s="114"/>
+      <c r="A32" s="106"/>
+      <c r="B32" s="103"/>
       <c r="C32" s="31">
         <v>7.2</v>
       </c>
@@ -2774,8 +2829,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="117"/>
-      <c r="B33" s="114" t="s">
+      <c r="A33" s="106"/>
+      <c r="B33" s="103" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="35">
@@ -2798,8 +2853,8 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="117"/>
-      <c r="B34" s="114"/>
+      <c r="A34" s="106"/>
+      <c r="B34" s="103"/>
       <c r="C34" s="35">
         <v>8.1999999999999993</v>
       </c>
@@ -2820,8 +2875,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="117"/>
-      <c r="B35" s="114"/>
+      <c r="A35" s="106"/>
+      <c r="B35" s="103"/>
       <c r="C35" s="35">
         <v>8.3000000000000007</v>
       </c>
@@ -2842,8 +2897,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="117"/>
-      <c r="B36" s="114"/>
+      <c r="A36" s="106"/>
+      <c r="B36" s="103"/>
       <c r="C36" s="32">
         <v>8.1</v>
       </c>
@@ -2864,8 +2919,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="117"/>
-      <c r="B37" s="114"/>
+      <c r="A37" s="106"/>
+      <c r="B37" s="103"/>
       <c r="C37" s="32">
         <v>8.1999999999999993</v>
       </c>
@@ -2886,8 +2941,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="117"/>
-      <c r="B38" s="114"/>
+      <c r="A38" s="106"/>
+      <c r="B38" s="103"/>
       <c r="C38" s="32">
         <v>8.3000000000000007</v>
       </c>
@@ -2908,8 +2963,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="117"/>
-      <c r="B39" s="114"/>
+      <c r="A39" s="106"/>
+      <c r="B39" s="103"/>
       <c r="C39" s="32"/>
       <c r="D39" s="22" t="s">
         <v>72</v>
@@ -2921,8 +2976,8 @@
       <c r="G39" s="43"/>
     </row>
     <row r="40" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="117"/>
-      <c r="B40" s="114" t="s">
+      <c r="A40" s="106"/>
+      <c r="B40" s="103" t="s">
         <v>34</v>
       </c>
       <c r="C40" s="31">
@@ -2940,8 +2995,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="117"/>
-      <c r="B41" s="114"/>
+      <c r="A41" s="106"/>
+      <c r="B41" s="103"/>
       <c r="C41" s="31">
         <v>9.1999999999999993</v>
       </c>
@@ -2957,8 +3012,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="117"/>
-      <c r="B42" s="114"/>
+      <c r="A42" s="106"/>
+      <c r="B42" s="103"/>
       <c r="C42" s="31"/>
       <c r="D42" s="23" t="s">
         <v>59</v>
@@ -2970,8 +3025,8 @@
       <c r="G42" s="12"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="117"/>
-      <c r="B43" s="114"/>
+      <c r="A43" s="106"/>
+      <c r="B43" s="103"/>
       <c r="C43" s="31"/>
       <c r="D43" s="22" t="s">
         <v>86</v>
@@ -2986,8 +3041,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="117"/>
-      <c r="B44" s="114"/>
+      <c r="A44" s="106"/>
+      <c r="B44" s="103"/>
       <c r="C44" s="31"/>
       <c r="D44" s="22" t="s">
         <v>87</v>
@@ -3002,8 +3057,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="117"/>
-      <c r="B45" s="114"/>
+      <c r="A45" s="106"/>
+      <c r="B45" s="103"/>
       <c r="C45" s="31"/>
       <c r="D45" s="22" t="s">
         <v>100</v>
@@ -3018,10 +3073,10 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="117" t="s">
+      <c r="A46" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="116" t="s">
+      <c r="B46" s="105" t="s">
         <v>114</v>
       </c>
       <c r="C46" s="34">
@@ -3042,8 +3097,8 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="117"/>
-      <c r="B47" s="116"/>
+      <c r="A47" s="106"/>
+      <c r="B47" s="105"/>
       <c r="C47" s="34">
         <v>11.2</v>
       </c>
@@ -3062,8 +3117,8 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="117"/>
-      <c r="B48" s="116"/>
+      <c r="A48" s="106"/>
+      <c r="B48" s="105"/>
       <c r="C48" s="34">
         <v>11.3</v>
       </c>
@@ -3082,8 +3137,8 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="117"/>
-      <c r="B49" s="116"/>
+      <c r="A49" s="106"/>
+      <c r="B49" s="105"/>
       <c r="C49" s="34"/>
       <c r="D49" s="22" t="s">
         <v>66</v>
@@ -3098,8 +3153,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="117"/>
-      <c r="B50" s="116"/>
+      <c r="A50" s="106"/>
+      <c r="B50" s="105"/>
       <c r="C50" s="34"/>
       <c r="D50" s="22" t="s">
         <v>63</v>
@@ -3114,10 +3169,10 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="113" t="s">
+      <c r="A51" s="102" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="113"/>
+      <c r="B51" s="102"/>
       <c r="C51" s="62"/>
       <c r="D51" s="52" t="s">
         <v>115</v>
@@ -3130,8 +3185,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="113"/>
-      <c r="B52" s="113"/>
+      <c r="A52" s="102"/>
+      <c r="B52" s="102"/>
       <c r="C52" s="62"/>
       <c r="D52" s="52" t="s">
         <v>89</v>
@@ -3142,8 +3197,8 @@
       <c r="F52" s="47"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="113"/>
-      <c r="B53" s="113"/>
+      <c r="A53" s="102"/>
+      <c r="B53" s="102"/>
       <c r="C53" s="62"/>
       <c r="D53" s="54" t="s">
         <v>38</v>
@@ -3154,8 +3209,8 @@
       <c r="F53" s="47"/>
     </row>
     <row r="54" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="113"/>
-      <c r="B54" s="113"/>
+      <c r="A54" s="102"/>
+      <c r="B54" s="102"/>
       <c r="C54" s="62"/>
       <c r="D54" s="52" t="s">
         <v>81</v>
@@ -3166,41 +3221,41 @@
       <c r="F54" s="47"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="104" t="s">
+      <c r="A55" s="107" t="s">
         <v>126</v>
       </c>
-      <c r="B55" s="104"/>
-      <c r="C55" s="104"/>
-      <c r="D55" s="104"/>
-      <c r="E55" s="104"/>
+      <c r="B55" s="107"/>
+      <c r="C55" s="107"/>
+      <c r="D55" s="107"/>
+      <c r="E55" s="107"/>
       <c r="F55" s="47"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="105"/>
-      <c r="B56" s="105"/>
-      <c r="C56" s="105"/>
-      <c r="D56" s="105"/>
-      <c r="E56" s="105"/>
+      <c r="A56" s="108"/>
+      <c r="B56" s="108"/>
+      <c r="C56" s="108"/>
+      <c r="D56" s="108"/>
+      <c r="E56" s="108"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="105"/>
-      <c r="B57" s="105"/>
-      <c r="C57" s="105"/>
-      <c r="D57" s="105"/>
-      <c r="E57" s="105"/>
+      <c r="A57" s="108"/>
+      <c r="B57" s="108"/>
+      <c r="C57" s="108"/>
+      <c r="D57" s="108"/>
+      <c r="E57" s="108"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="106"/>
-      <c r="B58" s="106"/>
-      <c r="C58" s="106"/>
-      <c r="D58" s="106"/>
-      <c r="E58" s="106"/>
+      <c r="A58" s="109"/>
+      <c r="B58" s="109"/>
+      <c r="C58" s="109"/>
+      <c r="D58" s="109"/>
+      <c r="E58" s="109"/>
     </row>
     <row r="59" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A59" s="107" t="s">
+      <c r="A59" s="110" t="s">
         <v>118</v>
       </c>
-      <c r="B59" s="110" t="s">
+      <c r="B59" s="113" t="s">
         <v>125</v>
       </c>
       <c r="C59" s="64"/>
@@ -3215,8 +3270,8 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="107"/>
-      <c r="B60" s="111"/>
+      <c r="A60" s="110"/>
+      <c r="B60" s="114"/>
       <c r="C60" s="64"/>
       <c r="D60" s="69" t="s">
         <v>137</v>
@@ -3229,8 +3284,8 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="107"/>
-      <c r="B61" s="112"/>
+      <c r="A61" s="110"/>
+      <c r="B61" s="115"/>
       <c r="C61" s="64"/>
       <c r="D61" s="69" t="s">
         <v>138</v>
@@ -3243,8 +3298,8 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="107"/>
-      <c r="B62" s="108" t="s">
+      <c r="A62" s="110"/>
+      <c r="B62" s="111" t="s">
         <v>120</v>
       </c>
       <c r="C62" s="66"/>
@@ -3259,8 +3314,8 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="107"/>
-      <c r="B63" s="108"/>
+      <c r="A63" s="110"/>
+      <c r="B63" s="111"/>
       <c r="C63" s="66"/>
       <c r="D63" s="67" t="s">
         <v>139</v>
@@ -3273,8 +3328,8 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A64" s="107"/>
-      <c r="B64" s="108"/>
+      <c r="A64" s="110"/>
+      <c r="B64" s="111"/>
       <c r="C64" s="66"/>
       <c r="D64" s="67" t="s">
         <v>128</v>
@@ -3287,8 +3342,8 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A65" s="107"/>
-      <c r="B65" s="108"/>
+      <c r="A65" s="110"/>
+      <c r="B65" s="111"/>
       <c r="C65" s="66"/>
       <c r="D65" s="67" t="s">
         <v>129</v>
@@ -3301,8 +3356,8 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="107"/>
-      <c r="B66" s="108"/>
+      <c r="A66" s="110"/>
+      <c r="B66" s="111"/>
       <c r="C66" s="66"/>
       <c r="D66" s="67" t="s">
         <v>130</v>
@@ -3315,8 +3370,8 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="107"/>
-      <c r="B67" s="108" t="s">
+      <c r="A67" s="110"/>
+      <c r="B67" s="111" t="s">
         <v>122</v>
       </c>
       <c r="C67" s="66"/>
@@ -3331,8 +3386,8 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="107"/>
-      <c r="B68" s="108"/>
+      <c r="A68" s="110"/>
+      <c r="B68" s="111"/>
       <c r="C68" s="66"/>
       <c r="D68" s="67" t="s">
         <v>133</v>
@@ -3345,8 +3400,8 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A69" s="107"/>
-      <c r="B69" s="108"/>
+      <c r="A69" s="110"/>
+      <c r="B69" s="111"/>
       <c r="C69" s="66"/>
       <c r="D69" s="67" t="s">
         <v>132</v>
@@ -3359,8 +3414,8 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="107"/>
-      <c r="B70" s="108"/>
+      <c r="A70" s="110"/>
+      <c r="B70" s="111"/>
       <c r="C70" s="66"/>
       <c r="D70" s="68" t="s">
         <v>135</v>
@@ -3373,8 +3428,8 @@
       </c>
     </row>
     <row r="71" spans="1:8" s="16" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="107"/>
-      <c r="B71" s="109" t="s">
+      <c r="A71" s="110"/>
+      <c r="B71" s="112" t="s">
         <v>123</v>
       </c>
       <c r="C71" s="64"/>
@@ -3390,8 +3445,8 @@
       <c r="H71" s="71"/>
     </row>
     <row r="72" spans="1:8" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="107"/>
-      <c r="B72" s="109"/>
+      <c r="A72" s="110"/>
+      <c r="B72" s="112"/>
       <c r="C72" s="64"/>
       <c r="D72" s="69" t="s">
         <v>141</v>
@@ -3405,8 +3460,8 @@
       <c r="H72" s="71"/>
     </row>
     <row r="73" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="107"/>
-      <c r="B73" s="108" t="s">
+      <c r="A73" s="110"/>
+      <c r="B73" s="111" t="s">
         <v>124</v>
       </c>
       <c r="C73" s="66"/>
@@ -3421,8 +3476,8 @@
       </c>
     </row>
     <row r="74" spans="1:8" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.25">
-      <c r="A74" s="107"/>
-      <c r="B74" s="108"/>
+      <c r="A74" s="110"/>
+      <c r="B74" s="111"/>
       <c r="C74" s="64"/>
       <c r="D74" s="69" t="s">
         <v>134</v>
@@ -3445,6 +3500,13 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A55:E58"/>
+    <mergeCell ref="A59:A74"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="B59:B61"/>
     <mergeCell ref="A51:B54"/>
     <mergeCell ref="B16:B21"/>
     <mergeCell ref="H10:H11"/>
@@ -3459,13 +3521,6 @@
     <mergeCell ref="B22:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B32"/>
-    <mergeCell ref="A55:E58"/>
-    <mergeCell ref="A59:A74"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="B59:B61"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E53" location="_ftn2" display="_ftn2" xr:uid="{FFC9BABA-D715-48D2-801D-3C2A2DB136EB}"/>
@@ -3554,13 +3609,13 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="120" t="s">
+      <c r="D4" s="118" t="s">
         <v>161</v>
       </c>
-      <c r="E4" s="118" t="s">
+      <c r="E4" s="116" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="118" t="s">
+      <c r="F4" s="116" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3574,9 +3629,9 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="120"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
@@ -3588,11 +3643,11 @@
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="120" t="s">
+      <c r="D6" s="118" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="116"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
@@ -3604,9 +3659,9 @@
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="120"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
     </row>
     <row r="8" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="74" t="s">
@@ -3618,11 +3673,11 @@
       <c r="C8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="118" t="s">
+      <c r="D8" s="116" t="s">
         <v>164</v>
       </c>
-      <c r="E8" s="118"/>
-      <c r="F8" s="118"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="116"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
@@ -3634,9 +3689,9 @@
       <c r="C9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="118"/>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="116"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
@@ -3648,11 +3703,11 @@
       <c r="C10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="118" t="s">
+      <c r="D10" s="116" t="s">
         <v>165</v>
       </c>
-      <c r="E10" s="118"/>
-      <c r="F10" s="118"/>
+      <c r="E10" s="116"/>
+      <c r="F10" s="116"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="74" t="s">
@@ -3664,9 +3719,9 @@
       <c r="C11" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="118"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
+      <c r="D11" s="116"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="116"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
@@ -3678,9 +3733,9 @@
       <c r="C12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="118"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="78" t="s">
@@ -3692,11 +3747,11 @@
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="118" t="s">
+      <c r="D13" s="116" t="s">
         <v>166</v>
       </c>
-      <c r="E13" s="118"/>
-      <c r="F13" s="118"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="116"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="78" t="s">
@@ -3708,9 +3763,9 @@
       <c r="C14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="118"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="118"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="116"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="78" t="s">
@@ -3722,9 +3777,9 @@
       <c r="C15" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="116"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="78" t="s">
@@ -3736,9 +3791,9 @@
       <c r="C16" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="78" t="s">
@@ -3750,9 +3805,9 @@
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="118"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="116"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
@@ -3767,8 +3822,8 @@
       <c r="D18" s="79" t="s">
         <v>167</v>
       </c>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="116"/>
     </row>
     <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
@@ -3780,13 +3835,13 @@
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="118" t="s">
+      <c r="D19" s="116" t="s">
         <v>168</v>
       </c>
-      <c r="E19" s="118" t="s">
+      <c r="E19" s="116" t="s">
         <v>197</v>
       </c>
-      <c r="F19" s="118" t="s">
+      <c r="F19" s="116" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3800,9 +3855,9 @@
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="118"/>
-      <c r="E20" s="118"/>
-      <c r="F20" s="118"/>
+      <c r="D20" s="116"/>
+      <c r="E20" s="116"/>
+      <c r="F20" s="116"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
@@ -3814,13 +3869,13 @@
       <c r="C21" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="118" t="s">
+      <c r="D21" s="116" t="s">
         <v>170</v>
       </c>
-      <c r="E21" s="118" t="s">
+      <c r="E21" s="116" t="s">
         <v>172</v>
       </c>
-      <c r="F21" s="119" t="s">
+      <c r="F21" s="117" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3834,9 +3889,9 @@
       <c r="C22" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="118"/>
-      <c r="E22" s="118"/>
-      <c r="F22" s="119"/>
+      <c r="D22" s="116"/>
+      <c r="E22" s="116"/>
+      <c r="F22" s="117"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="74" t="s">
@@ -3848,9 +3903,9 @@
       <c r="C23" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="118"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="119"/>
+      <c r="D23" s="116"/>
+      <c r="E23" s="116"/>
+      <c r="F23" s="117"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="74" t="s">
@@ -3862,9 +3917,9 @@
       <c r="C24" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="118"/>
-      <c r="E24" s="118"/>
-      <c r="F24" s="119"/>
+      <c r="D24" s="116"/>
+      <c r="E24" s="116"/>
+      <c r="F24" s="117"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="74" t="s">
@@ -3876,9 +3931,9 @@
       <c r="C25" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="118"/>
-      <c r="E25" s="118"/>
-      <c r="F25" s="119"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="117"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="74" t="s">
@@ -3890,9 +3945,9 @@
       <c r="C26" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="118"/>
-      <c r="E26" s="118"/>
-      <c r="F26" s="119"/>
+      <c r="D26" s="116"/>
+      <c r="E26" s="116"/>
+      <c r="F26" s="117"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="74" t="s">
@@ -3904,13 +3959,13 @@
       <c r="C27" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="118" t="s">
+      <c r="D27" s="116" t="s">
         <v>174</v>
       </c>
-      <c r="E27" s="118" t="s">
+      <c r="E27" s="116" t="s">
         <v>175</v>
       </c>
-      <c r="F27" s="118" t="s">
+      <c r="F27" s="116" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3924,9 +3979,9 @@
       <c r="C28" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="118"/>
-      <c r="E28" s="118"/>
-      <c r="F28" s="118"/>
+      <c r="D28" s="116"/>
+      <c r="E28" s="116"/>
+      <c r="F28" s="116"/>
     </row>
     <row r="29" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="74" t="s">
@@ -3938,9 +3993,9 @@
       <c r="C29" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D29" s="118"/>
-      <c r="E29" s="118"/>
-      <c r="F29" s="118"/>
+      <c r="D29" s="116"/>
+      <c r="E29" s="116"/>
+      <c r="F29" s="116"/>
     </row>
     <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="74" t="s">
@@ -3952,9 +4007,9 @@
       <c r="C30" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="118"/>
-      <c r="E30" s="118"/>
-      <c r="F30" s="118"/>
+      <c r="D30" s="116"/>
+      <c r="E30" s="116"/>
+      <c r="F30" s="116"/>
     </row>
     <row r="31" spans="1:6" ht="409.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="74" t="s">
@@ -3986,13 +4041,13 @@
       <c r="C32" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="118" t="s">
+      <c r="D32" s="116" t="s">
         <v>176</v>
       </c>
-      <c r="E32" s="118" t="s">
+      <c r="E32" s="116" t="s">
         <v>177</v>
       </c>
-      <c r="F32" s="119" t="s">
+      <c r="F32" s="117" t="s">
         <v>178</v>
       </c>
     </row>
@@ -4006,9 +4061,9 @@
       <c r="C33" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="119"/>
-      <c r="E33" s="118"/>
-      <c r="F33" s="119"/>
+      <c r="D33" s="117"/>
+      <c r="E33" s="116"/>
+      <c r="F33" s="117"/>
     </row>
     <row r="34" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="74" t="s">
@@ -4020,9 +4075,9 @@
       <c r="C34" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="119"/>
-      <c r="E34" s="118"/>
-      <c r="F34" s="119"/>
+      <c r="D34" s="117"/>
+      <c r="E34" s="116"/>
+      <c r="F34" s="117"/>
     </row>
     <row r="35" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="80" t="s">
@@ -4034,13 +4089,13 @@
       <c r="C35" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="118" t="s">
+      <c r="D35" s="116" t="s">
         <v>179</v>
       </c>
-      <c r="E35" s="118" t="s">
+      <c r="E35" s="116" t="s">
         <v>180</v>
       </c>
-      <c r="F35" s="118" t="s">
+      <c r="F35" s="116" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4054,9 +4109,9 @@
       <c r="C36" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="118"/>
-      <c r="E36" s="118"/>
-      <c r="F36" s="118"/>
+      <c r="D36" s="116"/>
+      <c r="E36" s="116"/>
+      <c r="F36" s="116"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="81" t="s">
@@ -4108,13 +4163,13 @@
       <c r="C39" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D39" s="118" t="s">
+      <c r="D39" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="E39" s="118" t="s">
+      <c r="E39" s="116" t="s">
         <v>188</v>
       </c>
-      <c r="F39" s="118" t="s">
+      <c r="F39" s="116" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4128,9 +4183,9 @@
       <c r="C40" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="118"/>
-      <c r="E40" s="118"/>
-      <c r="F40" s="118"/>
+      <c r="D40" s="116"/>
+      <c r="E40" s="116"/>
+      <c r="F40" s="116"/>
     </row>
     <row r="41" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A41" s="78" t="s">
@@ -4142,9 +4197,9 @@
       <c r="C41" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="118"/>
-      <c r="E41" s="118"/>
-      <c r="F41" s="118"/>
+      <c r="D41" s="116"/>
+      <c r="E41" s="116"/>
+      <c r="F41" s="116"/>
     </row>
     <row r="42" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="78" t="s">
@@ -4156,13 +4211,13 @@
       <c r="C42" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="118" t="s">
+      <c r="D42" s="116" t="s">
         <v>189</v>
       </c>
-      <c r="E42" s="118" t="s">
+      <c r="E42" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="F42" s="118" t="s">
+      <c r="F42" s="116" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4176,9 +4231,9 @@
       <c r="C43" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="118"/>
-      <c r="E43" s="118"/>
-      <c r="F43" s="118"/>
+      <c r="D43" s="116"/>
+      <c r="E43" s="116"/>
+      <c r="F43" s="116"/>
     </row>
     <row r="44" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A44" s="78" t="s">
@@ -4190,9 +4245,9 @@
       <c r="C44" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D44" s="118"/>
-      <c r="E44" s="118"/>
-      <c r="F44" s="118"/>
+      <c r="D44" s="116"/>
+      <c r="E44" s="116"/>
+      <c r="F44" s="116"/>
     </row>
     <row r="45" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A45" s="78" t="s">
@@ -4204,9 +4259,9 @@
       <c r="C45" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="118"/>
-      <c r="E45" s="118"/>
-      <c r="F45" s="118"/>
+      <c r="D45" s="116"/>
+      <c r="E45" s="116"/>
+      <c r="F45" s="116"/>
     </row>
     <row r="46" spans="1:6" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="78" t="s">
@@ -4218,9 +4273,9 @@
       <c r="C46" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D46" s="118"/>
-      <c r="E46" s="118"/>
-      <c r="F46" s="118"/>
+      <c r="D46" s="116"/>
+      <c r="E46" s="116"/>
+      <c r="F46" s="116"/>
     </row>
     <row r="47" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A47" s="78" t="s">
@@ -4232,9 +4287,9 @@
       <c r="C47" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D47" s="118"/>
-      <c r="E47" s="118"/>
-      <c r="F47" s="118"/>
+      <c r="D47" s="116"/>
+      <c r="E47" s="116"/>
+      <c r="F47" s="116"/>
     </row>
     <row r="48" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A48" s="78" t="s">
@@ -4246,9 +4301,9 @@
       <c r="C48" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D48" s="118"/>
-      <c r="E48" s="118"/>
-      <c r="F48" s="118"/>
+      <c r="D48" s="116"/>
+      <c r="E48" s="116"/>
+      <c r="F48" s="116"/>
     </row>
     <row r="49" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" s="78" t="s">
@@ -4260,9 +4315,9 @@
       <c r="C49" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D49" s="118"/>
-      <c r="E49" s="118"/>
-      <c r="F49" s="118"/>
+      <c r="D49" s="116"/>
+      <c r="E49" s="116"/>
+      <c r="F49" s="116"/>
     </row>
     <row r="50" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A50" s="78" t="s">
@@ -4274,9 +4329,9 @@
       <c r="C50" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D50" s="118"/>
-      <c r="E50" s="118"/>
-      <c r="F50" s="118"/>
+      <c r="D50" s="116"/>
+      <c r="E50" s="116"/>
+      <c r="F50" s="116"/>
     </row>
     <row r="51" spans="1:6" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="78" t="s">
@@ -4288,9 +4343,9 @@
       <c r="C51" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D51" s="118"/>
-      <c r="E51" s="118"/>
-      <c r="F51" s="118"/>
+      <c r="D51" s="116"/>
+      <c r="E51" s="116"/>
+      <c r="F51" s="116"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="78" t="s">
@@ -4302,13 +4357,13 @@
       <c r="C52" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D52" s="118" t="s">
+      <c r="D52" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="E52" s="118" t="s">
+      <c r="E52" s="116" t="s">
         <v>192</v>
       </c>
-      <c r="F52" s="118" t="s">
+      <c r="F52" s="116" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4322,9 +4377,9 @@
       <c r="C53" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D53" s="118"/>
-      <c r="E53" s="118"/>
-      <c r="F53" s="118"/>
+      <c r="D53" s="116"/>
+      <c r="E53" s="116"/>
+      <c r="F53" s="116"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="78" t="s">
@@ -4336,9 +4391,9 @@
       <c r="C54" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="118"/>
-      <c r="E54" s="118"/>
-      <c r="F54" s="118"/>
+      <c r="D54" s="116"/>
+      <c r="E54" s="116"/>
+      <c r="F54" s="116"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="78" t="s">
@@ -4350,30 +4405,12 @@
       <c r="C55" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D55" s="118"/>
-      <c r="E55" s="118"/>
-      <c r="F55" s="118"/>
+      <c r="D55" s="116"/>
+      <c r="E55" s="116"/>
+      <c r="F55" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="F52:F55"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="D42:D51"/>
-    <mergeCell ref="E42:E51"/>
-    <mergeCell ref="F42:F51"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="F32:F34"/>
     <mergeCell ref="D13:D17"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
@@ -4387,6 +4424,24 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="F52:F55"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="D42:D51"/>
+    <mergeCell ref="E42:E51"/>
+    <mergeCell ref="F42:F51"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C37" location="_ftn2" display="_ftn2" xr:uid="{25CB2AF1-E91C-4F96-A745-EB04437048A9}"/>
@@ -4478,16 +4533,16 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="120" t="s">
+      <c r="D4" s="118" t="s">
         <v>215</v>
       </c>
-      <c r="E4" s="118" t="s">
+      <c r="E4" s="116" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="118" t="s">
+      <c r="F4" s="116" t="s">
         <v>158</v>
       </c>
-      <c r="G4" s="120"/>
+      <c r="G4" s="118"/>
       <c r="H4" s="87"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4500,10 +4555,10 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="120"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="120"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="118"/>
       <c r="H5" s="87"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4516,12 +4571,12 @@
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="120" t="s">
+      <c r="D6" s="118" t="s">
         <v>216</v>
       </c>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="120"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="116"/>
+      <c r="G6" s="118"/>
       <c r="H6" s="87"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4534,10 +4589,10 @@
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="120"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="120"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="118"/>
       <c r="H7" s="87"/>
     </row>
     <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4550,12 +4605,12 @@
       <c r="C8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="120" t="s">
+      <c r="D8" s="118" t="s">
         <v>164</v>
       </c>
-      <c r="E8" s="118"/>
-      <c r="F8" s="118"/>
-      <c r="G8" s="120"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="116"/>
+      <c r="G8" s="118"/>
       <c r="H8" s="87"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4568,10 +4623,10 @@
       <c r="C9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="120"/>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
-      <c r="G9" s="120"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="116"/>
+      <c r="G9" s="118"/>
       <c r="H9" s="87"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4584,12 +4639,12 @@
       <c r="C10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="120" t="s">
+      <c r="D10" s="118" t="s">
         <v>217</v>
       </c>
-      <c r="E10" s="118"/>
-      <c r="F10" s="118"/>
-      <c r="G10" s="120"/>
+      <c r="E10" s="116"/>
+      <c r="F10" s="116"/>
+      <c r="G10" s="118"/>
       <c r="H10" s="87"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4602,10 +4657,10 @@
       <c r="C11" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="120"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="120"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="116"/>
+      <c r="G11" s="118"/>
       <c r="H11" s="87"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4618,10 +4673,10 @@
       <c r="C12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="120"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="120"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="118"/>
       <c r="H12" s="87"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4634,12 +4689,12 @@
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="120" t="s">
+      <c r="D13" s="118" t="s">
         <v>218</v>
       </c>
-      <c r="E13" s="118"/>
-      <c r="F13" s="118"/>
-      <c r="G13" s="120"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="116"/>
+      <c r="G13" s="118"/>
       <c r="H13" s="87"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4652,10 +4707,10 @@
       <c r="C14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="120"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="118"/>
-      <c r="G14" s="120"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="116"/>
+      <c r="G14" s="118"/>
       <c r="H14" s="87"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4668,10 +4723,10 @@
       <c r="C15" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="120"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="120"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="116"/>
+      <c r="G15" s="118"/>
       <c r="H15" s="87"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4684,10 +4739,10 @@
       <c r="C16" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="120"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
-      <c r="G16" s="120"/>
+      <c r="D16" s="118"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="118"/>
       <c r="H16" s="87"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -4700,10 +4755,10 @@
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="120"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
-      <c r="G17" s="120"/>
+      <c r="D17" s="118"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="116"/>
+      <c r="G17" s="118"/>
       <c r="H17" s="87"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -4719,9 +4774,9 @@
       <c r="D18" s="83" t="s">
         <v>219</v>
       </c>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
-      <c r="G18" s="120"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="116"/>
+      <c r="G18" s="118"/>
       <c r="H18" s="87"/>
     </row>
     <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -4734,19 +4789,19 @@
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="120" t="s">
+      <c r="D19" s="118" t="s">
         <v>220</v>
       </c>
-      <c r="E19" s="118" t="s">
+      <c r="E19" s="116" t="s">
         <v>197</v>
       </c>
-      <c r="F19" s="118" t="s">
+      <c r="F19" s="116" t="s">
         <v>169</v>
       </c>
-      <c r="G19" s="120" t="s">
+      <c r="G19" s="118" t="s">
         <v>235</v>
       </c>
-      <c r="H19" s="122" t="s">
+      <c r="H19" s="119" t="s">
         <v>234</v>
       </c>
     </row>
@@ -4760,11 +4815,11 @@
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="120"/>
-      <c r="E20" s="118"/>
-      <c r="F20" s="118"/>
-      <c r="G20" s="120"/>
-      <c r="H20" s="122"/>
+      <c r="D20" s="118"/>
+      <c r="E20" s="116"/>
+      <c r="F20" s="116"/>
+      <c r="G20" s="118"/>
+      <c r="H20" s="119"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
@@ -4776,16 +4831,16 @@
       <c r="C21" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="120" t="s">
+      <c r="D21" s="118" t="s">
         <v>221</v>
       </c>
-      <c r="E21" s="118" t="s">
+      <c r="E21" s="116" t="s">
         <v>172</v>
       </c>
-      <c r="F21" s="119" t="s">
+      <c r="F21" s="117" t="s">
         <v>173</v>
       </c>
-      <c r="G21" s="123"/>
+      <c r="G21" s="121"/>
       <c r="H21" s="87"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -4798,10 +4853,10 @@
       <c r="C22" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="120"/>
-      <c r="E22" s="118"/>
-      <c r="F22" s="119"/>
-      <c r="G22" s="123"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="116"/>
+      <c r="F22" s="117"/>
+      <c r="G22" s="121"/>
       <c r="H22" s="87"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -4814,10 +4869,10 @@
       <c r="C23" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="120"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="119"/>
-      <c r="G23" s="123"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="116"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="121"/>
       <c r="H23" s="87"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -4830,10 +4885,10 @@
       <c r="C24" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="120"/>
-      <c r="E24" s="118"/>
-      <c r="F24" s="119"/>
-      <c r="G24" s="123"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="116"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="121"/>
       <c r="H24" s="87"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -4846,10 +4901,10 @@
       <c r="C25" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="120"/>
-      <c r="E25" s="118"/>
-      <c r="F25" s="119"/>
-      <c r="G25" s="123"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="117"/>
+      <c r="G25" s="121"/>
       <c r="H25" s="87"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -4862,10 +4917,10 @@
       <c r="C26" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="120"/>
-      <c r="E26" s="118"/>
-      <c r="F26" s="119"/>
-      <c r="G26" s="123"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="116"/>
+      <c r="F26" s="117"/>
+      <c r="G26" s="121"/>
       <c r="H26" s="87"/>
     </row>
     <row r="27" spans="1:8" ht="374.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4904,19 +4959,19 @@
       <c r="C28" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="120" t="s">
+      <c r="D28" s="118" t="s">
         <v>224</v>
       </c>
-      <c r="E28" s="118" t="s">
+      <c r="E28" s="116" t="s">
         <v>229</v>
       </c>
-      <c r="F28" s="119" t="s">
+      <c r="F28" s="117" t="s">
         <v>178</v>
       </c>
-      <c r="G28" s="123" t="s">
+      <c r="G28" s="121" t="s">
         <v>243</v>
       </c>
-      <c r="H28" s="121" t="s">
+      <c r="H28" s="120" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4930,11 +4985,11 @@
       <c r="C29" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="123"/>
-      <c r="E29" s="118"/>
-      <c r="F29" s="119"/>
-      <c r="G29" s="123"/>
-      <c r="H29" s="121"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="116"/>
+      <c r="F29" s="117"/>
+      <c r="G29" s="121"/>
+      <c r="H29" s="120"/>
     </row>
     <row r="30" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="74" t="s">
@@ -4946,11 +5001,11 @@
       <c r="C30" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="123"/>
-      <c r="E30" s="118"/>
-      <c r="F30" s="119"/>
-      <c r="G30" s="123"/>
-      <c r="H30" s="121"/>
+      <c r="D30" s="121"/>
+      <c r="E30" s="116"/>
+      <c r="F30" s="117"/>
+      <c r="G30" s="121"/>
+      <c r="H30" s="120"/>
     </row>
     <row r="31" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="80" t="s">
@@ -4962,17 +5017,17 @@
       <c r="C31" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="120" t="s">
+      <c r="D31" s="118" t="s">
         <v>179</v>
       </c>
-      <c r="E31" s="118" t="s">
+      <c r="E31" s="116" t="s">
         <v>180</v>
       </c>
-      <c r="F31" s="118" t="s">
+      <c r="F31" s="116" t="s">
         <v>181</v>
       </c>
-      <c r="G31" s="120"/>
-      <c r="H31" s="121"/>
+      <c r="G31" s="118"/>
+      <c r="H31" s="120"/>
     </row>
     <row r="32" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="80" t="s">
@@ -4984,11 +5039,11 @@
       <c r="C32" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="120"/>
-      <c r="E32" s="118"/>
-      <c r="F32" s="118"/>
-      <c r="G32" s="120"/>
-      <c r="H32" s="121"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="116"/>
+      <c r="F32" s="116"/>
+      <c r="G32" s="118"/>
+      <c r="H32" s="120"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="81" t="s">
@@ -5048,19 +5103,19 @@
       <c r="C35" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="120" t="s">
+      <c r="D35" s="118" t="s">
         <v>231</v>
       </c>
-      <c r="E35" s="118" t="s">
+      <c r="E35" s="116" t="s">
         <v>188</v>
       </c>
-      <c r="F35" s="118" t="s">
+      <c r="F35" s="116" t="s">
         <v>144</v>
       </c>
-      <c r="G35" s="120" t="s">
+      <c r="G35" s="118" t="s">
         <v>237</v>
       </c>
-      <c r="H35" s="122" t="s">
+      <c r="H35" s="119" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5074,11 +5129,11 @@
       <c r="C36" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D36" s="120"/>
-      <c r="E36" s="118"/>
-      <c r="F36" s="118"/>
-      <c r="G36" s="120"/>
-      <c r="H36" s="122"/>
+      <c r="D36" s="118"/>
+      <c r="E36" s="116"/>
+      <c r="F36" s="116"/>
+      <c r="G36" s="118"/>
+      <c r="H36" s="119"/>
     </row>
     <row r="37" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A37" s="78" t="s">
@@ -5090,11 +5145,11 @@
       <c r="C37" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D37" s="120"/>
-      <c r="E37" s="118"/>
-      <c r="F37" s="118"/>
-      <c r="G37" s="120"/>
-      <c r="H37" s="122"/>
+      <c r="D37" s="118"/>
+      <c r="E37" s="116"/>
+      <c r="F37" s="116"/>
+      <c r="G37" s="118"/>
+      <c r="H37" s="119"/>
     </row>
     <row r="38" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="78" t="s">
@@ -5106,19 +5161,19 @@
       <c r="C38" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D38" s="120" t="s">
+      <c r="D38" s="118" t="s">
         <v>226</v>
       </c>
-      <c r="E38" s="118" t="s">
+      <c r="E38" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="F38" s="118" t="s">
+      <c r="F38" s="116" t="s">
         <v>244</v>
       </c>
-      <c r="G38" s="120" t="s">
+      <c r="G38" s="118" t="s">
         <v>237</v>
       </c>
-      <c r="H38" s="121" t="s">
+      <c r="H38" s="120" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5132,11 +5187,11 @@
       <c r="C39" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="120"/>
-      <c r="E39" s="118"/>
-      <c r="F39" s="118"/>
-      <c r="G39" s="120"/>
-      <c r="H39" s="121"/>
+      <c r="D39" s="118"/>
+      <c r="E39" s="116"/>
+      <c r="F39" s="116"/>
+      <c r="G39" s="118"/>
+      <c r="H39" s="120"/>
     </row>
     <row r="40" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A40" s="78" t="s">
@@ -5148,11 +5203,11 @@
       <c r="C40" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D40" s="120"/>
-      <c r="E40" s="118"/>
-      <c r="F40" s="118"/>
-      <c r="G40" s="120"/>
-      <c r="H40" s="121"/>
+      <c r="D40" s="118"/>
+      <c r="E40" s="116"/>
+      <c r="F40" s="116"/>
+      <c r="G40" s="118"/>
+      <c r="H40" s="120"/>
     </row>
     <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A41" s="78" t="s">
@@ -5164,11 +5219,11 @@
       <c r="C41" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="120"/>
-      <c r="E41" s="118"/>
-      <c r="F41" s="118"/>
-      <c r="G41" s="120"/>
-      <c r="H41" s="121"/>
+      <c r="D41" s="118"/>
+      <c r="E41" s="116"/>
+      <c r="F41" s="116"/>
+      <c r="G41" s="118"/>
+      <c r="H41" s="120"/>
     </row>
     <row r="42" spans="1:8" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="78" t="s">
@@ -5180,11 +5235,11 @@
       <c r="C42" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="120"/>
-      <c r="E42" s="118"/>
-      <c r="F42" s="118"/>
-      <c r="G42" s="120"/>
-      <c r="H42" s="121"/>
+      <c r="D42" s="118"/>
+      <c r="E42" s="116"/>
+      <c r="F42" s="116"/>
+      <c r="G42" s="118"/>
+      <c r="H42" s="120"/>
     </row>
     <row r="43" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A43" s="78" t="s">
@@ -5196,11 +5251,11 @@
       <c r="C43" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="120"/>
-      <c r="E43" s="118"/>
-      <c r="F43" s="118"/>
-      <c r="G43" s="120"/>
-      <c r="H43" s="121"/>
+      <c r="D43" s="118"/>
+      <c r="E43" s="116"/>
+      <c r="F43" s="116"/>
+      <c r="G43" s="118"/>
+      <c r="H43" s="120"/>
     </row>
     <row r="44" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A44" s="78" t="s">
@@ -5212,11 +5267,11 @@
       <c r="C44" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D44" s="120"/>
-      <c r="E44" s="118"/>
-      <c r="F44" s="118"/>
-      <c r="G44" s="120"/>
-      <c r="H44" s="121"/>
+      <c r="D44" s="118"/>
+      <c r="E44" s="116"/>
+      <c r="F44" s="116"/>
+      <c r="G44" s="118"/>
+      <c r="H44" s="120"/>
     </row>
     <row r="45" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A45" s="78" t="s">
@@ -5228,11 +5283,11 @@
       <c r="C45" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="120"/>
-      <c r="E45" s="118"/>
-      <c r="F45" s="118"/>
-      <c r="G45" s="120"/>
-      <c r="H45" s="121"/>
+      <c r="D45" s="118"/>
+      <c r="E45" s="116"/>
+      <c r="F45" s="116"/>
+      <c r="G45" s="118"/>
+      <c r="H45" s="120"/>
     </row>
     <row r="46" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A46" s="78" t="s">
@@ -5244,11 +5299,11 @@
       <c r="C46" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D46" s="120"/>
-      <c r="E46" s="118"/>
-      <c r="F46" s="118"/>
-      <c r="G46" s="120"/>
-      <c r="H46" s="121"/>
+      <c r="D46" s="118"/>
+      <c r="E46" s="116"/>
+      <c r="F46" s="116"/>
+      <c r="G46" s="118"/>
+      <c r="H46" s="120"/>
     </row>
     <row r="47" spans="1:8" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="78" t="s">
@@ -5260,11 +5315,11 @@
       <c r="C47" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D47" s="120"/>
-      <c r="E47" s="118"/>
-      <c r="F47" s="118"/>
-      <c r="G47" s="120"/>
-      <c r="H47" s="121"/>
+      <c r="D47" s="118"/>
+      <c r="E47" s="116"/>
+      <c r="F47" s="116"/>
+      <c r="G47" s="118"/>
+      <c r="H47" s="120"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="78" t="s">
@@ -5276,19 +5331,19 @@
       <c r="C48" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D48" s="120" t="s">
+      <c r="D48" s="118" t="s">
         <v>227</v>
       </c>
-      <c r="E48" s="118" t="s">
+      <c r="E48" s="116" t="s">
         <v>192</v>
       </c>
-      <c r="F48" s="118" t="s">
+      <c r="F48" s="116" t="s">
         <v>144</v>
       </c>
-      <c r="G48" s="120" t="s">
+      <c r="G48" s="118" t="s">
         <v>237</v>
       </c>
-      <c r="H48" s="121" t="s">
+      <c r="H48" s="120" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5302,11 +5357,11 @@
       <c r="C49" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D49" s="120"/>
-      <c r="E49" s="118"/>
-      <c r="F49" s="118"/>
-      <c r="G49" s="120"/>
-      <c r="H49" s="121"/>
+      <c r="D49" s="118"/>
+      <c r="E49" s="116"/>
+      <c r="F49" s="116"/>
+      <c r="G49" s="118"/>
+      <c r="H49" s="120"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="78" t="s">
@@ -5318,11 +5373,11 @@
       <c r="C50" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D50" s="120"/>
-      <c r="E50" s="118"/>
-      <c r="F50" s="118"/>
-      <c r="G50" s="120"/>
-      <c r="H50" s="121"/>
+      <c r="D50" s="118"/>
+      <c r="E50" s="116"/>
+      <c r="F50" s="116"/>
+      <c r="G50" s="118"/>
+      <c r="H50" s="120"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="78" t="s">
@@ -5334,25 +5389,29 @@
       <c r="C51" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D51" s="120"/>
-      <c r="E51" s="118"/>
-      <c r="F51" s="118"/>
-      <c r="G51" s="120"/>
-      <c r="H51" s="121"/>
+      <c r="D51" s="118"/>
+      <c r="E51" s="116"/>
+      <c r="F51" s="116"/>
+      <c r="G51" s="118"/>
+      <c r="H51" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E18"/>
-    <mergeCell ref="F4:F18"/>
-    <mergeCell ref="G4:G18"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="F48:F51"/>
+    <mergeCell ref="G48:G51"/>
+    <mergeCell ref="H48:H51"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="D38:D47"/>
+    <mergeCell ref="E38:E47"/>
+    <mergeCell ref="F38:F47"/>
+    <mergeCell ref="G38:G47"/>
+    <mergeCell ref="H38:H47"/>
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="H28:H30"/>
     <mergeCell ref="D31:D32"/>
@@ -5369,21 +5428,17 @@
     <mergeCell ref="F21:F26"/>
     <mergeCell ref="G21:G26"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D38:D47"/>
-    <mergeCell ref="E38:E47"/>
-    <mergeCell ref="F38:F47"/>
-    <mergeCell ref="G38:G47"/>
-    <mergeCell ref="H38:H47"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="F48:F51"/>
-    <mergeCell ref="G48:G51"/>
-    <mergeCell ref="H48:H51"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E18"/>
+    <mergeCell ref="F4:F18"/>
+    <mergeCell ref="G4:G18"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C33" location="_ftn2" display="_ftn2" xr:uid="{E50DF5A1-13E6-4004-9692-0F820274B734}"/>
@@ -5395,10 +5450,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE037D9D-4E45-4C5B-8392-AE943DD18A55}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5409,7 +5464,7 @@
     <col min="4" max="16384" width="29.7109375" style="88"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
@@ -5420,161 +5475,175 @@
         <v>3</v>
       </c>
       <c r="D1" s="63" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="122" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="94" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="95" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="96" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="124" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="97" t="s">
+      <c r="E2" s="133" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="123"/>
+      <c r="B3" s="94" t="s">
+        <v>249</v>
+      </c>
+      <c r="C3" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="96" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="124"/>
+      <c r="B4" s="94" t="s">
+        <v>289</v>
+      </c>
+      <c r="C4" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="96" t="s">
+        <v>283</v>
+      </c>
+      <c r="E4" s="101"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="140" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="137" t="s">
+        <v>250</v>
+      </c>
+      <c r="C5" s="138" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="139" t="s">
+        <v>283</v>
+      </c>
+      <c r="E5" s="133" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="141"/>
+      <c r="B6" s="137" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" s="138" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="139" t="s">
+        <v>283</v>
+      </c>
+      <c r="E6" s="133" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="125" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="94" t="s">
+        <v>252</v>
+      </c>
+      <c r="C7" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="96" t="s">
+        <v>283</v>
+      </c>
+      <c r="E7" s="132"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="126"/>
+      <c r="B8" s="94" t="s">
+        <v>253</v>
+      </c>
+      <c r="C8" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="96" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="126"/>
+      <c r="B9" s="94" t="s">
+        <v>254</v>
+      </c>
+      <c r="C9" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="96" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="126"/>
+      <c r="B10" s="134" t="s">
+        <v>290</v>
+      </c>
+      <c r="C10" s="135" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="136" t="s">
+        <v>283</v>
+      </c>
+      <c r="E10" s="101"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="126"/>
+      <c r="B11" s="134" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="135" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="136" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A12" s="126"/>
+      <c r="B12" s="134" t="s">
+        <v>285</v>
+      </c>
+      <c r="C12" s="135" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="136" t="s">
+        <v>283</v>
+      </c>
+      <c r="E12" s="101"/>
+    </row>
+    <row r="13" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="126"/>
+      <c r="B13" s="90" t="s">
         <v>274</v>
-      </c>
-      <c r="C2" s="98" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="99" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="125"/>
-      <c r="B3" s="97" t="s">
-        <v>249</v>
-      </c>
-      <c r="C3" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="99" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="126"/>
-      <c r="B4" s="97" t="s">
-        <v>250</v>
-      </c>
-      <c r="C4" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="99" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="124" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="97" t="s">
-        <v>251</v>
-      </c>
-      <c r="C5" s="98" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="99" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="126"/>
-      <c r="B6" s="97" t="s">
-        <v>252</v>
-      </c>
-      <c r="C6" s="98" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="99" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="124" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="94" t="s">
-        <v>253</v>
-      </c>
-      <c r="C7" s="95" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="96" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="125"/>
-      <c r="B8" s="100" t="s">
-        <v>254</v>
-      </c>
-      <c r="C8" s="101" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="102" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="125"/>
-      <c r="B9" s="100" t="s">
-        <v>255</v>
-      </c>
-      <c r="C9" s="101" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="102" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="125"/>
-      <c r="B10" s="100" t="s">
-        <v>206</v>
-      </c>
-      <c r="C10" s="101" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="102" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="125"/>
-      <c r="B11" s="100" t="s">
-        <v>256</v>
-      </c>
-      <c r="C11" s="101" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="102" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A12" s="125"/>
-      <c r="B12" s="90" t="s">
-        <v>286</v>
-      </c>
-      <c r="C12" s="89" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" s="93" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="125"/>
-      <c r="B13" s="90" t="s">
-        <v>275</v>
       </c>
       <c r="C13" s="89" t="s">
         <v>119</v>
       </c>
       <c r="D13" s="93" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="125"/>
+        <v>283</v>
+      </c>
+      <c r="E13" s="101"/>
+    </row>
+    <row r="14" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="126"/>
       <c r="B14" s="90" t="s">
         <v>138</v>
       </c>
@@ -5582,11 +5651,11 @@
         <v>119</v>
       </c>
       <c r="D14" s="93" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="125"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="126"/>
       <c r="B15" s="91" t="s">
         <v>127</v>
       </c>
@@ -5594,11 +5663,11 @@
         <v>246</v>
       </c>
       <c r="D15" s="93" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="125"/>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="126"/>
       <c r="B16" s="90" t="s">
         <v>139</v>
       </c>
@@ -5606,394 +5675,403 @@
         <v>246</v>
       </c>
       <c r="D16" s="93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="125"/>
+      <c r="A17" s="126"/>
       <c r="B17" s="90" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C17" s="89" t="s">
         <v>246</v>
       </c>
       <c r="D17" s="93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="125"/>
+      <c r="A18" s="126"/>
       <c r="B18" s="90" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C18" s="89" t="s">
         <v>246</v>
       </c>
       <c r="D18" s="93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A19" s="125"/>
+      <c r="A19" s="126"/>
       <c r="B19" s="90" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C19" s="89" t="s">
         <v>246</v>
       </c>
       <c r="D19" s="93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A20" s="125"/>
+      <c r="A20" s="126"/>
       <c r="B20" s="90" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C20" s="89" t="s">
         <v>246</v>
       </c>
       <c r="D20" s="93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A21" s="125"/>
+      <c r="A21" s="126"/>
       <c r="B21" s="90" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C21" s="89" t="s">
         <v>246</v>
       </c>
       <c r="D21" s="93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="125"/>
+      <c r="A22" s="126"/>
       <c r="B22" s="90" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C22" s="89" t="s">
         <v>246</v>
       </c>
       <c r="D22" s="93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="125"/>
+      <c r="A23" s="126"/>
       <c r="B23" s="90" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C23" s="89" t="s">
         <v>246</v>
       </c>
       <c r="D23" s="93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="125"/>
+      <c r="A24" s="126"/>
       <c r="B24" s="90" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C24" s="89" t="s">
         <v>246</v>
       </c>
       <c r="D24" s="93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="125"/>
+      <c r="A25" s="126"/>
       <c r="B25" s="90" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C25" s="89" t="s">
         <v>144</v>
       </c>
       <c r="D25" s="93" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="125"/>
+      <c r="A26" s="126"/>
       <c r="B26" s="90" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C26" s="89" t="s">
         <v>144</v>
       </c>
       <c r="D26" s="93" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="125"/>
+      <c r="A27" s="126"/>
       <c r="B27" s="90" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C27" s="89" t="s">
         <v>144</v>
       </c>
       <c r="D27" s="93" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="126"/>
+      <c r="A28" s="127"/>
       <c r="B28" s="90" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C28" s="89" t="s">
         <v>144</v>
       </c>
       <c r="D28" s="93" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="124" t="s">
+      <c r="A29" s="125" t="s">
         <v>67</v>
       </c>
       <c r="B29" s="90" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C29" s="89" t="s">
         <v>116</v>
       </c>
       <c r="D29" s="93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="125"/>
+      <c r="A30" s="126"/>
       <c r="B30" s="90" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C30" s="89" t="s">
         <v>116</v>
       </c>
       <c r="D30" s="93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="125"/>
+      <c r="A31" s="126"/>
       <c r="B31" s="90" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C31" s="89" t="s">
         <v>116</v>
       </c>
       <c r="D31" s="93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="125"/>
+      <c r="A32" s="126"/>
       <c r="B32" s="90" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C32" s="89" t="s">
         <v>116</v>
       </c>
       <c r="D32" s="93" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="125"/>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="126"/>
       <c r="B33" s="90" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C33" s="89" t="s">
         <v>116</v>
       </c>
       <c r="D33" s="93" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="126"/>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="127"/>
       <c r="B34" s="90" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C34" s="89" t="s">
         <v>116</v>
       </c>
       <c r="D34" s="93" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="127" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="122" t="s">
+        <v>287</v>
+      </c>
+      <c r="B35" s="98" t="s">
+        <v>265</v>
+      </c>
+      <c r="C35" s="99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="100" t="s">
+        <v>283</v>
+      </c>
+      <c r="F35" s="97" t="s">
         <v>288</v>
       </c>
-      <c r="B35" s="97" t="s">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="124"/>
+      <c r="B36" s="98" t="s">
         <v>266</v>
       </c>
-      <c r="C35" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="99" t="s">
-        <v>284</v>
-      </c>
-      <c r="E35" s="103" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="128"/>
-      <c r="B36" s="97" t="s">
+      <c r="C36" s="99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="100" t="s">
+        <v>283</v>
+      </c>
+      <c r="F36" s="97" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="122" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="98" t="s">
         <v>267</v>
       </c>
-      <c r="C36" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="99" t="s">
-        <v>284</v>
-      </c>
-      <c r="E36" s="103" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="127" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="97" t="s">
+      <c r="C37" s="99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="100" t="s">
+        <v>283</v>
+      </c>
+      <c r="F37" s="97" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="124"/>
+      <c r="B38" s="98" t="s">
         <v>268</v>
       </c>
-      <c r="C37" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="99" t="s">
-        <v>284</v>
-      </c>
-      <c r="E37" s="103" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="128"/>
-      <c r="B38" s="97" t="s">
+      <c r="C38" s="99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="100" t="s">
+        <v>283</v>
+      </c>
+      <c r="F38" s="97"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="122" t="s">
+        <v>199</v>
+      </c>
+      <c r="B39" s="98" t="s">
         <v>269</v>
       </c>
-      <c r="C38" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="99" t="s">
-        <v>284</v>
-      </c>
-      <c r="E38" s="103"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="124" t="s">
-        <v>199</v>
-      </c>
-      <c r="B39" s="100" t="s">
+      <c r="C39" s="99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="100" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="123"/>
+      <c r="B40" s="98" t="s">
         <v>270</v>
       </c>
-      <c r="C39" s="101" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="102" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="125"/>
-      <c r="B40" s="100" t="s">
+      <c r="C40" s="99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="100" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="123"/>
+      <c r="B41" s="98" t="s">
         <v>271</v>
       </c>
-      <c r="C40" s="101" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="102" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="125"/>
-      <c r="B41" s="100" t="s">
-        <v>272</v>
-      </c>
-      <c r="C41" s="101" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="102" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="126"/>
-      <c r="B42" s="97" t="s">
+      <c r="C41" s="99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="100" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="124"/>
+      <c r="B42" s="98" t="s">
         <v>245</v>
       </c>
-      <c r="C42" s="98" t="s">
+      <c r="C42" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="D42" s="99" t="s">
-        <v>284</v>
-      </c>
-      <c r="E42" s="92" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="124" t="s">
+      <c r="D42" s="100" t="s">
+        <v>283</v>
+      </c>
+      <c r="F42" s="92" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="125" t="s">
         <v>198</v>
       </c>
-      <c r="B43" s="100" t="s">
+      <c r="B43" s="134" t="s">
         <v>248</v>
       </c>
-      <c r="C43" s="101" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="102" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="125"/>
-      <c r="B44" s="90" t="s">
+      <c r="C43" s="135" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="136" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="126"/>
+      <c r="B44" s="137" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="89" t="s">
+      <c r="C44" s="138" t="s">
         <v>88</v>
       </c>
-      <c r="D44" s="93" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="125"/>
-      <c r="B45" s="90" t="s">
+      <c r="D44" s="139" t="s">
+        <v>283</v>
+      </c>
+      <c r="E44" s="133" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="126"/>
+      <c r="B45" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="89" t="s">
+      <c r="C45" s="138" t="s">
         <v>88</v>
       </c>
-      <c r="D45" s="93" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="126"/>
-      <c r="B46" s="90" t="s">
+      <c r="D45" s="139" t="s">
+        <v>283</v>
+      </c>
+      <c r="E45" s="133" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="127"/>
+      <c r="B46" s="137" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="89" t="s">
+      <c r="C46" s="138" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="93" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="124" t="s">
+      <c r="D46" s="139" t="s">
+        <v>283</v>
+      </c>
+      <c r="E46" s="133" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="125" t="s">
         <v>151</v>
       </c>
       <c r="B47" s="90" t="s">
@@ -6003,11 +6081,11 @@
         <v>62</v>
       </c>
       <c r="D47" s="93" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="126"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="127"/>
       <c r="B48" s="90" t="s">
         <v>247</v>
       </c>
@@ -6015,7 +6093,7 @@
         <v>62</v>
       </c>
       <c r="D48" s="93" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -6031,6 +6109,7 @@
     <mergeCell ref="A37:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6116,16 +6195,16 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="120" t="s">
+      <c r="D4" s="118" t="s">
         <v>215</v>
       </c>
-      <c r="E4" s="118" t="s">
+      <c r="E4" s="116" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="118" t="s">
+      <c r="F4" s="116" t="s">
         <v>158</v>
       </c>
-      <c r="G4" s="120"/>
+      <c r="G4" s="118"/>
       <c r="H4" s="87"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6138,10 +6217,10 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="120"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="120"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="118"/>
       <c r="H5" s="87"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6154,12 +6233,12 @@
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="120" t="s">
+      <c r="D6" s="118" t="s">
         <v>216</v>
       </c>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="120"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="116"/>
+      <c r="G6" s="118"/>
       <c r="H6" s="87"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6172,10 +6251,10 @@
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="120"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="120"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="118"/>
       <c r="H7" s="87"/>
     </row>
     <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6188,12 +6267,12 @@
       <c r="C8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="120" t="s">
+      <c r="D8" s="118" t="s">
         <v>164</v>
       </c>
-      <c r="E8" s="118"/>
-      <c r="F8" s="118"/>
-      <c r="G8" s="120"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="116"/>
+      <c r="G8" s="118"/>
       <c r="H8" s="87"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6206,10 +6285,10 @@
       <c r="C9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="120"/>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
-      <c r="G9" s="120"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="116"/>
+      <c r="G9" s="118"/>
       <c r="H9" s="87"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -6222,12 +6301,12 @@
       <c r="C10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="120" t="s">
+      <c r="D10" s="118" t="s">
         <v>217</v>
       </c>
-      <c r="E10" s="118"/>
-      <c r="F10" s="118"/>
-      <c r="G10" s="120"/>
+      <c r="E10" s="116"/>
+      <c r="F10" s="116"/>
+      <c r="G10" s="118"/>
       <c r="H10" s="87"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -6240,10 +6319,10 @@
       <c r="C11" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="120"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="120"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="116"/>
+      <c r="G11" s="118"/>
       <c r="H11" s="87"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6256,10 +6335,10 @@
       <c r="C12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="120"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="120"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="118"/>
       <c r="H12" s="87"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6272,12 +6351,12 @@
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="120" t="s">
+      <c r="D13" s="118" t="s">
         <v>218</v>
       </c>
-      <c r="E13" s="118"/>
-      <c r="F13" s="118"/>
-      <c r="G13" s="120"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="116"/>
+      <c r="G13" s="118"/>
       <c r="H13" s="87"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -6290,10 +6369,10 @@
       <c r="C14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="120"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="118"/>
-      <c r="G14" s="120"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="116"/>
+      <c r="G14" s="118"/>
       <c r="H14" s="87"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6306,10 +6385,10 @@
       <c r="C15" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="120"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="120"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="116"/>
+      <c r="G15" s="118"/>
       <c r="H15" s="87"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -6322,10 +6401,10 @@
       <c r="C16" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="120"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
-      <c r="G16" s="120"/>
+      <c r="D16" s="118"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="118"/>
       <c r="H16" s="87"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -6338,10 +6417,10 @@
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="120"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
-      <c r="G17" s="120"/>
+      <c r="D17" s="118"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="116"/>
+      <c r="G17" s="118"/>
       <c r="H17" s="87"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -6357,9 +6436,9 @@
       <c r="D18" s="83" t="s">
         <v>219</v>
       </c>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
-      <c r="G18" s="120"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="116"/>
+      <c r="G18" s="118"/>
       <c r="H18" s="87"/>
     </row>
     <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -6372,19 +6451,19 @@
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="120" t="s">
+      <c r="D19" s="118" t="s">
         <v>220</v>
       </c>
-      <c r="E19" s="118" t="s">
+      <c r="E19" s="116" t="s">
         <v>197</v>
       </c>
-      <c r="F19" s="118" t="s">
+      <c r="F19" s="116" t="s">
         <v>169</v>
       </c>
-      <c r="G19" s="120" t="s">
+      <c r="G19" s="118" t="s">
         <v>235</v>
       </c>
-      <c r="H19" s="122" t="s">
+      <c r="H19" s="119" t="s">
         <v>234</v>
       </c>
     </row>
@@ -6398,11 +6477,11 @@
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="120"/>
-      <c r="E20" s="118"/>
-      <c r="F20" s="118"/>
-      <c r="G20" s="120"/>
-      <c r="H20" s="122"/>
+      <c r="D20" s="118"/>
+      <c r="E20" s="116"/>
+      <c r="F20" s="116"/>
+      <c r="G20" s="118"/>
+      <c r="H20" s="119"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
@@ -6414,16 +6493,16 @@
       <c r="C21" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="120" t="s">
+      <c r="D21" s="118" t="s">
         <v>221</v>
       </c>
-      <c r="E21" s="118" t="s">
+      <c r="E21" s="116" t="s">
         <v>172</v>
       </c>
-      <c r="F21" s="119" t="s">
+      <c r="F21" s="117" t="s">
         <v>173</v>
       </c>
-      <c r="G21" s="123"/>
+      <c r="G21" s="121"/>
       <c r="H21" s="87"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -6436,10 +6515,10 @@
       <c r="C22" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="120"/>
-      <c r="E22" s="118"/>
-      <c r="F22" s="119"/>
-      <c r="G22" s="123"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="116"/>
+      <c r="F22" s="117"/>
+      <c r="G22" s="121"/>
       <c r="H22" s="87"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -6452,10 +6531,10 @@
       <c r="C23" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="120"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="119"/>
-      <c r="G23" s="123"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="116"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="121"/>
       <c r="H23" s="87"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -6468,10 +6547,10 @@
       <c r="C24" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="120"/>
-      <c r="E24" s="118"/>
-      <c r="F24" s="119"/>
-      <c r="G24" s="123"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="116"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="121"/>
       <c r="H24" s="87"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -6484,10 +6563,10 @@
       <c r="C25" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="120"/>
-      <c r="E25" s="118"/>
-      <c r="F25" s="119"/>
-      <c r="G25" s="123"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="117"/>
+      <c r="G25" s="121"/>
       <c r="H25" s="87"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -6500,10 +6579,10 @@
       <c r="C26" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="120"/>
-      <c r="E26" s="118"/>
-      <c r="F26" s="119"/>
-      <c r="G26" s="123"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="116"/>
+      <c r="F26" s="117"/>
+      <c r="G26" s="121"/>
       <c r="H26" s="87"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -6516,16 +6595,16 @@
       <c r="C27" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="120" t="s">
+      <c r="D27" s="118" t="s">
         <v>222</v>
       </c>
-      <c r="E27" s="118" t="s">
+      <c r="E27" s="116" t="s">
         <v>175</v>
       </c>
-      <c r="F27" s="118" t="s">
+      <c r="F27" s="116" t="s">
         <v>158</v>
       </c>
-      <c r="G27" s="120"/>
+      <c r="G27" s="118"/>
       <c r="H27" s="87"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -6538,10 +6617,10 @@
       <c r="C28" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="120"/>
-      <c r="E28" s="118"/>
-      <c r="F28" s="118"/>
-      <c r="G28" s="120"/>
+      <c r="D28" s="118"/>
+      <c r="E28" s="116"/>
+      <c r="F28" s="116"/>
+      <c r="G28" s="118"/>
       <c r="H28" s="87"/>
     </row>
     <row r="29" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -6554,10 +6633,10 @@
       <c r="C29" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D29" s="120"/>
-      <c r="E29" s="118"/>
-      <c r="F29" s="118"/>
-      <c r="G29" s="120"/>
+      <c r="D29" s="118"/>
+      <c r="E29" s="116"/>
+      <c r="F29" s="116"/>
+      <c r="G29" s="118"/>
       <c r="H29" s="87"/>
     </row>
     <row r="30" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -6570,10 +6649,10 @@
       <c r="C30" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="120"/>
-      <c r="E30" s="118"/>
-      <c r="F30" s="118"/>
-      <c r="G30" s="120"/>
+      <c r="D30" s="118"/>
+      <c r="E30" s="116"/>
+      <c r="F30" s="116"/>
+      <c r="G30" s="118"/>
       <c r="H30" s="87"/>
     </row>
     <row r="31" spans="1:8" ht="374.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6612,19 +6691,19 @@
       <c r="C32" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="120" t="s">
+      <c r="D32" s="118" t="s">
         <v>224</v>
       </c>
-      <c r="E32" s="118" t="s">
+      <c r="E32" s="116" t="s">
         <v>229</v>
       </c>
-      <c r="F32" s="119" t="s">
+      <c r="F32" s="117" t="s">
         <v>178</v>
       </c>
-      <c r="G32" s="123" t="s">
+      <c r="G32" s="121" t="s">
         <v>243</v>
       </c>
-      <c r="H32" s="121" t="s">
+      <c r="H32" s="120" t="s">
         <v>242</v>
       </c>
     </row>
@@ -6638,11 +6717,11 @@
       <c r="C33" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="123"/>
-      <c r="E33" s="118"/>
-      <c r="F33" s="119"/>
-      <c r="G33" s="123"/>
-      <c r="H33" s="121"/>
+      <c r="D33" s="121"/>
+      <c r="E33" s="116"/>
+      <c r="F33" s="117"/>
+      <c r="G33" s="121"/>
+      <c r="H33" s="120"/>
     </row>
     <row r="34" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="74" t="s">
@@ -6654,11 +6733,11 @@
       <c r="C34" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="123"/>
-      <c r="E34" s="118"/>
-      <c r="F34" s="119"/>
-      <c r="G34" s="123"/>
-      <c r="H34" s="121"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="116"/>
+      <c r="F34" s="117"/>
+      <c r="G34" s="121"/>
+      <c r="H34" s="120"/>
     </row>
     <row r="35" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="80" t="s">
@@ -6670,17 +6749,17 @@
       <c r="C35" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="120" t="s">
+      <c r="D35" s="118" t="s">
         <v>179</v>
       </c>
-      <c r="E35" s="118" t="s">
+      <c r="E35" s="116" t="s">
         <v>180</v>
       </c>
-      <c r="F35" s="118" t="s">
+      <c r="F35" s="116" t="s">
         <v>181</v>
       </c>
-      <c r="G35" s="120"/>
-      <c r="H35" s="121"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="120"/>
     </row>
     <row r="36" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="80" t="s">
@@ -6692,11 +6771,11 @@
       <c r="C36" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="120"/>
-      <c r="E36" s="118"/>
-      <c r="F36" s="118"/>
-      <c r="G36" s="120"/>
-      <c r="H36" s="121"/>
+      <c r="D36" s="118"/>
+      <c r="E36" s="116"/>
+      <c r="F36" s="116"/>
+      <c r="G36" s="118"/>
+      <c r="H36" s="120"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="81" t="s">
@@ -6756,19 +6835,19 @@
       <c r="C39" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D39" s="120" t="s">
+      <c r="D39" s="118" t="s">
         <v>231</v>
       </c>
-      <c r="E39" s="118" t="s">
+      <c r="E39" s="116" t="s">
         <v>188</v>
       </c>
-      <c r="F39" s="118" t="s">
+      <c r="F39" s="116" t="s">
         <v>144</v>
       </c>
-      <c r="G39" s="120" t="s">
+      <c r="G39" s="118" t="s">
         <v>237</v>
       </c>
-      <c r="H39" s="122" t="s">
+      <c r="H39" s="119" t="s">
         <v>236</v>
       </c>
     </row>
@@ -6782,11 +6861,11 @@
       <c r="C40" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="120"/>
-      <c r="E40" s="118"/>
-      <c r="F40" s="118"/>
-      <c r="G40" s="120"/>
-      <c r="H40" s="122"/>
+      <c r="D40" s="118"/>
+      <c r="E40" s="116"/>
+      <c r="F40" s="116"/>
+      <c r="G40" s="118"/>
+      <c r="H40" s="119"/>
     </row>
     <row r="41" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A41" s="78" t="s">
@@ -6798,11 +6877,11 @@
       <c r="C41" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="120"/>
-      <c r="E41" s="118"/>
-      <c r="F41" s="118"/>
-      <c r="G41" s="120"/>
-      <c r="H41" s="122"/>
+      <c r="D41" s="118"/>
+      <c r="E41" s="116"/>
+      <c r="F41" s="116"/>
+      <c r="G41" s="118"/>
+      <c r="H41" s="119"/>
     </row>
     <row r="42" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="78" t="s">
@@ -6814,19 +6893,19 @@
       <c r="C42" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="120" t="s">
+      <c r="D42" s="118" t="s">
         <v>226</v>
       </c>
-      <c r="E42" s="118" t="s">
+      <c r="E42" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="F42" s="118" t="s">
+      <c r="F42" s="116" t="s">
         <v>244</v>
       </c>
-      <c r="G42" s="120" t="s">
+      <c r="G42" s="118" t="s">
         <v>237</v>
       </c>
-      <c r="H42" s="121" t="s">
+      <c r="H42" s="120" t="s">
         <v>236</v>
       </c>
     </row>
@@ -6840,11 +6919,11 @@
       <c r="C43" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="120"/>
-      <c r="E43" s="118"/>
-      <c r="F43" s="118"/>
-      <c r="G43" s="120"/>
-      <c r="H43" s="121"/>
+      <c r="D43" s="118"/>
+      <c r="E43" s="116"/>
+      <c r="F43" s="116"/>
+      <c r="G43" s="118"/>
+      <c r="H43" s="120"/>
     </row>
     <row r="44" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A44" s="78" t="s">
@@ -6856,11 +6935,11 @@
       <c r="C44" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D44" s="120"/>
-      <c r="E44" s="118"/>
-      <c r="F44" s="118"/>
-      <c r="G44" s="120"/>
-      <c r="H44" s="121"/>
+      <c r="D44" s="118"/>
+      <c r="E44" s="116"/>
+      <c r="F44" s="116"/>
+      <c r="G44" s="118"/>
+      <c r="H44" s="120"/>
     </row>
     <row r="45" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A45" s="78" t="s">
@@ -6872,11 +6951,11 @@
       <c r="C45" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="120"/>
-      <c r="E45" s="118"/>
-      <c r="F45" s="118"/>
-      <c r="G45" s="120"/>
-      <c r="H45" s="121"/>
+      <c r="D45" s="118"/>
+      <c r="E45" s="116"/>
+      <c r="F45" s="116"/>
+      <c r="G45" s="118"/>
+      <c r="H45" s="120"/>
     </row>
     <row r="46" spans="1:8" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="78" t="s">
@@ -6888,11 +6967,11 @@
       <c r="C46" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D46" s="120"/>
-      <c r="E46" s="118"/>
-      <c r="F46" s="118"/>
-      <c r="G46" s="120"/>
-      <c r="H46" s="121"/>
+      <c r="D46" s="118"/>
+      <c r="E46" s="116"/>
+      <c r="F46" s="116"/>
+      <c r="G46" s="118"/>
+      <c r="H46" s="120"/>
     </row>
     <row r="47" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A47" s="78" t="s">
@@ -6904,11 +6983,11 @@
       <c r="C47" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D47" s="120"/>
-      <c r="E47" s="118"/>
-      <c r="F47" s="118"/>
-      <c r="G47" s="120"/>
-      <c r="H47" s="121"/>
+      <c r="D47" s="118"/>
+      <c r="E47" s="116"/>
+      <c r="F47" s="116"/>
+      <c r="G47" s="118"/>
+      <c r="H47" s="120"/>
     </row>
     <row r="48" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A48" s="78" t="s">
@@ -6920,11 +6999,11 @@
       <c r="C48" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D48" s="120"/>
-      <c r="E48" s="118"/>
-      <c r="F48" s="118"/>
-      <c r="G48" s="120"/>
-      <c r="H48" s="121"/>
+      <c r="D48" s="118"/>
+      <c r="E48" s="116"/>
+      <c r="F48" s="116"/>
+      <c r="G48" s="118"/>
+      <c r="H48" s="120"/>
     </row>
     <row r="49" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" s="78" t="s">
@@ -6936,11 +7015,11 @@
       <c r="C49" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D49" s="120"/>
-      <c r="E49" s="118"/>
-      <c r="F49" s="118"/>
-      <c r="G49" s="120"/>
-      <c r="H49" s="121"/>
+      <c r="D49" s="118"/>
+      <c r="E49" s="116"/>
+      <c r="F49" s="116"/>
+      <c r="G49" s="118"/>
+      <c r="H49" s="120"/>
     </row>
     <row r="50" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A50" s="78" t="s">
@@ -6952,11 +7031,11 @@
       <c r="C50" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D50" s="120"/>
-      <c r="E50" s="118"/>
-      <c r="F50" s="118"/>
-      <c r="G50" s="120"/>
-      <c r="H50" s="121"/>
+      <c r="D50" s="118"/>
+      <c r="E50" s="116"/>
+      <c r="F50" s="116"/>
+      <c r="G50" s="118"/>
+      <c r="H50" s="120"/>
     </row>
     <row r="51" spans="1:8" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="78" t="s">
@@ -6968,11 +7047,11 @@
       <c r="C51" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D51" s="120"/>
-      <c r="E51" s="118"/>
-      <c r="F51" s="118"/>
-      <c r="G51" s="120"/>
-      <c r="H51" s="121"/>
+      <c r="D51" s="118"/>
+      <c r="E51" s="116"/>
+      <c r="F51" s="116"/>
+      <c r="G51" s="118"/>
+      <c r="H51" s="120"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="78" t="s">
@@ -6984,19 +7063,19 @@
       <c r="C52" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D52" s="120" t="s">
+      <c r="D52" s="118" t="s">
         <v>227</v>
       </c>
-      <c r="E52" s="118" t="s">
+      <c r="E52" s="116" t="s">
         <v>192</v>
       </c>
-      <c r="F52" s="118" t="s">
+      <c r="F52" s="116" t="s">
         <v>144</v>
       </c>
-      <c r="G52" s="120" t="s">
+      <c r="G52" s="118" t="s">
         <v>237</v>
       </c>
-      <c r="H52" s="121" t="s">
+      <c r="H52" s="120" t="s">
         <v>236</v>
       </c>
     </row>
@@ -7010,11 +7089,11 @@
       <c r="C53" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D53" s="120"/>
-      <c r="E53" s="118"/>
-      <c r="F53" s="118"/>
-      <c r="G53" s="120"/>
-      <c r="H53" s="121"/>
+      <c r="D53" s="118"/>
+      <c r="E53" s="116"/>
+      <c r="F53" s="116"/>
+      <c r="G53" s="118"/>
+      <c r="H53" s="120"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="78" t="s">
@@ -7026,11 +7105,11 @@
       <c r="C54" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="120"/>
-      <c r="E54" s="118"/>
-      <c r="F54" s="118"/>
-      <c r="G54" s="120"/>
-      <c r="H54" s="121"/>
+      <c r="D54" s="118"/>
+      <c r="E54" s="116"/>
+      <c r="F54" s="116"/>
+      <c r="G54" s="118"/>
+      <c r="H54" s="120"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="78" t="s">
@@ -7042,50 +7121,14 @@
       <c r="C55" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D55" s="120"/>
-      <c r="E55" s="118"/>
-      <c r="F55" s="118"/>
-      <c r="G55" s="120"/>
-      <c r="H55" s="121"/>
+      <c r="D55" s="118"/>
+      <c r="E55" s="116"/>
+      <c r="F55" s="116"/>
+      <c r="G55" s="118"/>
+      <c r="H55" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E18"/>
-    <mergeCell ref="F4:F18"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="D21:D26"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="F21:F26"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="D42:D51"/>
-    <mergeCell ref="E42:E51"/>
-    <mergeCell ref="F42:F51"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="F52:F55"/>
-    <mergeCell ref="G4:G18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G21:G26"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G32:G34"/>
     <mergeCell ref="G39:G41"/>
     <mergeCell ref="G42:G51"/>
     <mergeCell ref="G52:G55"/>
@@ -7096,6 +7139,42 @@
     <mergeCell ref="H35:H36"/>
     <mergeCell ref="H42:H51"/>
     <mergeCell ref="G35:G36"/>
+    <mergeCell ref="G4:G18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G21:G26"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="D42:D51"/>
+    <mergeCell ref="E42:E51"/>
+    <mergeCell ref="F42:F51"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="F52:F55"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="D21:D26"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="F21:F26"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E18"/>
+    <mergeCell ref="F4:F18"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C37" location="_ftn2" display="_ftn2" xr:uid="{74DB3199-791E-4FED-9C20-E93C69505EA4}"/>
@@ -7145,7 +7224,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="129" t="s">
+      <c r="A3" s="128" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2"/>
@@ -7159,7 +7238,7 @@
       <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="129"/>
+      <c r="A4" s="128"/>
       <c r="B4" s="2"/>
       <c r="C4" s="23" t="s">
         <v>65</v>
@@ -7171,7 +7250,7 @@
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="129"/>
+      <c r="A5" s="128"/>
       <c r="B5" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -7189,7 +7268,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="130" t="s">
+      <c r="A6" s="129" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2">
@@ -7207,7 +7286,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="130"/>
+      <c r="A7" s="129"/>
       <c r="B7" s="2">
         <v>2.2000000000000002</v>
       </c>
@@ -7223,7 +7302,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="130" t="s">
+      <c r="A8" s="129" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2">
@@ -7243,7 +7322,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="130"/>
+      <c r="A9" s="129"/>
       <c r="B9" s="2"/>
       <c r="C9" s="23" t="s">
         <v>64</v>
@@ -7255,7 +7334,7 @@
       <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="130"/>
+      <c r="A10" s="129"/>
       <c r="B10" s="2"/>
       <c r="C10" s="23" t="s">
         <v>55</v>
@@ -7267,7 +7346,7 @@
       <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="130"/>
+      <c r="A11" s="129"/>
       <c r="B11" s="2"/>
       <c r="C11" s="23" t="s">
         <v>50</v>
@@ -7279,7 +7358,7 @@
       <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="130"/>
+      <c r="A12" s="129"/>
       <c r="B12" s="2">
         <v>3.2</v>
       </c>
@@ -7297,7 +7376,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="130"/>
+      <c r="A13" s="129"/>
       <c r="B13" s="2">
         <v>12.1</v>
       </c>
@@ -7313,7 +7392,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="130"/>
+      <c r="A14" s="129"/>
       <c r="B14" s="2">
         <v>12.2</v>
       </c>
@@ -7329,7 +7408,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="130"/>
+      <c r="A15" s="129"/>
       <c r="B15" s="2">
         <v>12.3</v>
       </c>
@@ -7345,7 +7424,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="129" t="s">
+      <c r="A16" s="128" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="18">
@@ -7365,7 +7444,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="129"/>
+      <c r="A17" s="128"/>
       <c r="B17" s="18">
         <v>5.2</v>
       </c>
@@ -7383,7 +7462,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="129"/>
+      <c r="A18" s="128"/>
       <c r="B18" s="2">
         <v>5.3</v>
       </c>
@@ -7401,7 +7480,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="129"/>
+      <c r="A19" s="128"/>
       <c r="B19" s="18">
         <v>5.4</v>
       </c>
@@ -7419,7 +7498,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="129"/>
+      <c r="A20" s="128"/>
       <c r="B20" s="18"/>
       <c r="C20" s="22" t="s">
         <v>53</v>
@@ -7431,7 +7510,7 @@
       <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="129"/>
+      <c r="A21" s="128"/>
       <c r="B21" s="18"/>
       <c r="C21" s="22" t="s">
         <v>54</v>
@@ -7443,7 +7522,7 @@
       <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="129" t="s">
+      <c r="A22" s="128" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="18">
@@ -7463,7 +7542,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="129"/>
+      <c r="A23" s="128"/>
       <c r="B23" s="2"/>
       <c r="C23" s="22" t="s">
         <v>52</v>
@@ -7475,7 +7554,7 @@
       <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="129"/>
+      <c r="A24" s="128"/>
       <c r="B24" s="2"/>
       <c r="C24" s="22" t="s">
         <v>51</v>
@@ -7487,7 +7566,7 @@
       <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="130" t="s">
+      <c r="A25" s="129" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="2">
@@ -7505,7 +7584,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="130"/>
+      <c r="A26" s="129"/>
       <c r="B26" s="2">
         <v>7.2</v>
       </c>
@@ -7521,7 +7600,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="132" t="s">
+      <c r="A27" s="131" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="18">
@@ -7541,7 +7620,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="132"/>
+      <c r="A28" s="131"/>
       <c r="B28" s="18">
         <v>8.1999999999999993</v>
       </c>
@@ -7559,7 +7638,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="132"/>
+      <c r="A29" s="131"/>
       <c r="B29" s="18">
         <v>8.3000000000000007</v>
       </c>
@@ -7577,7 +7656,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="132"/>
+      <c r="A30" s="131"/>
       <c r="B30" s="24">
         <v>8.1</v>
       </c>
@@ -7595,7 +7674,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="132"/>
+      <c r="A31" s="131"/>
       <c r="B31" s="24">
         <v>8.1999999999999993</v>
       </c>
@@ -7613,7 +7692,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="132"/>
+      <c r="A32" s="131"/>
       <c r="B32" s="24">
         <v>8.3000000000000007</v>
       </c>
@@ -7631,7 +7710,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="129" t="s">
+      <c r="A33" s="128" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="2">
@@ -7649,7 +7728,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="129"/>
+      <c r="A34" s="128"/>
       <c r="B34" s="2">
         <v>9.1999999999999993</v>
       </c>
@@ -7665,7 +7744,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="129"/>
+      <c r="A35" s="128"/>
       <c r="B35" s="2"/>
       <c r="C35" s="23" t="s">
         <v>59</v>
@@ -7695,7 +7774,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="131" t="s">
+      <c r="A37" s="130" t="s">
         <v>39</v>
       </c>
       <c r="B37" s="4">
@@ -7713,7 +7792,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="131"/>
+      <c r="A38" s="130"/>
       <c r="B38" s="4">
         <v>11.2</v>
       </c>
@@ -7729,7 +7808,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" s="16" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="131"/>
+      <c r="A39" s="130"/>
       <c r="B39" s="4">
         <v>11.3</v>
       </c>
@@ -7745,7 +7824,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" s="16" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="131"/>
+      <c r="A40" s="130"/>
       <c r="B40" s="4"/>
       <c r="C40" s="22" t="s">
         <v>66</v>
@@ -7757,7 +7836,7 @@
       <c r="F40" s="28"/>
     </row>
     <row r="41" spans="1:6" s="16" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="131"/>
+      <c r="A41" s="130"/>
       <c r="B41" s="4"/>
       <c r="C41" s="22" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Automatic update of 17/05/2024 at 19:35
</commit_message>
<xml_diff>
--- a/Indicadores OPI-CETG rev 28.04.24 v3.xlsx
+++ b/Indicadores OPI-CETG rev 28.04.24 v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\03. Job\05. CONSULTORIAS\13. MEF\FIDT_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409D6B33-4D3D-4716-B96E-9403B0349FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81620A2A-F388-426A-9916-2634B9E5BC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{A4291CEF-37A6-4732-90F4-77F55B4FD4D0}"/>
   </bookViews>
@@ -1284,73 +1284,75 @@
     <t>v33_</t>
   </si>
   <si>
-    <t>v34_</t>
-  </si>
-  <si>
-    <t>v35_</t>
-  </si>
-  <si>
-    <t>v36_</t>
-  </si>
-  <si>
-    <t>v37_</t>
-  </si>
-  <si>
-    <t>v38_</t>
-  </si>
-  <si>
-    <t>v39_</t>
-  </si>
-  <si>
-    <t>v40_</t>
-  </si>
-  <si>
-    <t>v41_</t>
-  </si>
-  <si>
     <t>v42_</t>
   </si>
   <si>
-    <t>v43_</t>
-  </si>
-  <si>
-    <t>v44_</t>
-  </si>
-  <si>
-    <t>v45_</t>
-  </si>
-  <si>
     <t>v46_</t>
   </si>
   <si>
     <t>v47_</t>
   </si>
   <si>
-    <t>v01_</t>
-  </si>
-  <si>
-    <t>v02_</t>
-  </si>
-  <si>
-    <t>v03_</t>
-  </si>
-  <si>
-    <t>v04_</t>
-  </si>
-  <si>
-    <t>v05_</t>
-  </si>
-  <si>
-    <t>v06_</t>
-  </si>
-  <si>
-    <t>v07_</t>
-  </si>
-  <si>
-    <t>v08_</t>
-  </si>
-  <si>
-    <t>v09_</t>
+    <t>v01_Establecimientos_salud_SP</t>
+  </si>
+  <si>
+    <t>v02_Con_discapacidad</t>
+  </si>
+  <si>
+    <t>v03_Sin_seguro</t>
+  </si>
+  <si>
+    <t>v04_Desnutricion_cromica</t>
+  </si>
+  <si>
+    <t>v05_Anemia_total</t>
+  </si>
+  <si>
+    <t>v34_Sin_agua</t>
+  </si>
+  <si>
+    <t>v35_Sin_desagüe</t>
+  </si>
+  <si>
+    <t>v36_Sin_electricidad_rural</t>
+  </si>
+  <si>
+    <t>v37_P_Población_rural</t>
+  </si>
+  <si>
+    <t>v38_Sin_teléfono_celular_rural</t>
+  </si>
+  <si>
+    <t>v39_Sin_teléfono_fijo_rural</t>
+  </si>
+  <si>
+    <t>v40_Sin_conexión_internet_rural</t>
+  </si>
+  <si>
+    <t>v41_Cobertura_inter_fijo_rural
+v41_Cobertura_inter_movil_rural</t>
+  </si>
+  <si>
+    <t>v44_VBP_corriente_2023</t>
+  </si>
+  <si>
+    <t>v45_Número_productores</t>
+  </si>
+  <si>
+    <t>v43_Superficie_agrícola_ha
+v43_Superficie_territorial_ha</t>
+  </si>
+  <si>
+    <t>v06_No_leer_escribir</t>
+  </si>
+  <si>
+    <t>v07_Asiste_IE_otro_distrito</t>
+  </si>
+  <si>
+    <t>v08_Nivel_secundaria_más_17</t>
+  </si>
+  <si>
+    <t>v09_Años_escolaridad</t>
   </si>
 </sst>
 </file>
@@ -1552,7 +1554,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1971,21 +1973,30 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2013,21 +2024,6 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2037,12 +2033,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2064,12 +2060,6 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2080,6 +2070,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2456,8 +2458,8 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="124"/>
-      <c r="B3" s="121" t="s">
+      <c r="A3" s="113"/>
+      <c r="B3" s="110" t="s">
         <v>99</v>
       </c>
       <c r="C3" s="31"/>
@@ -2474,8 +2476,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="124"/>
-      <c r="B4" s="121"/>
+      <c r="A4" s="113"/>
+      <c r="B4" s="110"/>
       <c r="C4" s="31"/>
       <c r="D4" s="23" t="s">
         <v>65</v>
@@ -2487,8 +2489,8 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="124"/>
-      <c r="B5" s="121"/>
+      <c r="A5" s="113"/>
+      <c r="B5" s="110"/>
       <c r="C5" s="31">
         <v>1.1000000000000001</v>
       </c>
@@ -2506,8 +2508,8 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="124"/>
-      <c r="B6" s="121" t="s">
+      <c r="A6" s="113"/>
+      <c r="B6" s="110" t="s">
         <v>68</v>
       </c>
       <c r="C6" s="31">
@@ -2525,8 +2527,8 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="124"/>
-      <c r="B7" s="121"/>
+      <c r="A7" s="113"/>
+      <c r="B7" s="110"/>
       <c r="C7" s="31">
         <v>2.2000000000000002</v>
       </c>
@@ -2542,8 +2544,8 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="124"/>
-      <c r="B8" s="121" t="s">
+      <c r="A8" s="113"/>
+      <c r="B8" s="110" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="31">
@@ -2563,8 +2565,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="124"/>
-      <c r="B9" s="121"/>
+      <c r="A9" s="113"/>
+      <c r="B9" s="110"/>
       <c r="C9" s="31"/>
       <c r="D9" s="23" t="s">
         <v>117</v>
@@ -2579,8 +2581,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="124"/>
-      <c r="B10" s="121"/>
+      <c r="A10" s="113"/>
+      <c r="B10" s="110"/>
       <c r="C10" s="31"/>
       <c r="D10" s="23" t="s">
         <v>105</v>
@@ -2590,13 +2592,13 @@
       </c>
       <c r="F10" s="56"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="122" t="s">
+      <c r="H10" s="111" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="124"/>
-      <c r="B11" s="121"/>
+      <c r="A11" s="113"/>
+      <c r="B11" s="110"/>
       <c r="C11" s="31"/>
       <c r="D11" s="23" t="s">
         <v>50</v>
@@ -2606,11 +2608,11 @@
       </c>
       <c r="F11" s="56"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="122"/>
+      <c r="H11" s="111"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="124"/>
-      <c r="B12" s="121"/>
+      <c r="A12" s="113"/>
+      <c r="B12" s="110"/>
       <c r="C12" s="31">
         <v>3.2</v>
       </c>
@@ -2628,8 +2630,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="124"/>
-      <c r="B13" s="121"/>
+      <c r="A13" s="113"/>
+      <c r="B13" s="110"/>
       <c r="C13" s="31">
         <v>12.1</v>
       </c>
@@ -2645,8 +2647,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="124"/>
-      <c r="B14" s="121"/>
+      <c r="A14" s="113"/>
+      <c r="B14" s="110"/>
       <c r="C14" s="31">
         <v>12.2</v>
       </c>
@@ -2662,8 +2664,8 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="124"/>
-      <c r="B15" s="121"/>
+      <c r="A15" s="113"/>
+      <c r="B15" s="110"/>
       <c r="C15" s="31">
         <v>12.3</v>
       </c>
@@ -2679,8 +2681,8 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="124"/>
-      <c r="B16" s="121" t="s">
+      <c r="A16" s="113"/>
+      <c r="B16" s="110" t="s">
         <v>67</v>
       </c>
       <c r="C16" s="31"/>
@@ -2694,8 +2696,8 @@
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="124"/>
-      <c r="B17" s="121"/>
+      <c r="A17" s="113"/>
+      <c r="B17" s="110"/>
       <c r="C17" s="31"/>
       <c r="D17" s="23" t="s">
         <v>108</v>
@@ -2707,8 +2709,8 @@
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="124"/>
-      <c r="B18" s="121"/>
+      <c r="A18" s="113"/>
+      <c r="B18" s="110"/>
       <c r="C18" s="31"/>
       <c r="D18" s="23" t="s">
         <v>109</v>
@@ -2720,8 +2722,8 @@
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="124"/>
-      <c r="B19" s="121"/>
+      <c r="A19" s="113"/>
+      <c r="B19" s="110"/>
       <c r="C19" s="31"/>
       <c r="D19" s="23" t="s">
         <v>110</v>
@@ -2733,8 +2735,8 @@
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="124"/>
-      <c r="B20" s="121"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="110"/>
       <c r="C20" s="31"/>
       <c r="D20" s="23" t="s">
         <v>111</v>
@@ -2746,8 +2748,8 @@
       <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="124"/>
-      <c r="B21" s="121"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="110"/>
       <c r="C21" s="31"/>
       <c r="D21" s="23" t="s">
         <v>112</v>
@@ -2762,8 +2764,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="124"/>
-      <c r="B22" s="121" t="s">
+      <c r="A22" s="113"/>
+      <c r="B22" s="110" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="35">
@@ -2786,8 +2788,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="124"/>
-      <c r="B23" s="121"/>
+      <c r="A23" s="113"/>
+      <c r="B23" s="110"/>
       <c r="C23" s="35">
         <v>5.2</v>
       </c>
@@ -2808,8 +2810,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="124"/>
-      <c r="B24" s="121"/>
+      <c r="A24" s="113"/>
+      <c r="B24" s="110"/>
       <c r="C24" s="31">
         <v>5.3</v>
       </c>
@@ -2827,8 +2829,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="124"/>
-      <c r="B25" s="121"/>
+      <c r="A25" s="113"/>
+      <c r="B25" s="110"/>
       <c r="C25" s="35">
         <v>5.4</v>
       </c>
@@ -2849,8 +2851,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="124"/>
-      <c r="B26" s="121"/>
+      <c r="A26" s="113"/>
+      <c r="B26" s="110"/>
       <c r="C26" s="35"/>
       <c r="D26" s="41" t="s">
         <v>53</v>
@@ -2865,8 +2867,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="124"/>
-      <c r="B27" s="121"/>
+      <c r="A27" s="113"/>
+      <c r="B27" s="110"/>
       <c r="C27" s="35"/>
       <c r="D27" s="41" t="s">
         <v>54</v>
@@ -2881,8 +2883,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="124"/>
-      <c r="B28" s="121" t="s">
+      <c r="A28" s="113"/>
+      <c r="B28" s="110" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="35">
@@ -2905,8 +2907,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="124"/>
-      <c r="B29" s="121"/>
+      <c r="A29" s="113"/>
+      <c r="B29" s="110"/>
       <c r="C29" s="31"/>
       <c r="D29" s="41" t="s">
         <v>51</v>
@@ -2921,8 +2923,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="124"/>
-      <c r="B30" s="121"/>
+      <c r="A30" s="113"/>
+      <c r="B30" s="110"/>
       <c r="C30" s="31"/>
       <c r="D30" s="41" t="s">
         <v>52</v>
@@ -2937,8 +2939,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="124"/>
-      <c r="B31" s="121" t="s">
+      <c r="A31" s="113"/>
+      <c r="B31" s="110" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="31">
@@ -2956,8 +2958,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="124"/>
-      <c r="B32" s="121"/>
+      <c r="A32" s="113"/>
+      <c r="B32" s="110"/>
       <c r="C32" s="31">
         <v>7.2</v>
       </c>
@@ -2973,8 +2975,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="124"/>
-      <c r="B33" s="121" t="s">
+      <c r="A33" s="113"/>
+      <c r="B33" s="110" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="35">
@@ -2997,8 +2999,8 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="124"/>
-      <c r="B34" s="121"/>
+      <c r="A34" s="113"/>
+      <c r="B34" s="110"/>
       <c r="C34" s="35">
         <v>8.1999999999999993</v>
       </c>
@@ -3019,8 +3021,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="124"/>
-      <c r="B35" s="121"/>
+      <c r="A35" s="113"/>
+      <c r="B35" s="110"/>
       <c r="C35" s="35">
         <v>8.3000000000000007</v>
       </c>
@@ -3041,8 +3043,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="124"/>
-      <c r="B36" s="121"/>
+      <c r="A36" s="113"/>
+      <c r="B36" s="110"/>
       <c r="C36" s="32">
         <v>8.1</v>
       </c>
@@ -3063,8 +3065,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="124"/>
-      <c r="B37" s="121"/>
+      <c r="A37" s="113"/>
+      <c r="B37" s="110"/>
       <c r="C37" s="32">
         <v>8.1999999999999993</v>
       </c>
@@ -3085,8 +3087,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="124"/>
-      <c r="B38" s="121"/>
+      <c r="A38" s="113"/>
+      <c r="B38" s="110"/>
       <c r="C38" s="32">
         <v>8.3000000000000007</v>
       </c>
@@ -3107,8 +3109,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="124"/>
-      <c r="B39" s="121"/>
+      <c r="A39" s="113"/>
+      <c r="B39" s="110"/>
       <c r="C39" s="32"/>
       <c r="D39" s="22" t="s">
         <v>72</v>
@@ -3120,8 +3122,8 @@
       <c r="G39" s="43"/>
     </row>
     <row r="40" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="124"/>
-      <c r="B40" s="121" t="s">
+      <c r="A40" s="113"/>
+      <c r="B40" s="110" t="s">
         <v>34</v>
       </c>
       <c r="C40" s="31">
@@ -3139,8 +3141,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="124"/>
-      <c r="B41" s="121"/>
+      <c r="A41" s="113"/>
+      <c r="B41" s="110"/>
       <c r="C41" s="31">
         <v>9.1999999999999993</v>
       </c>
@@ -3156,8 +3158,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="124"/>
-      <c r="B42" s="121"/>
+      <c r="A42" s="113"/>
+      <c r="B42" s="110"/>
       <c r="C42" s="31"/>
       <c r="D42" s="23" t="s">
         <v>59</v>
@@ -3169,8 +3171,8 @@
       <c r="G42" s="12"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="124"/>
-      <c r="B43" s="121"/>
+      <c r="A43" s="113"/>
+      <c r="B43" s="110"/>
       <c r="C43" s="31"/>
       <c r="D43" s="22" t="s">
         <v>86</v>
@@ -3185,8 +3187,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="124"/>
-      <c r="B44" s="121"/>
+      <c r="A44" s="113"/>
+      <c r="B44" s="110"/>
       <c r="C44" s="31"/>
       <c r="D44" s="22" t="s">
         <v>87</v>
@@ -3201,8 +3203,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="124"/>
-      <c r="B45" s="121"/>
+      <c r="A45" s="113"/>
+      <c r="B45" s="110"/>
       <c r="C45" s="31"/>
       <c r="D45" s="22" t="s">
         <v>100</v>
@@ -3217,10 +3219,10 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="124" t="s">
+      <c r="A46" s="113" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="123" t="s">
+      <c r="B46" s="112" t="s">
         <v>114</v>
       </c>
       <c r="C46" s="34">
@@ -3241,8 +3243,8 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="124"/>
-      <c r="B47" s="123"/>
+      <c r="A47" s="113"/>
+      <c r="B47" s="112"/>
       <c r="C47" s="34">
         <v>11.2</v>
       </c>
@@ -3261,8 +3263,8 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="124"/>
-      <c r="B48" s="123"/>
+      <c r="A48" s="113"/>
+      <c r="B48" s="112"/>
       <c r="C48" s="34">
         <v>11.3</v>
       </c>
@@ -3281,8 +3283,8 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="124"/>
-      <c r="B49" s="123"/>
+      <c r="A49" s="113"/>
+      <c r="B49" s="112"/>
       <c r="C49" s="34"/>
       <c r="D49" s="22" t="s">
         <v>66</v>
@@ -3297,8 +3299,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="124"/>
-      <c r="B50" s="123"/>
+      <c r="A50" s="113"/>
+      <c r="B50" s="112"/>
       <c r="C50" s="34"/>
       <c r="D50" s="22" t="s">
         <v>63</v>
@@ -3313,10 +3315,10 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="120" t="s">
+      <c r="A51" s="109" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="120"/>
+      <c r="B51" s="109"/>
       <c r="C51" s="62"/>
       <c r="D51" s="52" t="s">
         <v>115</v>
@@ -3329,8 +3331,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="120"/>
-      <c r="B52" s="120"/>
+      <c r="A52" s="109"/>
+      <c r="B52" s="109"/>
       <c r="C52" s="62"/>
       <c r="D52" s="52" t="s">
         <v>89</v>
@@ -3341,8 +3343,8 @@
       <c r="F52" s="47"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="120"/>
-      <c r="B53" s="120"/>
+      <c r="A53" s="109"/>
+      <c r="B53" s="109"/>
       <c r="C53" s="62"/>
       <c r="D53" s="54" t="s">
         <v>38</v>
@@ -3353,8 +3355,8 @@
       <c r="F53" s="47"/>
     </row>
     <row r="54" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="120"/>
-      <c r="B54" s="120"/>
+      <c r="A54" s="109"/>
+      <c r="B54" s="109"/>
       <c r="C54" s="62"/>
       <c r="D54" s="52" t="s">
         <v>81</v>
@@ -3365,41 +3367,41 @@
       <c r="F54" s="47"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="111" t="s">
+      <c r="A55" s="114" t="s">
         <v>126</v>
       </c>
-      <c r="B55" s="111"/>
-      <c r="C55" s="111"/>
-      <c r="D55" s="111"/>
-      <c r="E55" s="111"/>
+      <c r="B55" s="114"/>
+      <c r="C55" s="114"/>
+      <c r="D55" s="114"/>
+      <c r="E55" s="114"/>
       <c r="F55" s="47"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="112"/>
-      <c r="B56" s="112"/>
-      <c r="C56" s="112"/>
-      <c r="D56" s="112"/>
-      <c r="E56" s="112"/>
+      <c r="A56" s="115"/>
+      <c r="B56" s="115"/>
+      <c r="C56" s="115"/>
+      <c r="D56" s="115"/>
+      <c r="E56" s="115"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="112"/>
-      <c r="B57" s="112"/>
-      <c r="C57" s="112"/>
-      <c r="D57" s="112"/>
-      <c r="E57" s="112"/>
+      <c r="A57" s="115"/>
+      <c r="B57" s="115"/>
+      <c r="C57" s="115"/>
+      <c r="D57" s="115"/>
+      <c r="E57" s="115"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="113"/>
-      <c r="B58" s="113"/>
-      <c r="C58" s="113"/>
-      <c r="D58" s="113"/>
-      <c r="E58" s="113"/>
+      <c r="A58" s="116"/>
+      <c r="B58" s="116"/>
+      <c r="C58" s="116"/>
+      <c r="D58" s="116"/>
+      <c r="E58" s="116"/>
     </row>
     <row r="59" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A59" s="114" t="s">
+      <c r="A59" s="117" t="s">
         <v>118</v>
       </c>
-      <c r="B59" s="117" t="s">
+      <c r="B59" s="120" t="s">
         <v>125</v>
       </c>
       <c r="C59" s="64"/>
@@ -3414,8 +3416,8 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="114"/>
-      <c r="B60" s="118"/>
+      <c r="A60" s="117"/>
+      <c r="B60" s="121"/>
       <c r="C60" s="64"/>
       <c r="D60" s="69" t="s">
         <v>137</v>
@@ -3428,8 +3430,8 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="114"/>
-      <c r="B61" s="119"/>
+      <c r="A61" s="117"/>
+      <c r="B61" s="122"/>
       <c r="C61" s="64"/>
       <c r="D61" s="69" t="s">
         <v>138</v>
@@ -3442,8 +3444,8 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="114"/>
-      <c r="B62" s="115" t="s">
+      <c r="A62" s="117"/>
+      <c r="B62" s="118" t="s">
         <v>120</v>
       </c>
       <c r="C62" s="66"/>
@@ -3458,8 +3460,8 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="114"/>
-      <c r="B63" s="115"/>
+      <c r="A63" s="117"/>
+      <c r="B63" s="118"/>
       <c r="C63" s="66"/>
       <c r="D63" s="67" t="s">
         <v>139</v>
@@ -3472,8 +3474,8 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A64" s="114"/>
-      <c r="B64" s="115"/>
+      <c r="A64" s="117"/>
+      <c r="B64" s="118"/>
       <c r="C64" s="66"/>
       <c r="D64" s="67" t="s">
         <v>128</v>
@@ -3486,8 +3488,8 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A65" s="114"/>
-      <c r="B65" s="115"/>
+      <c r="A65" s="117"/>
+      <c r="B65" s="118"/>
       <c r="C65" s="66"/>
       <c r="D65" s="67" t="s">
         <v>129</v>
@@ -3500,8 +3502,8 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="114"/>
-      <c r="B66" s="115"/>
+      <c r="A66" s="117"/>
+      <c r="B66" s="118"/>
       <c r="C66" s="66"/>
       <c r="D66" s="67" t="s">
         <v>130</v>
@@ -3514,8 +3516,8 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="114"/>
-      <c r="B67" s="115" t="s">
+      <c r="A67" s="117"/>
+      <c r="B67" s="118" t="s">
         <v>122</v>
       </c>
       <c r="C67" s="66"/>
@@ -3530,8 +3532,8 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="114"/>
-      <c r="B68" s="115"/>
+      <c r="A68" s="117"/>
+      <c r="B68" s="118"/>
       <c r="C68" s="66"/>
       <c r="D68" s="67" t="s">
         <v>133</v>
@@ -3544,8 +3546,8 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A69" s="114"/>
-      <c r="B69" s="115"/>
+      <c r="A69" s="117"/>
+      <c r="B69" s="118"/>
       <c r="C69" s="66"/>
       <c r="D69" s="67" t="s">
         <v>132</v>
@@ -3558,8 +3560,8 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="114"/>
-      <c r="B70" s="115"/>
+      <c r="A70" s="117"/>
+      <c r="B70" s="118"/>
       <c r="C70" s="66"/>
       <c r="D70" s="68" t="s">
         <v>135</v>
@@ -3572,8 +3574,8 @@
       </c>
     </row>
     <row r="71" spans="1:8" s="16" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="114"/>
-      <c r="B71" s="116" t="s">
+      <c r="A71" s="117"/>
+      <c r="B71" s="119" t="s">
         <v>123</v>
       </c>
       <c r="C71" s="64"/>
@@ -3589,8 +3591,8 @@
       <c r="H71" s="71"/>
     </row>
     <row r="72" spans="1:8" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="114"/>
-      <c r="B72" s="116"/>
+      <c r="A72" s="117"/>
+      <c r="B72" s="119"/>
       <c r="C72" s="64"/>
       <c r="D72" s="69" t="s">
         <v>141</v>
@@ -3604,8 +3606,8 @@
       <c r="H72" s="71"/>
     </row>
     <row r="73" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="114"/>
-      <c r="B73" s="115" t="s">
+      <c r="A73" s="117"/>
+      <c r="B73" s="118" t="s">
         <v>124</v>
       </c>
       <c r="C73" s="66"/>
@@ -3620,8 +3622,8 @@
       </c>
     </row>
     <row r="74" spans="1:8" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.25">
-      <c r="A74" s="114"/>
-      <c r="B74" s="115"/>
+      <c r="A74" s="117"/>
+      <c r="B74" s="118"/>
       <c r="C74" s="64"/>
       <c r="D74" s="69" t="s">
         <v>134</v>
@@ -3644,6 +3646,13 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A55:E58"/>
+    <mergeCell ref="A59:A74"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="B59:B61"/>
     <mergeCell ref="A51:B54"/>
     <mergeCell ref="B16:B21"/>
     <mergeCell ref="H10:H11"/>
@@ -3658,13 +3667,6 @@
     <mergeCell ref="B22:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B32"/>
-    <mergeCell ref="A55:E58"/>
-    <mergeCell ref="A59:A74"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="B59:B61"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E53" location="_ftn2" display="_ftn2" xr:uid="{FFC9BABA-D715-48D2-801D-3C2A2DB136EB}"/>
@@ -3753,13 +3755,13 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="127" t="s">
+      <c r="D4" s="125" t="s">
         <v>161</v>
       </c>
-      <c r="E4" s="125" t="s">
+      <c r="E4" s="123" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="125" t="s">
+      <c r="F4" s="123" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3773,9 +3775,9 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="127"/>
-      <c r="E5" s="125"/>
-      <c r="F5" s="125"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
@@ -3787,11 +3789,11 @@
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="127" t="s">
+      <c r="D6" s="125" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="125"/>
-      <c r="F6" s="125"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
@@ -3803,9 +3805,9 @@
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="127"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="123"/>
     </row>
     <row r="8" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="74" t="s">
@@ -3817,11 +3819,11 @@
       <c r="C8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="125" t="s">
+      <c r="D8" s="123" t="s">
         <v>164</v>
       </c>
-      <c r="E8" s="125"/>
-      <c r="F8" s="125"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
@@ -3833,9 +3835,9 @@
       <c r="C9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="125"/>
-      <c r="E9" s="125"/>
-      <c r="F9" s="125"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
@@ -3847,11 +3849,11 @@
       <c r="C10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="125" t="s">
+      <c r="D10" s="123" t="s">
         <v>165</v>
       </c>
-      <c r="E10" s="125"/>
-      <c r="F10" s="125"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="74" t="s">
@@ -3863,9 +3865,9 @@
       <c r="C11" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="125"/>
-      <c r="E11" s="125"/>
-      <c r="F11" s="125"/>
+      <c r="D11" s="123"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
@@ -3877,9 +3879,9 @@
       <c r="C12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="125"/>
-      <c r="E12" s="125"/>
-      <c r="F12" s="125"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="78" t="s">
@@ -3891,11 +3893,11 @@
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="125" t="s">
+      <c r="D13" s="123" t="s">
         <v>166</v>
       </c>
-      <c r="E13" s="125"/>
-      <c r="F13" s="125"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="123"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="78" t="s">
@@ -3907,9 +3909,9 @@
       <c r="C14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="125"/>
-      <c r="E14" s="125"/>
-      <c r="F14" s="125"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="123"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="78" t="s">
@@ -3921,9 +3923,9 @@
       <c r="C15" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="125"/>
-      <c r="E15" s="125"/>
-      <c r="F15" s="125"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="78" t="s">
@@ -3935,9 +3937,9 @@
       <c r="C16" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="125"/>
-      <c r="E16" s="125"/>
-      <c r="F16" s="125"/>
+      <c r="D16" s="123"/>
+      <c r="E16" s="123"/>
+      <c r="F16" s="123"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="78" t="s">
@@ -3949,9 +3951,9 @@
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="125"/>
-      <c r="E17" s="125"/>
-      <c r="F17" s="125"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="123"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
@@ -3966,8 +3968,8 @@
       <c r="D18" s="79" t="s">
         <v>167</v>
       </c>
-      <c r="E18" s="125"/>
-      <c r="F18" s="125"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="123"/>
     </row>
     <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
@@ -3979,13 +3981,13 @@
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="125" t="s">
+      <c r="D19" s="123" t="s">
         <v>168</v>
       </c>
-      <c r="E19" s="125" t="s">
+      <c r="E19" s="123" t="s">
         <v>197</v>
       </c>
-      <c r="F19" s="125" t="s">
+      <c r="F19" s="123" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3999,9 +4001,9 @@
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="125"/>
-      <c r="E20" s="125"/>
-      <c r="F20" s="125"/>
+      <c r="D20" s="123"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="123"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
@@ -4013,13 +4015,13 @@
       <c r="C21" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="125" t="s">
+      <c r="D21" s="123" t="s">
         <v>170</v>
       </c>
-      <c r="E21" s="125" t="s">
+      <c r="E21" s="123" t="s">
         <v>172</v>
       </c>
-      <c r="F21" s="126" t="s">
+      <c r="F21" s="124" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4033,9 +4035,9 @@
       <c r="C22" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="125"/>
-      <c r="E22" s="125"/>
-      <c r="F22" s="126"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="123"/>
+      <c r="F22" s="124"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="74" t="s">
@@ -4047,9 +4049,9 @@
       <c r="C23" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="125"/>
-      <c r="E23" s="125"/>
-      <c r="F23" s="126"/>
+      <c r="D23" s="123"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="124"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="74" t="s">
@@ -4061,9 +4063,9 @@
       <c r="C24" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="125"/>
-      <c r="E24" s="125"/>
-      <c r="F24" s="126"/>
+      <c r="D24" s="123"/>
+      <c r="E24" s="123"/>
+      <c r="F24" s="124"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="74" t="s">
@@ -4075,9 +4077,9 @@
       <c r="C25" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="125"/>
-      <c r="E25" s="125"/>
-      <c r="F25" s="126"/>
+      <c r="D25" s="123"/>
+      <c r="E25" s="123"/>
+      <c r="F25" s="124"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="74" t="s">
@@ -4089,9 +4091,9 @@
       <c r="C26" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="125"/>
-      <c r="E26" s="125"/>
-      <c r="F26" s="126"/>
+      <c r="D26" s="123"/>
+      <c r="E26" s="123"/>
+      <c r="F26" s="124"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="74" t="s">
@@ -4103,13 +4105,13 @@
       <c r="C27" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="125" t="s">
+      <c r="D27" s="123" t="s">
         <v>174</v>
       </c>
-      <c r="E27" s="125" t="s">
+      <c r="E27" s="123" t="s">
         <v>175</v>
       </c>
-      <c r="F27" s="125" t="s">
+      <c r="F27" s="123" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4123,9 +4125,9 @@
       <c r="C28" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="125"/>
-      <c r="E28" s="125"/>
-      <c r="F28" s="125"/>
+      <c r="D28" s="123"/>
+      <c r="E28" s="123"/>
+      <c r="F28" s="123"/>
     </row>
     <row r="29" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="74" t="s">
@@ -4137,9 +4139,9 @@
       <c r="C29" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D29" s="125"/>
-      <c r="E29" s="125"/>
-      <c r="F29" s="125"/>
+      <c r="D29" s="123"/>
+      <c r="E29" s="123"/>
+      <c r="F29" s="123"/>
     </row>
     <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="74" t="s">
@@ -4151,9 +4153,9 @@
       <c r="C30" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="125"/>
-      <c r="E30" s="125"/>
-      <c r="F30" s="125"/>
+      <c r="D30" s="123"/>
+      <c r="E30" s="123"/>
+      <c r="F30" s="123"/>
     </row>
     <row r="31" spans="1:6" ht="409.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="74" t="s">
@@ -4185,13 +4187,13 @@
       <c r="C32" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="125" t="s">
+      <c r="D32" s="123" t="s">
         <v>176</v>
       </c>
-      <c r="E32" s="125" t="s">
+      <c r="E32" s="123" t="s">
         <v>177</v>
       </c>
-      <c r="F32" s="126" t="s">
+      <c r="F32" s="124" t="s">
         <v>178</v>
       </c>
     </row>
@@ -4205,9 +4207,9 @@
       <c r="C33" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="126"/>
-      <c r="E33" s="125"/>
-      <c r="F33" s="126"/>
+      <c r="D33" s="124"/>
+      <c r="E33" s="123"/>
+      <c r="F33" s="124"/>
     </row>
     <row r="34" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="74" t="s">
@@ -4219,9 +4221,9 @@
       <c r="C34" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="126"/>
-      <c r="E34" s="125"/>
-      <c r="F34" s="126"/>
+      <c r="D34" s="124"/>
+      <c r="E34" s="123"/>
+      <c r="F34" s="124"/>
     </row>
     <row r="35" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="80" t="s">
@@ -4233,13 +4235,13 @@
       <c r="C35" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="125" t="s">
+      <c r="D35" s="123" t="s">
         <v>179</v>
       </c>
-      <c r="E35" s="125" t="s">
+      <c r="E35" s="123" t="s">
         <v>180</v>
       </c>
-      <c r="F35" s="125" t="s">
+      <c r="F35" s="123" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4253,9 +4255,9 @@
       <c r="C36" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="125"/>
-      <c r="E36" s="125"/>
-      <c r="F36" s="125"/>
+      <c r="D36" s="123"/>
+      <c r="E36" s="123"/>
+      <c r="F36" s="123"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="81" t="s">
@@ -4307,13 +4309,13 @@
       <c r="C39" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D39" s="125" t="s">
+      <c r="D39" s="123" t="s">
         <v>187</v>
       </c>
-      <c r="E39" s="125" t="s">
+      <c r="E39" s="123" t="s">
         <v>188</v>
       </c>
-      <c r="F39" s="125" t="s">
+      <c r="F39" s="123" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4327,9 +4329,9 @@
       <c r="C40" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="125"/>
-      <c r="E40" s="125"/>
-      <c r="F40" s="125"/>
+      <c r="D40" s="123"/>
+      <c r="E40" s="123"/>
+      <c r="F40" s="123"/>
     </row>
     <row r="41" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A41" s="78" t="s">
@@ -4341,9 +4343,9 @@
       <c r="C41" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="125"/>
-      <c r="E41" s="125"/>
-      <c r="F41" s="125"/>
+      <c r="D41" s="123"/>
+      <c r="E41" s="123"/>
+      <c r="F41" s="123"/>
     </row>
     <row r="42" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="78" t="s">
@@ -4355,13 +4357,13 @@
       <c r="C42" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="125" t="s">
+      <c r="D42" s="123" t="s">
         <v>189</v>
       </c>
-      <c r="E42" s="125" t="s">
+      <c r="E42" s="123" t="s">
         <v>190</v>
       </c>
-      <c r="F42" s="125" t="s">
+      <c r="F42" s="123" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4375,9 +4377,9 @@
       <c r="C43" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="125"/>
-      <c r="E43" s="125"/>
-      <c r="F43" s="125"/>
+      <c r="D43" s="123"/>
+      <c r="E43" s="123"/>
+      <c r="F43" s="123"/>
     </row>
     <row r="44" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A44" s="78" t="s">
@@ -4389,9 +4391,9 @@
       <c r="C44" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D44" s="125"/>
-      <c r="E44" s="125"/>
-      <c r="F44" s="125"/>
+      <c r="D44" s="123"/>
+      <c r="E44" s="123"/>
+      <c r="F44" s="123"/>
     </row>
     <row r="45" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A45" s="78" t="s">
@@ -4403,9 +4405,9 @@
       <c r="C45" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="125"/>
-      <c r="E45" s="125"/>
-      <c r="F45" s="125"/>
+      <c r="D45" s="123"/>
+      <c r="E45" s="123"/>
+      <c r="F45" s="123"/>
     </row>
     <row r="46" spans="1:6" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="78" t="s">
@@ -4417,9 +4419,9 @@
       <c r="C46" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D46" s="125"/>
-      <c r="E46" s="125"/>
-      <c r="F46" s="125"/>
+      <c r="D46" s="123"/>
+      <c r="E46" s="123"/>
+      <c r="F46" s="123"/>
     </row>
     <row r="47" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A47" s="78" t="s">
@@ -4431,9 +4433,9 @@
       <c r="C47" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D47" s="125"/>
-      <c r="E47" s="125"/>
-      <c r="F47" s="125"/>
+      <c r="D47" s="123"/>
+      <c r="E47" s="123"/>
+      <c r="F47" s="123"/>
     </row>
     <row r="48" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A48" s="78" t="s">
@@ -4445,9 +4447,9 @@
       <c r="C48" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D48" s="125"/>
-      <c r="E48" s="125"/>
-      <c r="F48" s="125"/>
+      <c r="D48" s="123"/>
+      <c r="E48" s="123"/>
+      <c r="F48" s="123"/>
     </row>
     <row r="49" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" s="78" t="s">
@@ -4459,9 +4461,9 @@
       <c r="C49" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D49" s="125"/>
-      <c r="E49" s="125"/>
-      <c r="F49" s="125"/>
+      <c r="D49" s="123"/>
+      <c r="E49" s="123"/>
+      <c r="F49" s="123"/>
     </row>
     <row r="50" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A50" s="78" t="s">
@@ -4473,9 +4475,9 @@
       <c r="C50" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D50" s="125"/>
-      <c r="E50" s="125"/>
-      <c r="F50" s="125"/>
+      <c r="D50" s="123"/>
+      <c r="E50" s="123"/>
+      <c r="F50" s="123"/>
     </row>
     <row r="51" spans="1:6" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="78" t="s">
@@ -4487,9 +4489,9 @@
       <c r="C51" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D51" s="125"/>
-      <c r="E51" s="125"/>
-      <c r="F51" s="125"/>
+      <c r="D51" s="123"/>
+      <c r="E51" s="123"/>
+      <c r="F51" s="123"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="78" t="s">
@@ -4501,13 +4503,13 @@
       <c r="C52" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D52" s="125" t="s">
+      <c r="D52" s="123" t="s">
         <v>191</v>
       </c>
-      <c r="E52" s="125" t="s">
+      <c r="E52" s="123" t="s">
         <v>192</v>
       </c>
-      <c r="F52" s="125" t="s">
+      <c r="F52" s="123" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4521,9 +4523,9 @@
       <c r="C53" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D53" s="125"/>
-      <c r="E53" s="125"/>
-      <c r="F53" s="125"/>
+      <c r="D53" s="123"/>
+      <c r="E53" s="123"/>
+      <c r="F53" s="123"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="78" t="s">
@@ -4535,9 +4537,9 @@
       <c r="C54" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="125"/>
-      <c r="E54" s="125"/>
-      <c r="F54" s="125"/>
+      <c r="D54" s="123"/>
+      <c r="E54" s="123"/>
+      <c r="F54" s="123"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="78" t="s">
@@ -4549,30 +4551,12 @@
       <c r="C55" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D55" s="125"/>
-      <c r="E55" s="125"/>
-      <c r="F55" s="125"/>
+      <c r="D55" s="123"/>
+      <c r="E55" s="123"/>
+      <c r="F55" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="F52:F55"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="D42:D51"/>
-    <mergeCell ref="E42:E51"/>
-    <mergeCell ref="F42:F51"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="F32:F34"/>
     <mergeCell ref="D13:D17"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
@@ -4586,6 +4570,24 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="F52:F55"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="D42:D51"/>
+    <mergeCell ref="E42:E51"/>
+    <mergeCell ref="F42:F51"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C37" location="_ftn2" display="_ftn2" xr:uid="{25CB2AF1-E91C-4F96-A745-EB04437048A9}"/>
@@ -4677,16 +4679,16 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="127" t="s">
+      <c r="D4" s="125" t="s">
         <v>215</v>
       </c>
-      <c r="E4" s="125" t="s">
+      <c r="E4" s="123" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="125" t="s">
+      <c r="F4" s="123" t="s">
         <v>158</v>
       </c>
-      <c r="G4" s="127"/>
+      <c r="G4" s="125"/>
       <c r="H4" s="87"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4699,10 +4701,10 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="127"/>
-      <c r="E5" s="125"/>
-      <c r="F5" s="125"/>
-      <c r="G5" s="127"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="125"/>
       <c r="H5" s="87"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4715,12 +4717,12 @@
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="127" t="s">
+      <c r="D6" s="125" t="s">
         <v>216</v>
       </c>
-      <c r="E6" s="125"/>
-      <c r="F6" s="125"/>
-      <c r="G6" s="127"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="125"/>
       <c r="H6" s="87"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4733,10 +4735,10 @@
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="127"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="127"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="125"/>
       <c r="H7" s="87"/>
     </row>
     <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4749,12 +4751,12 @@
       <c r="C8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="127" t="s">
+      <c r="D8" s="125" t="s">
         <v>164</v>
       </c>
-      <c r="E8" s="125"/>
-      <c r="F8" s="125"/>
-      <c r="G8" s="127"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="125"/>
       <c r="H8" s="87"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4767,10 +4769,10 @@
       <c r="C9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="127"/>
-      <c r="E9" s="125"/>
-      <c r="F9" s="125"/>
-      <c r="G9" s="127"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="125"/>
       <c r="H9" s="87"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4783,12 +4785,12 @@
       <c r="C10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="127" t="s">
+      <c r="D10" s="125" t="s">
         <v>217</v>
       </c>
-      <c r="E10" s="125"/>
-      <c r="F10" s="125"/>
-      <c r="G10" s="127"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="125"/>
       <c r="H10" s="87"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4801,10 +4803,10 @@
       <c r="C11" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="127"/>
-      <c r="E11" s="125"/>
-      <c r="F11" s="125"/>
-      <c r="G11" s="127"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="125"/>
       <c r="H11" s="87"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4817,10 +4819,10 @@
       <c r="C12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="127"/>
-      <c r="E12" s="125"/>
-      <c r="F12" s="125"/>
-      <c r="G12" s="127"/>
+      <c r="D12" s="125"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="125"/>
       <c r="H12" s="87"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4833,12 +4835,12 @@
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="127" t="s">
+      <c r="D13" s="125" t="s">
         <v>218</v>
       </c>
-      <c r="E13" s="125"/>
-      <c r="F13" s="125"/>
-      <c r="G13" s="127"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="125"/>
       <c r="H13" s="87"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4851,10 +4853,10 @@
       <c r="C14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="127"/>
-      <c r="E14" s="125"/>
-      <c r="F14" s="125"/>
-      <c r="G14" s="127"/>
+      <c r="D14" s="125"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="125"/>
       <c r="H14" s="87"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4867,10 +4869,10 @@
       <c r="C15" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="127"/>
-      <c r="E15" s="125"/>
-      <c r="F15" s="125"/>
-      <c r="G15" s="127"/>
+      <c r="D15" s="125"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
+      <c r="G15" s="125"/>
       <c r="H15" s="87"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4883,10 +4885,10 @@
       <c r="C16" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="127"/>
-      <c r="E16" s="125"/>
-      <c r="F16" s="125"/>
-      <c r="G16" s="127"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="123"/>
+      <c r="F16" s="123"/>
+      <c r="G16" s="125"/>
       <c r="H16" s="87"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -4899,10 +4901,10 @@
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="127"/>
-      <c r="E17" s="125"/>
-      <c r="F17" s="125"/>
-      <c r="G17" s="127"/>
+      <c r="D17" s="125"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="123"/>
+      <c r="G17" s="125"/>
       <c r="H17" s="87"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -4918,9 +4920,9 @@
       <c r="D18" s="83" t="s">
         <v>219</v>
       </c>
-      <c r="E18" s="125"/>
-      <c r="F18" s="125"/>
-      <c r="G18" s="127"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="123"/>
+      <c r="G18" s="125"/>
       <c r="H18" s="87"/>
     </row>
     <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -4933,19 +4935,19 @@
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="127" t="s">
+      <c r="D19" s="125" t="s">
         <v>220</v>
       </c>
-      <c r="E19" s="125" t="s">
+      <c r="E19" s="123" t="s">
         <v>197</v>
       </c>
-      <c r="F19" s="125" t="s">
+      <c r="F19" s="123" t="s">
         <v>169</v>
       </c>
-      <c r="G19" s="127" t="s">
+      <c r="G19" s="125" t="s">
         <v>235</v>
       </c>
-      <c r="H19" s="129" t="s">
+      <c r="H19" s="126" t="s">
         <v>234</v>
       </c>
     </row>
@@ -4959,11 +4961,11 @@
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="127"/>
-      <c r="E20" s="125"/>
-      <c r="F20" s="125"/>
-      <c r="G20" s="127"/>
-      <c r="H20" s="129"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="123"/>
+      <c r="G20" s="125"/>
+      <c r="H20" s="126"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
@@ -4975,16 +4977,16 @@
       <c r="C21" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="127" t="s">
+      <c r="D21" s="125" t="s">
         <v>221</v>
       </c>
-      <c r="E21" s="125" t="s">
+      <c r="E21" s="123" t="s">
         <v>172</v>
       </c>
-      <c r="F21" s="126" t="s">
+      <c r="F21" s="124" t="s">
         <v>173</v>
       </c>
-      <c r="G21" s="130"/>
+      <c r="G21" s="128"/>
       <c r="H21" s="87"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -4997,10 +4999,10 @@
       <c r="C22" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="127"/>
-      <c r="E22" s="125"/>
-      <c r="F22" s="126"/>
-      <c r="G22" s="130"/>
+      <c r="D22" s="125"/>
+      <c r="E22" s="123"/>
+      <c r="F22" s="124"/>
+      <c r="G22" s="128"/>
       <c r="H22" s="87"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -5013,10 +5015,10 @@
       <c r="C23" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="127"/>
-      <c r="E23" s="125"/>
-      <c r="F23" s="126"/>
-      <c r="G23" s="130"/>
+      <c r="D23" s="125"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="124"/>
+      <c r="G23" s="128"/>
       <c r="H23" s="87"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -5029,10 +5031,10 @@
       <c r="C24" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="127"/>
-      <c r="E24" s="125"/>
-      <c r="F24" s="126"/>
-      <c r="G24" s="130"/>
+      <c r="D24" s="125"/>
+      <c r="E24" s="123"/>
+      <c r="F24" s="124"/>
+      <c r="G24" s="128"/>
       <c r="H24" s="87"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -5045,10 +5047,10 @@
       <c r="C25" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="127"/>
-      <c r="E25" s="125"/>
-      <c r="F25" s="126"/>
-      <c r="G25" s="130"/>
+      <c r="D25" s="125"/>
+      <c r="E25" s="123"/>
+      <c r="F25" s="124"/>
+      <c r="G25" s="128"/>
       <c r="H25" s="87"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -5061,10 +5063,10 @@
       <c r="C26" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="127"/>
-      <c r="E26" s="125"/>
-      <c r="F26" s="126"/>
-      <c r="G26" s="130"/>
+      <c r="D26" s="125"/>
+      <c r="E26" s="123"/>
+      <c r="F26" s="124"/>
+      <c r="G26" s="128"/>
       <c r="H26" s="87"/>
     </row>
     <row r="27" spans="1:8" ht="374.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5103,19 +5105,19 @@
       <c r="C28" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="127" t="s">
+      <c r="D28" s="125" t="s">
         <v>224</v>
       </c>
-      <c r="E28" s="125" t="s">
+      <c r="E28" s="123" t="s">
         <v>229</v>
       </c>
-      <c r="F28" s="126" t="s">
+      <c r="F28" s="124" t="s">
         <v>178</v>
       </c>
-      <c r="G28" s="130" t="s">
+      <c r="G28" s="128" t="s">
         <v>243</v>
       </c>
-      <c r="H28" s="128" t="s">
+      <c r="H28" s="127" t="s">
         <v>242</v>
       </c>
     </row>
@@ -5129,11 +5131,11 @@
       <c r="C29" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="130"/>
-      <c r="E29" s="125"/>
-      <c r="F29" s="126"/>
-      <c r="G29" s="130"/>
-      <c r="H29" s="128"/>
+      <c r="D29" s="128"/>
+      <c r="E29" s="123"/>
+      <c r="F29" s="124"/>
+      <c r="G29" s="128"/>
+      <c r="H29" s="127"/>
     </row>
     <row r="30" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="74" t="s">
@@ -5145,11 +5147,11 @@
       <c r="C30" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="130"/>
-      <c r="E30" s="125"/>
-      <c r="F30" s="126"/>
-      <c r="G30" s="130"/>
-      <c r="H30" s="128"/>
+      <c r="D30" s="128"/>
+      <c r="E30" s="123"/>
+      <c r="F30" s="124"/>
+      <c r="G30" s="128"/>
+      <c r="H30" s="127"/>
     </row>
     <row r="31" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="80" t="s">
@@ -5161,17 +5163,17 @@
       <c r="C31" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="127" t="s">
+      <c r="D31" s="125" t="s">
         <v>179</v>
       </c>
-      <c r="E31" s="125" t="s">
+      <c r="E31" s="123" t="s">
         <v>180</v>
       </c>
-      <c r="F31" s="125" t="s">
+      <c r="F31" s="123" t="s">
         <v>181</v>
       </c>
-      <c r="G31" s="127"/>
-      <c r="H31" s="128"/>
+      <c r="G31" s="125"/>
+      <c r="H31" s="127"/>
     </row>
     <row r="32" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="80" t="s">
@@ -5183,11 +5185,11 @@
       <c r="C32" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="127"/>
-      <c r="E32" s="125"/>
-      <c r="F32" s="125"/>
-      <c r="G32" s="127"/>
-      <c r="H32" s="128"/>
+      <c r="D32" s="125"/>
+      <c r="E32" s="123"/>
+      <c r="F32" s="123"/>
+      <c r="G32" s="125"/>
+      <c r="H32" s="127"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="81" t="s">
@@ -5247,19 +5249,19 @@
       <c r="C35" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="127" t="s">
+      <c r="D35" s="125" t="s">
         <v>231</v>
       </c>
-      <c r="E35" s="125" t="s">
+      <c r="E35" s="123" t="s">
         <v>188</v>
       </c>
-      <c r="F35" s="125" t="s">
+      <c r="F35" s="123" t="s">
         <v>144</v>
       </c>
-      <c r="G35" s="127" t="s">
+      <c r="G35" s="125" t="s">
         <v>237</v>
       </c>
-      <c r="H35" s="129" t="s">
+      <c r="H35" s="126" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5273,11 +5275,11 @@
       <c r="C36" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D36" s="127"/>
-      <c r="E36" s="125"/>
-      <c r="F36" s="125"/>
-      <c r="G36" s="127"/>
-      <c r="H36" s="129"/>
+      <c r="D36" s="125"/>
+      <c r="E36" s="123"/>
+      <c r="F36" s="123"/>
+      <c r="G36" s="125"/>
+      <c r="H36" s="126"/>
     </row>
     <row r="37" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A37" s="78" t="s">
@@ -5289,11 +5291,11 @@
       <c r="C37" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D37" s="127"/>
-      <c r="E37" s="125"/>
-      <c r="F37" s="125"/>
-      <c r="G37" s="127"/>
-      <c r="H37" s="129"/>
+      <c r="D37" s="125"/>
+      <c r="E37" s="123"/>
+      <c r="F37" s="123"/>
+      <c r="G37" s="125"/>
+      <c r="H37" s="126"/>
     </row>
     <row r="38" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="78" t="s">
@@ -5305,19 +5307,19 @@
       <c r="C38" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D38" s="127" t="s">
+      <c r="D38" s="125" t="s">
         <v>226</v>
       </c>
-      <c r="E38" s="125" t="s">
+      <c r="E38" s="123" t="s">
         <v>190</v>
       </c>
-      <c r="F38" s="125" t="s">
+      <c r="F38" s="123" t="s">
         <v>244</v>
       </c>
-      <c r="G38" s="127" t="s">
+      <c r="G38" s="125" t="s">
         <v>237</v>
       </c>
-      <c r="H38" s="128" t="s">
+      <c r="H38" s="127" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5331,11 +5333,11 @@
       <c r="C39" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="127"/>
-      <c r="E39" s="125"/>
-      <c r="F39" s="125"/>
-      <c r="G39" s="127"/>
-      <c r="H39" s="128"/>
+      <c r="D39" s="125"/>
+      <c r="E39" s="123"/>
+      <c r="F39" s="123"/>
+      <c r="G39" s="125"/>
+      <c r="H39" s="127"/>
     </row>
     <row r="40" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A40" s="78" t="s">
@@ -5347,11 +5349,11 @@
       <c r="C40" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D40" s="127"/>
-      <c r="E40" s="125"/>
-      <c r="F40" s="125"/>
-      <c r="G40" s="127"/>
-      <c r="H40" s="128"/>
+      <c r="D40" s="125"/>
+      <c r="E40" s="123"/>
+      <c r="F40" s="123"/>
+      <c r="G40" s="125"/>
+      <c r="H40" s="127"/>
     </row>
     <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A41" s="78" t="s">
@@ -5363,11 +5365,11 @@
       <c r="C41" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="127"/>
-      <c r="E41" s="125"/>
-      <c r="F41" s="125"/>
-      <c r="G41" s="127"/>
-      <c r="H41" s="128"/>
+      <c r="D41" s="125"/>
+      <c r="E41" s="123"/>
+      <c r="F41" s="123"/>
+      <c r="G41" s="125"/>
+      <c r="H41" s="127"/>
     </row>
     <row r="42" spans="1:8" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="78" t="s">
@@ -5379,11 +5381,11 @@
       <c r="C42" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="127"/>
-      <c r="E42" s="125"/>
-      <c r="F42" s="125"/>
-      <c r="G42" s="127"/>
-      <c r="H42" s="128"/>
+      <c r="D42" s="125"/>
+      <c r="E42" s="123"/>
+      <c r="F42" s="123"/>
+      <c r="G42" s="125"/>
+      <c r="H42" s="127"/>
     </row>
     <row r="43" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A43" s="78" t="s">
@@ -5395,11 +5397,11 @@
       <c r="C43" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="127"/>
-      <c r="E43" s="125"/>
-      <c r="F43" s="125"/>
-      <c r="G43" s="127"/>
-      <c r="H43" s="128"/>
+      <c r="D43" s="125"/>
+      <c r="E43" s="123"/>
+      <c r="F43" s="123"/>
+      <c r="G43" s="125"/>
+      <c r="H43" s="127"/>
     </row>
     <row r="44" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A44" s="78" t="s">
@@ -5411,11 +5413,11 @@
       <c r="C44" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D44" s="127"/>
-      <c r="E44" s="125"/>
-      <c r="F44" s="125"/>
-      <c r="G44" s="127"/>
-      <c r="H44" s="128"/>
+      <c r="D44" s="125"/>
+      <c r="E44" s="123"/>
+      <c r="F44" s="123"/>
+      <c r="G44" s="125"/>
+      <c r="H44" s="127"/>
     </row>
     <row r="45" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A45" s="78" t="s">
@@ -5427,11 +5429,11 @@
       <c r="C45" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="127"/>
-      <c r="E45" s="125"/>
-      <c r="F45" s="125"/>
-      <c r="G45" s="127"/>
-      <c r="H45" s="128"/>
+      <c r="D45" s="125"/>
+      <c r="E45" s="123"/>
+      <c r="F45" s="123"/>
+      <c r="G45" s="125"/>
+      <c r="H45" s="127"/>
     </row>
     <row r="46" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A46" s="78" t="s">
@@ -5443,11 +5445,11 @@
       <c r="C46" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D46" s="127"/>
-      <c r="E46" s="125"/>
-      <c r="F46" s="125"/>
-      <c r="G46" s="127"/>
-      <c r="H46" s="128"/>
+      <c r="D46" s="125"/>
+      <c r="E46" s="123"/>
+      <c r="F46" s="123"/>
+      <c r="G46" s="125"/>
+      <c r="H46" s="127"/>
     </row>
     <row r="47" spans="1:8" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="78" t="s">
@@ -5459,11 +5461,11 @@
       <c r="C47" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D47" s="127"/>
-      <c r="E47" s="125"/>
-      <c r="F47" s="125"/>
-      <c r="G47" s="127"/>
-      <c r="H47" s="128"/>
+      <c r="D47" s="125"/>
+      <c r="E47" s="123"/>
+      <c r="F47" s="123"/>
+      <c r="G47" s="125"/>
+      <c r="H47" s="127"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="78" t="s">
@@ -5475,19 +5477,19 @@
       <c r="C48" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D48" s="127" t="s">
+      <c r="D48" s="125" t="s">
         <v>227</v>
       </c>
-      <c r="E48" s="125" t="s">
+      <c r="E48" s="123" t="s">
         <v>192</v>
       </c>
-      <c r="F48" s="125" t="s">
+      <c r="F48" s="123" t="s">
         <v>144</v>
       </c>
-      <c r="G48" s="127" t="s">
+      <c r="G48" s="125" t="s">
         <v>237</v>
       </c>
-      <c r="H48" s="128" t="s">
+      <c r="H48" s="127" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5501,11 +5503,11 @@
       <c r="C49" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D49" s="127"/>
-      <c r="E49" s="125"/>
-      <c r="F49" s="125"/>
-      <c r="G49" s="127"/>
-      <c r="H49" s="128"/>
+      <c r="D49" s="125"/>
+      <c r="E49" s="123"/>
+      <c r="F49" s="123"/>
+      <c r="G49" s="125"/>
+      <c r="H49" s="127"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="78" t="s">
@@ -5517,11 +5519,11 @@
       <c r="C50" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D50" s="127"/>
-      <c r="E50" s="125"/>
-      <c r="F50" s="125"/>
-      <c r="G50" s="127"/>
-      <c r="H50" s="128"/>
+      <c r="D50" s="125"/>
+      <c r="E50" s="123"/>
+      <c r="F50" s="123"/>
+      <c r="G50" s="125"/>
+      <c r="H50" s="127"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="78" t="s">
@@ -5533,25 +5535,29 @@
       <c r="C51" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D51" s="127"/>
-      <c r="E51" s="125"/>
-      <c r="F51" s="125"/>
-      <c r="G51" s="127"/>
-      <c r="H51" s="128"/>
+      <c r="D51" s="125"/>
+      <c r="E51" s="123"/>
+      <c r="F51" s="123"/>
+      <c r="G51" s="125"/>
+      <c r="H51" s="127"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E18"/>
-    <mergeCell ref="F4:F18"/>
-    <mergeCell ref="G4:G18"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="F48:F51"/>
+    <mergeCell ref="G48:G51"/>
+    <mergeCell ref="H48:H51"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="D38:D47"/>
+    <mergeCell ref="E38:E47"/>
+    <mergeCell ref="F38:F47"/>
+    <mergeCell ref="G38:G47"/>
+    <mergeCell ref="H38:H47"/>
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="H28:H30"/>
     <mergeCell ref="D31:D32"/>
@@ -5568,21 +5574,17 @@
     <mergeCell ref="F21:F26"/>
     <mergeCell ref="G21:G26"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D38:D47"/>
-    <mergeCell ref="E38:E47"/>
-    <mergeCell ref="F38:F47"/>
-    <mergeCell ref="G38:G47"/>
-    <mergeCell ref="H38:H47"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="F48:F51"/>
-    <mergeCell ref="G48:G51"/>
-    <mergeCell ref="H48:H51"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E18"/>
+    <mergeCell ref="F4:F18"/>
+    <mergeCell ref="G4:G18"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C33" location="_ftn2" display="_ftn2" xr:uid="{E50DF5A1-13E6-4004-9692-0F820274B734}"/>
@@ -5596,13 +5598,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE037D9D-4E45-4C5B-8392-AE943DD18A55}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.5703125" style="88" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" style="88" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" style="88" customWidth="1"/>
     <col min="3" max="3" width="57.140625" style="92" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" style="88" customWidth="1"/>
     <col min="5" max="16384" width="29.7109375" style="88"/>
@@ -5626,11 +5629,11 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="131" t="s">
+      <c r="A2" s="129" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="109" t="s">
-        <v>330</v>
+      <c r="B2" s="106" t="s">
+        <v>319</v>
       </c>
       <c r="C2" s="94" t="s">
         <v>273</v>
@@ -5646,9 +5649,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="132"/>
-      <c r="B3" s="110" t="s">
-        <v>331</v>
+      <c r="A3" s="130"/>
+      <c r="B3" s="107" t="s">
+        <v>320</v>
       </c>
       <c r="C3" s="94" t="s">
         <v>249</v>
@@ -5661,9 +5664,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="133"/>
-      <c r="B4" s="110" t="s">
-        <v>332</v>
+      <c r="A4" s="131"/>
+      <c r="B4" s="107" t="s">
+        <v>321</v>
       </c>
       <c r="C4" s="94" t="s">
         <v>288</v>
@@ -5677,19 +5680,19 @@
       <c r="F4" s="100"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="137" t="s">
+      <c r="A5" s="129" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="110" t="s">
-        <v>333</v>
-      </c>
-      <c r="C5" s="106" t="s">
+      <c r="B5" s="107" t="s">
+        <v>322</v>
+      </c>
+      <c r="C5" s="94" t="s">
         <v>250</v>
       </c>
-      <c r="D5" s="107" t="s">
+      <c r="D5" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="108" t="s">
+      <c r="E5" s="96" t="s">
         <v>283</v>
       </c>
       <c r="F5" s="102" t="s">
@@ -5697,17 +5700,17 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="138"/>
-      <c r="B6" s="110" t="s">
-        <v>334</v>
-      </c>
-      <c r="C6" s="106" t="s">
+      <c r="A6" s="131"/>
+      <c r="B6" s="107" t="s">
+        <v>323</v>
+      </c>
+      <c r="C6" s="94" t="s">
         <v>251</v>
       </c>
-      <c r="D6" s="107" t="s">
+      <c r="D6" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="108" t="s">
+      <c r="E6" s="96" t="s">
         <v>283</v>
       </c>
       <c r="F6" s="102" t="s">
@@ -5715,10 +5718,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="134" t="s">
+      <c r="A7" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="110" t="s">
+      <c r="B7" s="108" t="s">
         <v>335</v>
       </c>
       <c r="C7" s="94" t="s">
@@ -5733,8 +5736,8 @@
       <c r="F7" s="101"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="135"/>
-      <c r="B8" s="110" t="s">
+      <c r="A8" s="133"/>
+      <c r="B8" s="108" t="s">
         <v>336</v>
       </c>
       <c r="C8" s="94" t="s">
@@ -5748,8 +5751,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="135"/>
-      <c r="B9" s="110" t="s">
+      <c r="A9" s="133"/>
+      <c r="B9" s="108" t="s">
         <v>337</v>
       </c>
       <c r="C9" s="94" t="s">
@@ -5763,39 +5766,39 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="135"/>
-      <c r="B10" s="110" t="s">
+      <c r="A10" s="133"/>
+      <c r="B10" s="108" t="s">
         <v>338</v>
       </c>
-      <c r="C10" s="103" t="s">
+      <c r="C10" s="94" t="s">
         <v>289</v>
       </c>
-      <c r="D10" s="104" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="105" t="s">
+      <c r="D10" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="96" t="s">
         <v>283</v>
       </c>
       <c r="F10" s="100"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="135"/>
-      <c r="B11" s="110" t="s">
+      <c r="A11" s="133"/>
+      <c r="B11" s="142" t="s">
         <v>292</v>
       </c>
-      <c r="C11" s="103" t="s">
+      <c r="C11" s="139" t="s">
         <v>255</v>
       </c>
-      <c r="D11" s="104" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="105" t="s">
+      <c r="D11" s="140" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="141" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.25">
-      <c r="A12" s="135"/>
-      <c r="B12" s="110" t="s">
+      <c r="A12" s="133"/>
+      <c r="B12" s="107" t="s">
         <v>293</v>
       </c>
       <c r="C12" s="103" t="s">
@@ -5809,8 +5812,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="135"/>
-      <c r="B13" s="110" t="s">
+      <c r="A13" s="133"/>
+      <c r="B13" s="107" t="s">
         <v>294</v>
       </c>
       <c r="C13" s="90" t="s">
@@ -5825,8 +5828,8 @@
       <c r="F13" s="100"/>
     </row>
     <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="135"/>
-      <c r="B14" s="110" t="s">
+      <c r="A14" s="133"/>
+      <c r="B14" s="107" t="s">
         <v>295</v>
       </c>
       <c r="C14" s="90" t="s">
@@ -5840,8 +5843,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="135"/>
-      <c r="B15" s="110" t="s">
+      <c r="A15" s="133"/>
+      <c r="B15" s="107" t="s">
         <v>296</v>
       </c>
       <c r="C15" s="91" t="s">
@@ -5855,8 +5858,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="135"/>
-      <c r="B16" s="110" t="s">
+      <c r="A16" s="133"/>
+      <c r="B16" s="107" t="s">
         <v>297</v>
       </c>
       <c r="C16" s="90" t="s">
@@ -5870,8 +5873,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="135"/>
-      <c r="B17" s="110" t="s">
+      <c r="A17" s="133"/>
+      <c r="B17" s="107" t="s">
         <v>298</v>
       </c>
       <c r="C17" s="90" t="s">
@@ -5885,8 +5888,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="135"/>
-      <c r="B18" s="110" t="s">
+      <c r="A18" s="133"/>
+      <c r="B18" s="107" t="s">
         <v>299</v>
       </c>
       <c r="C18" s="90" t="s">
@@ -5900,8 +5903,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A19" s="135"/>
-      <c r="B19" s="110" t="s">
+      <c r="A19" s="133"/>
+      <c r="B19" s="107" t="s">
         <v>300</v>
       </c>
       <c r="C19" s="90" t="s">
@@ -5915,8 +5918,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A20" s="135"/>
-      <c r="B20" s="110" t="s">
+      <c r="A20" s="133"/>
+      <c r="B20" s="107" t="s">
         <v>301</v>
       </c>
       <c r="C20" s="90" t="s">
@@ -5930,8 +5933,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A21" s="135"/>
-      <c r="B21" s="110" t="s">
+      <c r="A21" s="133"/>
+      <c r="B21" s="107" t="s">
         <v>302</v>
       </c>
       <c r="C21" s="90" t="s">
@@ -5945,8 +5948,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="135"/>
-      <c r="B22" s="110" t="s">
+      <c r="A22" s="133"/>
+      <c r="B22" s="107" t="s">
         <v>303</v>
       </c>
       <c r="C22" s="90" t="s">
@@ -5960,8 +5963,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="135"/>
-      <c r="B23" s="110" t="s">
+      <c r="A23" s="133"/>
+      <c r="B23" s="107" t="s">
         <v>304</v>
       </c>
       <c r="C23" s="90" t="s">
@@ -5975,8 +5978,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="135"/>
-      <c r="B24" s="110" t="s">
+      <c r="A24" s="133"/>
+      <c r="B24" s="107" t="s">
         <v>305</v>
       </c>
       <c r="C24" s="90" t="s">
@@ -5990,8 +5993,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="135"/>
-      <c r="B25" s="110" t="s">
+      <c r="A25" s="133"/>
+      <c r="B25" s="107" t="s">
         <v>306</v>
       </c>
       <c r="C25" s="90" t="s">
@@ -6005,8 +6008,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="135"/>
-      <c r="B26" s="110" t="s">
+      <c r="A26" s="133"/>
+      <c r="B26" s="107" t="s">
         <v>307</v>
       </c>
       <c r="C26" s="90" t="s">
@@ -6020,8 +6023,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="135"/>
-      <c r="B27" s="110" t="s">
+      <c r="A27" s="133"/>
+      <c r="B27" s="107" t="s">
         <v>308</v>
       </c>
       <c r="C27" s="90" t="s">
@@ -6035,8 +6038,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="136"/>
-      <c r="B28" s="110" t="s">
+      <c r="A28" s="134"/>
+      <c r="B28" s="107" t="s">
         <v>309</v>
       </c>
       <c r="C28" s="90" t="s">
@@ -6050,10 +6053,10 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="134" t="s">
+      <c r="A29" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="110" t="s">
+      <c r="B29" s="107" t="s">
         <v>310</v>
       </c>
       <c r="C29" s="90" t="s">
@@ -6067,8 +6070,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="135"/>
-      <c r="B30" s="110" t="s">
+      <c r="A30" s="133"/>
+      <c r="B30" s="107" t="s">
         <v>311</v>
       </c>
       <c r="C30" s="90" t="s">
@@ -6082,8 +6085,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="135"/>
-      <c r="B31" s="110" t="s">
+      <c r="A31" s="133"/>
+      <c r="B31" s="107" t="s">
         <v>312</v>
       </c>
       <c r="C31" s="90" t="s">
@@ -6097,8 +6100,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="135"/>
-      <c r="B32" s="110" t="s">
+      <c r="A32" s="133"/>
+      <c r="B32" s="107" t="s">
         <v>313</v>
       </c>
       <c r="C32" s="90" t="s">
@@ -6112,8 +6115,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="135"/>
-      <c r="B33" s="110" t="s">
+      <c r="A33" s="133"/>
+      <c r="B33" s="107" t="s">
         <v>314</v>
       </c>
       <c r="C33" s="90" t="s">
@@ -6127,8 +6130,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="136"/>
-      <c r="B34" s="110" t="s">
+      <c r="A34" s="134"/>
+      <c r="B34" s="107" t="s">
         <v>315</v>
       </c>
       <c r="C34" s="90" t="s">
@@ -6142,11 +6145,11 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="131" t="s">
+      <c r="A35" s="129" t="s">
         <v>287</v>
       </c>
-      <c r="B35" s="110" t="s">
-        <v>316</v>
+      <c r="B35" s="107" t="s">
+        <v>324</v>
       </c>
       <c r="C35" s="97" t="s">
         <v>265</v>
@@ -6159,9 +6162,9 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="133"/>
-      <c r="B36" s="110" t="s">
-        <v>317</v>
+      <c r="A36" s="131"/>
+      <c r="B36" s="107" t="s">
+        <v>325</v>
       </c>
       <c r="C36" s="97" t="s">
         <v>266</v>
@@ -6174,11 +6177,11 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="131" t="s">
+      <c r="A37" s="129" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="110" t="s">
-        <v>318</v>
+      <c r="B37" s="107" t="s">
+        <v>326</v>
       </c>
       <c r="C37" s="97" t="s">
         <v>267</v>
@@ -6191,9 +6194,9 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="133"/>
-      <c r="B38" s="110" t="s">
-        <v>319</v>
+      <c r="A38" s="131"/>
+      <c r="B38" s="107" t="s">
+        <v>327</v>
       </c>
       <c r="C38" s="97" t="s">
         <v>268</v>
@@ -6206,11 +6209,11 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="131" t="s">
+      <c r="A39" s="129" t="s">
         <v>199</v>
       </c>
-      <c r="B39" s="110" t="s">
-        <v>320</v>
+      <c r="B39" s="107" t="s">
+        <v>328</v>
       </c>
       <c r="C39" s="97" t="s">
         <v>269</v>
@@ -6223,9 +6226,9 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="132"/>
-      <c r="B40" s="110" t="s">
-        <v>321</v>
+      <c r="A40" s="130"/>
+      <c r="B40" s="107" t="s">
+        <v>329</v>
       </c>
       <c r="C40" s="97" t="s">
         <v>270</v>
@@ -6238,9 +6241,9 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="132"/>
-      <c r="B41" s="110" t="s">
-        <v>322</v>
+      <c r="A41" s="130"/>
+      <c r="B41" s="107" t="s">
+        <v>330</v>
       </c>
       <c r="C41" s="97" t="s">
         <v>271</v>
@@ -6252,10 +6255,10 @@
         <v>283</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="133"/>
-      <c r="B42" s="110" t="s">
-        <v>323</v>
+    <row r="42" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="131"/>
+      <c r="B42" s="107" t="s">
+        <v>331</v>
       </c>
       <c r="C42" s="97" t="s">
         <v>245</v>
@@ -6268,34 +6271,34 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="134" t="s">
+      <c r="A43" s="132" t="s">
         <v>198</v>
       </c>
-      <c r="B43" s="110" t="s">
-        <v>324</v>
-      </c>
-      <c r="C43" s="103" t="s">
+      <c r="B43" s="142" t="s">
+        <v>316</v>
+      </c>
+      <c r="C43" s="139" t="s">
         <v>248</v>
       </c>
-      <c r="D43" s="104" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" s="105" t="s">
+      <c r="D43" s="140" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="141" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="135"/>
-      <c r="B44" s="110" t="s">
-        <v>325</v>
-      </c>
-      <c r="C44" s="106" t="s">
+    <row r="44" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="133"/>
+      <c r="B44" s="107" t="s">
+        <v>334</v>
+      </c>
+      <c r="C44" s="97" t="s">
         <v>86</v>
       </c>
-      <c r="D44" s="107" t="s">
+      <c r="D44" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="E44" s="108" t="s">
+      <c r="E44" s="99" t="s">
         <v>283</v>
       </c>
       <c r="F44" s="102" t="s">
@@ -6303,17 +6306,17 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="135"/>
-      <c r="B45" s="110" t="s">
-        <v>326</v>
-      </c>
-      <c r="C45" s="106" t="s">
+      <c r="A45" s="133"/>
+      <c r="B45" s="107" t="s">
+        <v>332</v>
+      </c>
+      <c r="C45" s="97" t="s">
         <v>87</v>
       </c>
-      <c r="D45" s="107" t="s">
+      <c r="D45" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="E45" s="108" t="s">
+      <c r="E45" s="99" t="s">
         <v>283</v>
       </c>
       <c r="F45" s="102" t="s">
@@ -6321,17 +6324,17 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="136"/>
-      <c r="B46" s="110" t="s">
-        <v>327</v>
-      </c>
-      <c r="C46" s="106" t="s">
+      <c r="A46" s="134"/>
+      <c r="B46" s="107" t="s">
+        <v>333</v>
+      </c>
+      <c r="C46" s="97" t="s">
         <v>100</v>
       </c>
-      <c r="D46" s="107" t="s">
+      <c r="D46" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="E46" s="108" t="s">
+      <c r="E46" s="99" t="s">
         <v>283</v>
       </c>
       <c r="F46" s="102" t="s">
@@ -6339,11 +6342,11 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="134" t="s">
+      <c r="A47" s="132" t="s">
         <v>151</v>
       </c>
-      <c r="B47" s="110" t="s">
-        <v>328</v>
+      <c r="B47" s="107" t="s">
+        <v>317</v>
       </c>
       <c r="C47" s="90" t="s">
         <v>209</v>
@@ -6356,9 +6359,9 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="136"/>
-      <c r="B48" s="110" t="s">
-        <v>329</v>
+      <c r="A48" s="134"/>
+      <c r="B48" s="107" t="s">
+        <v>318</v>
       </c>
       <c r="C48" s="90" t="s">
         <v>247</v>
@@ -6469,16 +6472,16 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="127" t="s">
+      <c r="D4" s="125" t="s">
         <v>215</v>
       </c>
-      <c r="E4" s="125" t="s">
+      <c r="E4" s="123" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="125" t="s">
+      <c r="F4" s="123" t="s">
         <v>158</v>
       </c>
-      <c r="G4" s="127"/>
+      <c r="G4" s="125"/>
       <c r="H4" s="87"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6491,10 +6494,10 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="127"/>
-      <c r="E5" s="125"/>
-      <c r="F5" s="125"/>
-      <c r="G5" s="127"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="125"/>
       <c r="H5" s="87"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6507,12 +6510,12 @@
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="127" t="s">
+      <c r="D6" s="125" t="s">
         <v>216</v>
       </c>
-      <c r="E6" s="125"/>
-      <c r="F6" s="125"/>
-      <c r="G6" s="127"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="125"/>
       <c r="H6" s="87"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6525,10 +6528,10 @@
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="127"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="127"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="125"/>
       <c r="H7" s="87"/>
     </row>
     <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6541,12 +6544,12 @@
       <c r="C8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="127" t="s">
+      <c r="D8" s="125" t="s">
         <v>164</v>
       </c>
-      <c r="E8" s="125"/>
-      <c r="F8" s="125"/>
-      <c r="G8" s="127"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="125"/>
       <c r="H8" s="87"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6559,10 +6562,10 @@
       <c r="C9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="127"/>
-      <c r="E9" s="125"/>
-      <c r="F9" s="125"/>
-      <c r="G9" s="127"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="125"/>
       <c r="H9" s="87"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -6575,12 +6578,12 @@
       <c r="C10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="127" t="s">
+      <c r="D10" s="125" t="s">
         <v>217</v>
       </c>
-      <c r="E10" s="125"/>
-      <c r="F10" s="125"/>
-      <c r="G10" s="127"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="125"/>
       <c r="H10" s="87"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -6593,10 +6596,10 @@
       <c r="C11" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="127"/>
-      <c r="E11" s="125"/>
-      <c r="F11" s="125"/>
-      <c r="G11" s="127"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="125"/>
       <c r="H11" s="87"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6609,10 +6612,10 @@
       <c r="C12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="127"/>
-      <c r="E12" s="125"/>
-      <c r="F12" s="125"/>
-      <c r="G12" s="127"/>
+      <c r="D12" s="125"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="125"/>
       <c r="H12" s="87"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6625,12 +6628,12 @@
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="127" t="s">
+      <c r="D13" s="125" t="s">
         <v>218</v>
       </c>
-      <c r="E13" s="125"/>
-      <c r="F13" s="125"/>
-      <c r="G13" s="127"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="125"/>
       <c r="H13" s="87"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -6643,10 +6646,10 @@
       <c r="C14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="127"/>
-      <c r="E14" s="125"/>
-      <c r="F14" s="125"/>
-      <c r="G14" s="127"/>
+      <c r="D14" s="125"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="125"/>
       <c r="H14" s="87"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6659,10 +6662,10 @@
       <c r="C15" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="127"/>
-      <c r="E15" s="125"/>
-      <c r="F15" s="125"/>
-      <c r="G15" s="127"/>
+      <c r="D15" s="125"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
+      <c r="G15" s="125"/>
       <c r="H15" s="87"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -6675,10 +6678,10 @@
       <c r="C16" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="127"/>
-      <c r="E16" s="125"/>
-      <c r="F16" s="125"/>
-      <c r="G16" s="127"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="123"/>
+      <c r="F16" s="123"/>
+      <c r="G16" s="125"/>
       <c r="H16" s="87"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -6691,10 +6694,10 @@
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="127"/>
-      <c r="E17" s="125"/>
-      <c r="F17" s="125"/>
-      <c r="G17" s="127"/>
+      <c r="D17" s="125"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="123"/>
+      <c r="G17" s="125"/>
       <c r="H17" s="87"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -6710,9 +6713,9 @@
       <c r="D18" s="83" t="s">
         <v>219</v>
       </c>
-      <c r="E18" s="125"/>
-      <c r="F18" s="125"/>
-      <c r="G18" s="127"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="123"/>
+      <c r="G18" s="125"/>
       <c r="H18" s="87"/>
     </row>
     <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -6725,19 +6728,19 @@
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="127" t="s">
+      <c r="D19" s="125" t="s">
         <v>220</v>
       </c>
-      <c r="E19" s="125" t="s">
+      <c r="E19" s="123" t="s">
         <v>197</v>
       </c>
-      <c r="F19" s="125" t="s">
+      <c r="F19" s="123" t="s">
         <v>169</v>
       </c>
-      <c r="G19" s="127" t="s">
+      <c r="G19" s="125" t="s">
         <v>235</v>
       </c>
-      <c r="H19" s="129" t="s">
+      <c r="H19" s="126" t="s">
         <v>234</v>
       </c>
     </row>
@@ -6751,11 +6754,11 @@
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="127"/>
-      <c r="E20" s="125"/>
-      <c r="F20" s="125"/>
-      <c r="G20" s="127"/>
-      <c r="H20" s="129"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="123"/>
+      <c r="G20" s="125"/>
+      <c r="H20" s="126"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
@@ -6767,16 +6770,16 @@
       <c r="C21" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="127" t="s">
+      <c r="D21" s="125" t="s">
         <v>221</v>
       </c>
-      <c r="E21" s="125" t="s">
+      <c r="E21" s="123" t="s">
         <v>172</v>
       </c>
-      <c r="F21" s="126" t="s">
+      <c r="F21" s="124" t="s">
         <v>173</v>
       </c>
-      <c r="G21" s="130"/>
+      <c r="G21" s="128"/>
       <c r="H21" s="87"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -6789,10 +6792,10 @@
       <c r="C22" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="127"/>
-      <c r="E22" s="125"/>
-      <c r="F22" s="126"/>
-      <c r="G22" s="130"/>
+      <c r="D22" s="125"/>
+      <c r="E22" s="123"/>
+      <c r="F22" s="124"/>
+      <c r="G22" s="128"/>
       <c r="H22" s="87"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -6805,10 +6808,10 @@
       <c r="C23" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="127"/>
-      <c r="E23" s="125"/>
-      <c r="F23" s="126"/>
-      <c r="G23" s="130"/>
+      <c r="D23" s="125"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="124"/>
+      <c r="G23" s="128"/>
       <c r="H23" s="87"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -6821,10 +6824,10 @@
       <c r="C24" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="127"/>
-      <c r="E24" s="125"/>
-      <c r="F24" s="126"/>
-      <c r="G24" s="130"/>
+      <c r="D24" s="125"/>
+      <c r="E24" s="123"/>
+      <c r="F24" s="124"/>
+      <c r="G24" s="128"/>
       <c r="H24" s="87"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -6837,10 +6840,10 @@
       <c r="C25" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="127"/>
-      <c r="E25" s="125"/>
-      <c r="F25" s="126"/>
-      <c r="G25" s="130"/>
+      <c r="D25" s="125"/>
+      <c r="E25" s="123"/>
+      <c r="F25" s="124"/>
+      <c r="G25" s="128"/>
       <c r="H25" s="87"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -6853,10 +6856,10 @@
       <c r="C26" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="127"/>
-      <c r="E26" s="125"/>
-      <c r="F26" s="126"/>
-      <c r="G26" s="130"/>
+      <c r="D26" s="125"/>
+      <c r="E26" s="123"/>
+      <c r="F26" s="124"/>
+      <c r="G26" s="128"/>
       <c r="H26" s="87"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -6869,16 +6872,16 @@
       <c r="C27" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="127" t="s">
+      <c r="D27" s="125" t="s">
         <v>222</v>
       </c>
-      <c r="E27" s="125" t="s">
+      <c r="E27" s="123" t="s">
         <v>175</v>
       </c>
-      <c r="F27" s="125" t="s">
+      <c r="F27" s="123" t="s">
         <v>158</v>
       </c>
-      <c r="G27" s="127"/>
+      <c r="G27" s="125"/>
       <c r="H27" s="87"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -6891,10 +6894,10 @@
       <c r="C28" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="127"/>
-      <c r="E28" s="125"/>
-      <c r="F28" s="125"/>
-      <c r="G28" s="127"/>
+      <c r="D28" s="125"/>
+      <c r="E28" s="123"/>
+      <c r="F28" s="123"/>
+      <c r="G28" s="125"/>
       <c r="H28" s="87"/>
     </row>
     <row r="29" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -6907,10 +6910,10 @@
       <c r="C29" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D29" s="127"/>
-      <c r="E29" s="125"/>
-      <c r="F29" s="125"/>
-      <c r="G29" s="127"/>
+      <c r="D29" s="125"/>
+      <c r="E29" s="123"/>
+      <c r="F29" s="123"/>
+      <c r="G29" s="125"/>
       <c r="H29" s="87"/>
     </row>
     <row r="30" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -6923,10 +6926,10 @@
       <c r="C30" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="127"/>
-      <c r="E30" s="125"/>
-      <c r="F30" s="125"/>
-      <c r="G30" s="127"/>
+      <c r="D30" s="125"/>
+      <c r="E30" s="123"/>
+      <c r="F30" s="123"/>
+      <c r="G30" s="125"/>
       <c r="H30" s="87"/>
     </row>
     <row r="31" spans="1:8" ht="374.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6965,19 +6968,19 @@
       <c r="C32" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="127" t="s">
+      <c r="D32" s="125" t="s">
         <v>224</v>
       </c>
-      <c r="E32" s="125" t="s">
+      <c r="E32" s="123" t="s">
         <v>229</v>
       </c>
-      <c r="F32" s="126" t="s">
+      <c r="F32" s="124" t="s">
         <v>178</v>
       </c>
-      <c r="G32" s="130" t="s">
+      <c r="G32" s="128" t="s">
         <v>243</v>
       </c>
-      <c r="H32" s="128" t="s">
+      <c r="H32" s="127" t="s">
         <v>242</v>
       </c>
     </row>
@@ -6991,11 +6994,11 @@
       <c r="C33" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="130"/>
-      <c r="E33" s="125"/>
-      <c r="F33" s="126"/>
-      <c r="G33" s="130"/>
-      <c r="H33" s="128"/>
+      <c r="D33" s="128"/>
+      <c r="E33" s="123"/>
+      <c r="F33" s="124"/>
+      <c r="G33" s="128"/>
+      <c r="H33" s="127"/>
     </row>
     <row r="34" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="74" t="s">
@@ -7007,11 +7010,11 @@
       <c r="C34" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="130"/>
-      <c r="E34" s="125"/>
-      <c r="F34" s="126"/>
-      <c r="G34" s="130"/>
-      <c r="H34" s="128"/>
+      <c r="D34" s="128"/>
+      <c r="E34" s="123"/>
+      <c r="F34" s="124"/>
+      <c r="G34" s="128"/>
+      <c r="H34" s="127"/>
     </row>
     <row r="35" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="80" t="s">
@@ -7023,17 +7026,17 @@
       <c r="C35" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="127" t="s">
+      <c r="D35" s="125" t="s">
         <v>179</v>
       </c>
-      <c r="E35" s="125" t="s">
+      <c r="E35" s="123" t="s">
         <v>180</v>
       </c>
-      <c r="F35" s="125" t="s">
+      <c r="F35" s="123" t="s">
         <v>181</v>
       </c>
-      <c r="G35" s="127"/>
-      <c r="H35" s="128"/>
+      <c r="G35" s="125"/>
+      <c r="H35" s="127"/>
     </row>
     <row r="36" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="80" t="s">
@@ -7045,11 +7048,11 @@
       <c r="C36" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="127"/>
-      <c r="E36" s="125"/>
-      <c r="F36" s="125"/>
-      <c r="G36" s="127"/>
-      <c r="H36" s="128"/>
+      <c r="D36" s="125"/>
+      <c r="E36" s="123"/>
+      <c r="F36" s="123"/>
+      <c r="G36" s="125"/>
+      <c r="H36" s="127"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="81" t="s">
@@ -7109,19 +7112,19 @@
       <c r="C39" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D39" s="127" t="s">
+      <c r="D39" s="125" t="s">
         <v>231</v>
       </c>
-      <c r="E39" s="125" t="s">
+      <c r="E39" s="123" t="s">
         <v>188</v>
       </c>
-      <c r="F39" s="125" t="s">
+      <c r="F39" s="123" t="s">
         <v>144</v>
       </c>
-      <c r="G39" s="127" t="s">
+      <c r="G39" s="125" t="s">
         <v>237</v>
       </c>
-      <c r="H39" s="129" t="s">
+      <c r="H39" s="126" t="s">
         <v>236</v>
       </c>
     </row>
@@ -7135,11 +7138,11 @@
       <c r="C40" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="127"/>
-      <c r="E40" s="125"/>
-      <c r="F40" s="125"/>
-      <c r="G40" s="127"/>
-      <c r="H40" s="129"/>
+      <c r="D40" s="125"/>
+      <c r="E40" s="123"/>
+      <c r="F40" s="123"/>
+      <c r="G40" s="125"/>
+      <c r="H40" s="126"/>
     </row>
     <row r="41" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A41" s="78" t="s">
@@ -7151,11 +7154,11 @@
       <c r="C41" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="127"/>
-      <c r="E41" s="125"/>
-      <c r="F41" s="125"/>
-      <c r="G41" s="127"/>
-      <c r="H41" s="129"/>
+      <c r="D41" s="125"/>
+      <c r="E41" s="123"/>
+      <c r="F41" s="123"/>
+      <c r="G41" s="125"/>
+      <c r="H41" s="126"/>
     </row>
     <row r="42" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="78" t="s">
@@ -7167,19 +7170,19 @@
       <c r="C42" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="127" t="s">
+      <c r="D42" s="125" t="s">
         <v>226</v>
       </c>
-      <c r="E42" s="125" t="s">
+      <c r="E42" s="123" t="s">
         <v>190</v>
       </c>
-      <c r="F42" s="125" t="s">
+      <c r="F42" s="123" t="s">
         <v>244</v>
       </c>
-      <c r="G42" s="127" t="s">
+      <c r="G42" s="125" t="s">
         <v>237</v>
       </c>
-      <c r="H42" s="128" t="s">
+      <c r="H42" s="127" t="s">
         <v>236</v>
       </c>
     </row>
@@ -7193,11 +7196,11 @@
       <c r="C43" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="127"/>
-      <c r="E43" s="125"/>
-      <c r="F43" s="125"/>
-      <c r="G43" s="127"/>
-      <c r="H43" s="128"/>
+      <c r="D43" s="125"/>
+      <c r="E43" s="123"/>
+      <c r="F43" s="123"/>
+      <c r="G43" s="125"/>
+      <c r="H43" s="127"/>
     </row>
     <row r="44" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A44" s="78" t="s">
@@ -7209,11 +7212,11 @@
       <c r="C44" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D44" s="127"/>
-      <c r="E44" s="125"/>
-      <c r="F44" s="125"/>
-      <c r="G44" s="127"/>
-      <c r="H44" s="128"/>
+      <c r="D44" s="125"/>
+      <c r="E44" s="123"/>
+      <c r="F44" s="123"/>
+      <c r="G44" s="125"/>
+      <c r="H44" s="127"/>
     </row>
     <row r="45" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A45" s="78" t="s">
@@ -7225,11 +7228,11 @@
       <c r="C45" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="127"/>
-      <c r="E45" s="125"/>
-      <c r="F45" s="125"/>
-      <c r="G45" s="127"/>
-      <c r="H45" s="128"/>
+      <c r="D45" s="125"/>
+      <c r="E45" s="123"/>
+      <c r="F45" s="123"/>
+      <c r="G45" s="125"/>
+      <c r="H45" s="127"/>
     </row>
     <row r="46" spans="1:8" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="78" t="s">
@@ -7241,11 +7244,11 @@
       <c r="C46" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D46" s="127"/>
-      <c r="E46" s="125"/>
-      <c r="F46" s="125"/>
-      <c r="G46" s="127"/>
-      <c r="H46" s="128"/>
+      <c r="D46" s="125"/>
+      <c r="E46" s="123"/>
+      <c r="F46" s="123"/>
+      <c r="G46" s="125"/>
+      <c r="H46" s="127"/>
     </row>
     <row r="47" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A47" s="78" t="s">
@@ -7257,11 +7260,11 @@
       <c r="C47" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D47" s="127"/>
-      <c r="E47" s="125"/>
-      <c r="F47" s="125"/>
-      <c r="G47" s="127"/>
-      <c r="H47" s="128"/>
+      <c r="D47" s="125"/>
+      <c r="E47" s="123"/>
+      <c r="F47" s="123"/>
+      <c r="G47" s="125"/>
+      <c r="H47" s="127"/>
     </row>
     <row r="48" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A48" s="78" t="s">
@@ -7273,11 +7276,11 @@
       <c r="C48" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D48" s="127"/>
-      <c r="E48" s="125"/>
-      <c r="F48" s="125"/>
-      <c r="G48" s="127"/>
-      <c r="H48" s="128"/>
+      <c r="D48" s="125"/>
+      <c r="E48" s="123"/>
+      <c r="F48" s="123"/>
+      <c r="G48" s="125"/>
+      <c r="H48" s="127"/>
     </row>
     <row r="49" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" s="78" t="s">
@@ -7289,11 +7292,11 @@
       <c r="C49" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D49" s="127"/>
-      <c r="E49" s="125"/>
-      <c r="F49" s="125"/>
-      <c r="G49" s="127"/>
-      <c r="H49" s="128"/>
+      <c r="D49" s="125"/>
+      <c r="E49" s="123"/>
+      <c r="F49" s="123"/>
+      <c r="G49" s="125"/>
+      <c r="H49" s="127"/>
     </row>
     <row r="50" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A50" s="78" t="s">
@@ -7305,11 +7308,11 @@
       <c r="C50" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D50" s="127"/>
-      <c r="E50" s="125"/>
-      <c r="F50" s="125"/>
-      <c r="G50" s="127"/>
-      <c r="H50" s="128"/>
+      <c r="D50" s="125"/>
+      <c r="E50" s="123"/>
+      <c r="F50" s="123"/>
+      <c r="G50" s="125"/>
+      <c r="H50" s="127"/>
     </row>
     <row r="51" spans="1:8" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="78" t="s">
@@ -7321,11 +7324,11 @@
       <c r="C51" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D51" s="127"/>
-      <c r="E51" s="125"/>
-      <c r="F51" s="125"/>
-      <c r="G51" s="127"/>
-      <c r="H51" s="128"/>
+      <c r="D51" s="125"/>
+      <c r="E51" s="123"/>
+      <c r="F51" s="123"/>
+      <c r="G51" s="125"/>
+      <c r="H51" s="127"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="78" t="s">
@@ -7337,19 +7340,19 @@
       <c r="C52" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D52" s="127" t="s">
+      <c r="D52" s="125" t="s">
         <v>227</v>
       </c>
-      <c r="E52" s="125" t="s">
+      <c r="E52" s="123" t="s">
         <v>192</v>
       </c>
-      <c r="F52" s="125" t="s">
+      <c r="F52" s="123" t="s">
         <v>144</v>
       </c>
-      <c r="G52" s="127" t="s">
+      <c r="G52" s="125" t="s">
         <v>237</v>
       </c>
-      <c r="H52" s="128" t="s">
+      <c r="H52" s="127" t="s">
         <v>236</v>
       </c>
     </row>
@@ -7363,11 +7366,11 @@
       <c r="C53" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D53" s="127"/>
-      <c r="E53" s="125"/>
-      <c r="F53" s="125"/>
-      <c r="G53" s="127"/>
-      <c r="H53" s="128"/>
+      <c r="D53" s="125"/>
+      <c r="E53" s="123"/>
+      <c r="F53" s="123"/>
+      <c r="G53" s="125"/>
+      <c r="H53" s="127"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="78" t="s">
@@ -7379,11 +7382,11 @@
       <c r="C54" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="127"/>
-      <c r="E54" s="125"/>
-      <c r="F54" s="125"/>
-      <c r="G54" s="127"/>
-      <c r="H54" s="128"/>
+      <c r="D54" s="125"/>
+      <c r="E54" s="123"/>
+      <c r="F54" s="123"/>
+      <c r="G54" s="125"/>
+      <c r="H54" s="127"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="78" t="s">
@@ -7395,50 +7398,14 @@
       <c r="C55" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D55" s="127"/>
-      <c r="E55" s="125"/>
-      <c r="F55" s="125"/>
-      <c r="G55" s="127"/>
-      <c r="H55" s="128"/>
+      <c r="D55" s="125"/>
+      <c r="E55" s="123"/>
+      <c r="F55" s="123"/>
+      <c r="G55" s="125"/>
+      <c r="H55" s="127"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E18"/>
-    <mergeCell ref="F4:F18"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="D21:D26"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="F21:F26"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="D42:D51"/>
-    <mergeCell ref="E42:E51"/>
-    <mergeCell ref="F42:F51"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="F52:F55"/>
-    <mergeCell ref="G4:G18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G21:G26"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G32:G34"/>
     <mergeCell ref="G39:G41"/>
     <mergeCell ref="G42:G51"/>
     <mergeCell ref="G52:G55"/>
@@ -7449,6 +7416,42 @@
     <mergeCell ref="H35:H36"/>
     <mergeCell ref="H42:H51"/>
     <mergeCell ref="G35:G36"/>
+    <mergeCell ref="G4:G18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G21:G26"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="D42:D51"/>
+    <mergeCell ref="E42:E51"/>
+    <mergeCell ref="F42:F51"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="F52:F55"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="D21:D26"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="F21:F26"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E18"/>
+    <mergeCell ref="F4:F18"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C37" location="_ftn2" display="_ftn2" xr:uid="{74DB3199-791E-4FED-9C20-E93C69505EA4}"/>
@@ -7498,7 +7501,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="139" t="s">
+      <c r="A3" s="135" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2"/>
@@ -7512,7 +7515,7 @@
       <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="139"/>
+      <c r="A4" s="135"/>
       <c r="B4" s="2"/>
       <c r="C4" s="23" t="s">
         <v>65</v>
@@ -7524,7 +7527,7 @@
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="139"/>
+      <c r="A5" s="135"/>
       <c r="B5" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -7542,7 +7545,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="140" t="s">
+      <c r="A6" s="136" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2">
@@ -7560,7 +7563,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="140"/>
+      <c r="A7" s="136"/>
       <c r="B7" s="2">
         <v>2.2000000000000002</v>
       </c>
@@ -7576,7 +7579,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="140" t="s">
+      <c r="A8" s="136" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2">
@@ -7596,7 +7599,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="140"/>
+      <c r="A9" s="136"/>
       <c r="B9" s="2"/>
       <c r="C9" s="23" t="s">
         <v>64</v>
@@ -7608,7 +7611,7 @@
       <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="140"/>
+      <c r="A10" s="136"/>
       <c r="B10" s="2"/>
       <c r="C10" s="23" t="s">
         <v>55</v>
@@ -7620,7 +7623,7 @@
       <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="140"/>
+      <c r="A11" s="136"/>
       <c r="B11" s="2"/>
       <c r="C11" s="23" t="s">
         <v>50</v>
@@ -7632,7 +7635,7 @@
       <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="140"/>
+      <c r="A12" s="136"/>
       <c r="B12" s="2">
         <v>3.2</v>
       </c>
@@ -7650,7 +7653,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="140"/>
+      <c r="A13" s="136"/>
       <c r="B13" s="2">
         <v>12.1</v>
       </c>
@@ -7666,7 +7669,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="140"/>
+      <c r="A14" s="136"/>
       <c r="B14" s="2">
         <v>12.2</v>
       </c>
@@ -7682,7 +7685,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="140"/>
+      <c r="A15" s="136"/>
       <c r="B15" s="2">
         <v>12.3</v>
       </c>
@@ -7698,7 +7701,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="139" t="s">
+      <c r="A16" s="135" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="18">
@@ -7718,7 +7721,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="139"/>
+      <c r="A17" s="135"/>
       <c r="B17" s="18">
         <v>5.2</v>
       </c>
@@ -7736,7 +7739,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="139"/>
+      <c r="A18" s="135"/>
       <c r="B18" s="2">
         <v>5.3</v>
       </c>
@@ -7754,7 +7757,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="139"/>
+      <c r="A19" s="135"/>
       <c r="B19" s="18">
         <v>5.4</v>
       </c>
@@ -7772,7 +7775,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="139"/>
+      <c r="A20" s="135"/>
       <c r="B20" s="18"/>
       <c r="C20" s="22" t="s">
         <v>53</v>
@@ -7784,7 +7787,7 @@
       <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="139"/>
+      <c r="A21" s="135"/>
       <c r="B21" s="18"/>
       <c r="C21" s="22" t="s">
         <v>54</v>
@@ -7796,7 +7799,7 @@
       <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="139" t="s">
+      <c r="A22" s="135" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="18">
@@ -7816,7 +7819,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="139"/>
+      <c r="A23" s="135"/>
       <c r="B23" s="2"/>
       <c r="C23" s="22" t="s">
         <v>52</v>
@@ -7828,7 +7831,7 @@
       <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="139"/>
+      <c r="A24" s="135"/>
       <c r="B24" s="2"/>
       <c r="C24" s="22" t="s">
         <v>51</v>
@@ -7840,7 +7843,7 @@
       <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="140" t="s">
+      <c r="A25" s="136" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="2">
@@ -7858,7 +7861,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="140"/>
+      <c r="A26" s="136"/>
       <c r="B26" s="2">
         <v>7.2</v>
       </c>
@@ -7874,7 +7877,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="142" t="s">
+      <c r="A27" s="138" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="18">
@@ -7894,7 +7897,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="142"/>
+      <c r="A28" s="138"/>
       <c r="B28" s="18">
         <v>8.1999999999999993</v>
       </c>
@@ -7912,7 +7915,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="142"/>
+      <c r="A29" s="138"/>
       <c r="B29" s="18">
         <v>8.3000000000000007</v>
       </c>
@@ -7930,7 +7933,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="142"/>
+      <c r="A30" s="138"/>
       <c r="B30" s="24">
         <v>8.1</v>
       </c>
@@ -7948,7 +7951,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="142"/>
+      <c r="A31" s="138"/>
       <c r="B31" s="24">
         <v>8.1999999999999993</v>
       </c>
@@ -7966,7 +7969,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="142"/>
+      <c r="A32" s="138"/>
       <c r="B32" s="24">
         <v>8.3000000000000007</v>
       </c>
@@ -7984,7 +7987,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="139" t="s">
+      <c r="A33" s="135" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="2">
@@ -8002,7 +8005,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="139"/>
+      <c r="A34" s="135"/>
       <c r="B34" s="2">
         <v>9.1999999999999993</v>
       </c>
@@ -8018,7 +8021,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="139"/>
+      <c r="A35" s="135"/>
       <c r="B35" s="2"/>
       <c r="C35" s="23" t="s">
         <v>59</v>
@@ -8048,7 +8051,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="141" t="s">
+      <c r="A37" s="137" t="s">
         <v>39</v>
       </c>
       <c r="B37" s="4">
@@ -8066,7 +8069,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="141"/>
+      <c r="A38" s="137"/>
       <c r="B38" s="4">
         <v>11.2</v>
       </c>
@@ -8082,7 +8085,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" s="16" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="141"/>
+      <c r="A39" s="137"/>
       <c r="B39" s="4">
         <v>11.3</v>
       </c>
@@ -8098,7 +8101,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" s="16" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="141"/>
+      <c r="A40" s="137"/>
       <c r="B40" s="4"/>
       <c r="C40" s="22" t="s">
         <v>66</v>
@@ -8110,7 +8113,7 @@
       <c r="F40" s="28"/>
     </row>
     <row r="41" spans="1:6" s="16" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="141"/>
+      <c r="A41" s="137"/>
       <c r="B41" s="4"/>
       <c r="C41" s="22" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Automatic update of 18/05/2024 at 05:28
</commit_message>
<xml_diff>
--- a/Indicadores OPI-CETG rev 28.04.24 v3.xlsx
+++ b/Indicadores OPI-CETG rev 28.04.24 v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\03. Job\05. CONSULTORIAS\13. MEF\FIDT_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81620A2A-F388-426A-9916-2634B9E5BC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56C0AF8-AC83-42A1-B475-DA6777E9499C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{A4291CEF-37A6-4732-90F4-77F55B4FD4D0}"/>
   </bookViews>
@@ -72,6 +72,112 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>51985</author>
+  </authors>
+  <commentList>
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{9744D5A9-97A7-4568-B8D4-F953D8E1A749}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>51985:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Loc_P108_SaFiLe.dbf:</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{EC39B6B2-0B0D-4542-8211-D4ECE638AF5A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>51985:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Loc_P200_ServBa.dbf:</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{6BB04020-EC9C-41D8-8CD0-25A32602687F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>51985:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Loc_P200_ServBa.dbf:</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{2CF77156-3E88-422D-9FD5-3FAE1038E747}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>51985:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Loc_P200_ServBa.dbf:</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="339">
   <si>
@@ -1212,48 +1318,12 @@
     <t>VARIABLES</t>
   </si>
   <si>
-    <t>v10_</t>
-  </si>
-  <si>
     <t>v11_</t>
   </si>
   <si>
-    <t>v12_</t>
-  </si>
-  <si>
-    <t>v13_</t>
-  </si>
-  <si>
     <t>v14_</t>
   </si>
   <si>
-    <t>v15_</t>
-  </si>
-  <si>
-    <t>v16_</t>
-  </si>
-  <si>
-    <t>v17_</t>
-  </si>
-  <si>
-    <t>v18_</t>
-  </si>
-  <si>
-    <t>v19_</t>
-  </si>
-  <si>
-    <t>v20_</t>
-  </si>
-  <si>
-    <t>v21_</t>
-  </si>
-  <si>
-    <t>v22_</t>
-  </si>
-  <si>
-    <t>v23_</t>
-  </si>
-  <si>
     <t>v24_</t>
   </si>
   <si>
@@ -1282,9 +1352,6 @@
   </si>
   <si>
     <t>v33_</t>
-  </si>
-  <si>
-    <t>v42_</t>
   </si>
   <si>
     <t>v46_</t>
@@ -1353,13 +1420,54 @@
   </si>
   <si>
     <t>v09_Años_escolaridad</t>
+  </si>
+  <si>
+    <t>v42_PEA_Agri_gana_silvi_pesca</t>
+  </si>
+  <si>
+    <t>v19_Sin_agua_LE</t>
+  </si>
+  <si>
+    <t>v20_Sin_desagüe_LE</t>
+  </si>
+  <si>
+    <t>v21_Sin_luz_LE</t>
+  </si>
+  <si>
+    <t>v15_No_Registros_Públicos_LE</t>
+  </si>
+  <si>
+    <t>v10_No_estudian_6_17</t>
+  </si>
+  <si>
+    <t>v13_Sin_PC_Tablet_Laptop</t>
+  </si>
+  <si>
+    <t>v12_P_aulas_bueno_regular</t>
+  </si>
+  <si>
+    <t>v16_No_paredes_LE</t>
+  </si>
+  <si>
+    <t>v17_No_techo_LE</t>
+  </si>
+  <si>
+    <t>v18_No_piso_LE</t>
+  </si>
+  <si>
+    <t>v22_No_Electricidad_LE</t>
+  </si>
+  <si>
+    <t>v23_Cerco_perimétrico_total
+v23_Cerco_perimétrico_parcial
+v23_Cerco_perimétrico_no_tiene</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1514,8 +1622,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1549,12 +1670,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1664,7 +1779,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -1964,15 +2079,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1982,6 +2088,36 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1997,33 +2133,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2033,12 +2142,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2070,18 +2179,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2458,8 +2555,8 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="113"/>
-      <c r="B3" s="110" t="s">
+      <c r="A3" s="120"/>
+      <c r="B3" s="117" t="s">
         <v>99</v>
       </c>
       <c r="C3" s="31"/>
@@ -2476,8 +2573,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="113"/>
-      <c r="B4" s="110"/>
+      <c r="A4" s="120"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="31"/>
       <c r="D4" s="23" t="s">
         <v>65</v>
@@ -2489,8 +2586,8 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="113"/>
-      <c r="B5" s="110"/>
+      <c r="A5" s="120"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="31">
         <v>1.1000000000000001</v>
       </c>
@@ -2508,8 +2605,8 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="113"/>
-      <c r="B6" s="110" t="s">
+      <c r="A6" s="120"/>
+      <c r="B6" s="117" t="s">
         <v>68</v>
       </c>
       <c r="C6" s="31">
@@ -2527,8 +2624,8 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="113"/>
-      <c r="B7" s="110"/>
+      <c r="A7" s="120"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="31">
         <v>2.2000000000000002</v>
       </c>
@@ -2544,8 +2641,8 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="113"/>
-      <c r="B8" s="110" t="s">
+      <c r="A8" s="120"/>
+      <c r="B8" s="117" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="31">
@@ -2565,8 +2662,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="113"/>
-      <c r="B9" s="110"/>
+      <c r="A9" s="120"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="31"/>
       <c r="D9" s="23" t="s">
         <v>117</v>
@@ -2581,8 +2678,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="113"/>
-      <c r="B10" s="110"/>
+      <c r="A10" s="120"/>
+      <c r="B10" s="117"/>
       <c r="C10" s="31"/>
       <c r="D10" s="23" t="s">
         <v>105</v>
@@ -2592,13 +2689,13 @@
       </c>
       <c r="F10" s="56"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="111" t="s">
+      <c r="H10" s="118" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="113"/>
-      <c r="B11" s="110"/>
+      <c r="A11" s="120"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="31"/>
       <c r="D11" s="23" t="s">
         <v>50</v>
@@ -2608,11 +2705,11 @@
       </c>
       <c r="F11" s="56"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="111"/>
+      <c r="H11" s="118"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="113"/>
-      <c r="B12" s="110"/>
+      <c r="A12" s="120"/>
+      <c r="B12" s="117"/>
       <c r="C12" s="31">
         <v>3.2</v>
       </c>
@@ -2630,8 +2727,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="113"/>
-      <c r="B13" s="110"/>
+      <c r="A13" s="120"/>
+      <c r="B13" s="117"/>
       <c r="C13" s="31">
         <v>12.1</v>
       </c>
@@ -2647,8 +2744,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="113"/>
-      <c r="B14" s="110"/>
+      <c r="A14" s="120"/>
+      <c r="B14" s="117"/>
       <c r="C14" s="31">
         <v>12.2</v>
       </c>
@@ -2664,8 +2761,8 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="113"/>
-      <c r="B15" s="110"/>
+      <c r="A15" s="120"/>
+      <c r="B15" s="117"/>
       <c r="C15" s="31">
         <v>12.3</v>
       </c>
@@ -2681,8 +2778,8 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="113"/>
-      <c r="B16" s="110" t="s">
+      <c r="A16" s="120"/>
+      <c r="B16" s="117" t="s">
         <v>67</v>
       </c>
       <c r="C16" s="31"/>
@@ -2696,8 +2793,8 @@
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="113"/>
-      <c r="B17" s="110"/>
+      <c r="A17" s="120"/>
+      <c r="B17" s="117"/>
       <c r="C17" s="31"/>
       <c r="D17" s="23" t="s">
         <v>108</v>
@@ -2709,8 +2806,8 @@
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="113"/>
-      <c r="B18" s="110"/>
+      <c r="A18" s="120"/>
+      <c r="B18" s="117"/>
       <c r="C18" s="31"/>
       <c r="D18" s="23" t="s">
         <v>109</v>
@@ -2722,8 +2819,8 @@
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="113"/>
-      <c r="B19" s="110"/>
+      <c r="A19" s="120"/>
+      <c r="B19" s="117"/>
       <c r="C19" s="31"/>
       <c r="D19" s="23" t="s">
         <v>110</v>
@@ -2735,8 +2832,8 @@
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="113"/>
-      <c r="B20" s="110"/>
+      <c r="A20" s="120"/>
+      <c r="B20" s="117"/>
       <c r="C20" s="31"/>
       <c r="D20" s="23" t="s">
         <v>111</v>
@@ -2748,8 +2845,8 @@
       <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="113"/>
-      <c r="B21" s="110"/>
+      <c r="A21" s="120"/>
+      <c r="B21" s="117"/>
       <c r="C21" s="31"/>
       <c r="D21" s="23" t="s">
         <v>112</v>
@@ -2764,8 +2861,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="113"/>
-      <c r="B22" s="110" t="s">
+      <c r="A22" s="120"/>
+      <c r="B22" s="117" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="35">
@@ -2788,8 +2885,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="113"/>
-      <c r="B23" s="110"/>
+      <c r="A23" s="120"/>
+      <c r="B23" s="117"/>
       <c r="C23" s="35">
         <v>5.2</v>
       </c>
@@ -2810,8 +2907,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="113"/>
-      <c r="B24" s="110"/>
+      <c r="A24" s="120"/>
+      <c r="B24" s="117"/>
       <c r="C24" s="31">
         <v>5.3</v>
       </c>
@@ -2829,8 +2926,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="113"/>
-      <c r="B25" s="110"/>
+      <c r="A25" s="120"/>
+      <c r="B25" s="117"/>
       <c r="C25" s="35">
         <v>5.4</v>
       </c>
@@ -2851,8 +2948,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="113"/>
-      <c r="B26" s="110"/>
+      <c r="A26" s="120"/>
+      <c r="B26" s="117"/>
       <c r="C26" s="35"/>
       <c r="D26" s="41" t="s">
         <v>53</v>
@@ -2867,8 +2964,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="113"/>
-      <c r="B27" s="110"/>
+      <c r="A27" s="120"/>
+      <c r="B27" s="117"/>
       <c r="C27" s="35"/>
       <c r="D27" s="41" t="s">
         <v>54</v>
@@ -2883,8 +2980,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="113"/>
-      <c r="B28" s="110" t="s">
+      <c r="A28" s="120"/>
+      <c r="B28" s="117" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="35">
@@ -2907,8 +3004,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="113"/>
-      <c r="B29" s="110"/>
+      <c r="A29" s="120"/>
+      <c r="B29" s="117"/>
       <c r="C29" s="31"/>
       <c r="D29" s="41" t="s">
         <v>51</v>
@@ -2923,8 +3020,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="113"/>
-      <c r="B30" s="110"/>
+      <c r="A30" s="120"/>
+      <c r="B30" s="117"/>
       <c r="C30" s="31"/>
       <c r="D30" s="41" t="s">
         <v>52</v>
@@ -2939,8 +3036,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="113"/>
-      <c r="B31" s="110" t="s">
+      <c r="A31" s="120"/>
+      <c r="B31" s="117" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="31">
@@ -2958,8 +3055,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="113"/>
-      <c r="B32" s="110"/>
+      <c r="A32" s="120"/>
+      <c r="B32" s="117"/>
       <c r="C32" s="31">
         <v>7.2</v>
       </c>
@@ -2975,8 +3072,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="113"/>
-      <c r="B33" s="110" t="s">
+      <c r="A33" s="120"/>
+      <c r="B33" s="117" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="35">
@@ -2999,8 +3096,8 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="113"/>
-      <c r="B34" s="110"/>
+      <c r="A34" s="120"/>
+      <c r="B34" s="117"/>
       <c r="C34" s="35">
         <v>8.1999999999999993</v>
       </c>
@@ -3021,8 +3118,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="113"/>
-      <c r="B35" s="110"/>
+      <c r="A35" s="120"/>
+      <c r="B35" s="117"/>
       <c r="C35" s="35">
         <v>8.3000000000000007</v>
       </c>
@@ -3043,8 +3140,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="113"/>
-      <c r="B36" s="110"/>
+      <c r="A36" s="120"/>
+      <c r="B36" s="117"/>
       <c r="C36" s="32">
         <v>8.1</v>
       </c>
@@ -3065,8 +3162,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="113"/>
-      <c r="B37" s="110"/>
+      <c r="A37" s="120"/>
+      <c r="B37" s="117"/>
       <c r="C37" s="32">
         <v>8.1999999999999993</v>
       </c>
@@ -3087,8 +3184,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="113"/>
-      <c r="B38" s="110"/>
+      <c r="A38" s="120"/>
+      <c r="B38" s="117"/>
       <c r="C38" s="32">
         <v>8.3000000000000007</v>
       </c>
@@ -3109,8 +3206,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="113"/>
-      <c r="B39" s="110"/>
+      <c r="A39" s="120"/>
+      <c r="B39" s="117"/>
       <c r="C39" s="32"/>
       <c r="D39" s="22" t="s">
         <v>72</v>
@@ -3122,8 +3219,8 @@
       <c r="G39" s="43"/>
     </row>
     <row r="40" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="113"/>
-      <c r="B40" s="110" t="s">
+      <c r="A40" s="120"/>
+      <c r="B40" s="117" t="s">
         <v>34</v>
       </c>
       <c r="C40" s="31">
@@ -3141,8 +3238,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="113"/>
-      <c r="B41" s="110"/>
+      <c r="A41" s="120"/>
+      <c r="B41" s="117"/>
       <c r="C41" s="31">
         <v>9.1999999999999993</v>
       </c>
@@ -3158,8 +3255,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="113"/>
-      <c r="B42" s="110"/>
+      <c r="A42" s="120"/>
+      <c r="B42" s="117"/>
       <c r="C42" s="31"/>
       <c r="D42" s="23" t="s">
         <v>59</v>
@@ -3171,8 +3268,8 @@
       <c r="G42" s="12"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="113"/>
-      <c r="B43" s="110"/>
+      <c r="A43" s="120"/>
+      <c r="B43" s="117"/>
       <c r="C43" s="31"/>
       <c r="D43" s="22" t="s">
         <v>86</v>
@@ -3187,8 +3284,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="113"/>
-      <c r="B44" s="110"/>
+      <c r="A44" s="120"/>
+      <c r="B44" s="117"/>
       <c r="C44" s="31"/>
       <c r="D44" s="22" t="s">
         <v>87</v>
@@ -3203,8 +3300,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="113"/>
-      <c r="B45" s="110"/>
+      <c r="A45" s="120"/>
+      <c r="B45" s="117"/>
       <c r="C45" s="31"/>
       <c r="D45" s="22" t="s">
         <v>100</v>
@@ -3219,10 +3316,10 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="113" t="s">
+      <c r="A46" s="120" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="112" t="s">
+      <c r="B46" s="119" t="s">
         <v>114</v>
       </c>
       <c r="C46" s="34">
@@ -3243,8 +3340,8 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="113"/>
-      <c r="B47" s="112"/>
+      <c r="A47" s="120"/>
+      <c r="B47" s="119"/>
       <c r="C47" s="34">
         <v>11.2</v>
       </c>
@@ -3263,8 +3360,8 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="113"/>
-      <c r="B48" s="112"/>
+      <c r="A48" s="120"/>
+      <c r="B48" s="119"/>
       <c r="C48" s="34">
         <v>11.3</v>
       </c>
@@ -3283,8 +3380,8 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="113"/>
-      <c r="B49" s="112"/>
+      <c r="A49" s="120"/>
+      <c r="B49" s="119"/>
       <c r="C49" s="34"/>
       <c r="D49" s="22" t="s">
         <v>66</v>
@@ -3299,8 +3396,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="113"/>
-      <c r="B50" s="112"/>
+      <c r="A50" s="120"/>
+      <c r="B50" s="119"/>
       <c r="C50" s="34"/>
       <c r="D50" s="22" t="s">
         <v>63</v>
@@ -3315,10 +3412,10 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="109" t="s">
+      <c r="A51" s="116" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="109"/>
+      <c r="B51" s="116"/>
       <c r="C51" s="62"/>
       <c r="D51" s="52" t="s">
         <v>115</v>
@@ -3331,8 +3428,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="109"/>
-      <c r="B52" s="109"/>
+      <c r="A52" s="116"/>
+      <c r="B52" s="116"/>
       <c r="C52" s="62"/>
       <c r="D52" s="52" t="s">
         <v>89</v>
@@ -3343,8 +3440,8 @@
       <c r="F52" s="47"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="109"/>
-      <c r="B53" s="109"/>
+      <c r="A53" s="116"/>
+      <c r="B53" s="116"/>
       <c r="C53" s="62"/>
       <c r="D53" s="54" t="s">
         <v>38</v>
@@ -3355,8 +3452,8 @@
       <c r="F53" s="47"/>
     </row>
     <row r="54" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="109"/>
-      <c r="B54" s="109"/>
+      <c r="A54" s="116"/>
+      <c r="B54" s="116"/>
       <c r="C54" s="62"/>
       <c r="D54" s="52" t="s">
         <v>81</v>
@@ -3367,41 +3464,41 @@
       <c r="F54" s="47"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="114" t="s">
+      <c r="A55" s="107" t="s">
         <v>126</v>
       </c>
-      <c r="B55" s="114"/>
-      <c r="C55" s="114"/>
-      <c r="D55" s="114"/>
-      <c r="E55" s="114"/>
+      <c r="B55" s="107"/>
+      <c r="C55" s="107"/>
+      <c r="D55" s="107"/>
+      <c r="E55" s="107"/>
       <c r="F55" s="47"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="115"/>
-      <c r="B56" s="115"/>
-      <c r="C56" s="115"/>
-      <c r="D56" s="115"/>
-      <c r="E56" s="115"/>
+      <c r="A56" s="108"/>
+      <c r="B56" s="108"/>
+      <c r="C56" s="108"/>
+      <c r="D56" s="108"/>
+      <c r="E56" s="108"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="115"/>
-      <c r="B57" s="115"/>
-      <c r="C57" s="115"/>
-      <c r="D57" s="115"/>
-      <c r="E57" s="115"/>
+      <c r="A57" s="108"/>
+      <c r="B57" s="108"/>
+      <c r="C57" s="108"/>
+      <c r="D57" s="108"/>
+      <c r="E57" s="108"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="116"/>
-      <c r="B58" s="116"/>
-      <c r="C58" s="116"/>
-      <c r="D58" s="116"/>
-      <c r="E58" s="116"/>
+      <c r="A58" s="109"/>
+      <c r="B58" s="109"/>
+      <c r="C58" s="109"/>
+      <c r="D58" s="109"/>
+      <c r="E58" s="109"/>
     </row>
     <row r="59" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A59" s="117" t="s">
+      <c r="A59" s="110" t="s">
         <v>118</v>
       </c>
-      <c r="B59" s="120" t="s">
+      <c r="B59" s="113" t="s">
         <v>125</v>
       </c>
       <c r="C59" s="64"/>
@@ -3416,8 +3513,8 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="117"/>
-      <c r="B60" s="121"/>
+      <c r="A60" s="110"/>
+      <c r="B60" s="114"/>
       <c r="C60" s="64"/>
       <c r="D60" s="69" t="s">
         <v>137</v>
@@ -3430,8 +3527,8 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="117"/>
-      <c r="B61" s="122"/>
+      <c r="A61" s="110"/>
+      <c r="B61" s="115"/>
       <c r="C61" s="64"/>
       <c r="D61" s="69" t="s">
         <v>138</v>
@@ -3444,8 +3541,8 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="117"/>
-      <c r="B62" s="118" t="s">
+      <c r="A62" s="110"/>
+      <c r="B62" s="111" t="s">
         <v>120</v>
       </c>
       <c r="C62" s="66"/>
@@ -3460,8 +3557,8 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="117"/>
-      <c r="B63" s="118"/>
+      <c r="A63" s="110"/>
+      <c r="B63" s="111"/>
       <c r="C63" s="66"/>
       <c r="D63" s="67" t="s">
         <v>139</v>
@@ -3474,8 +3571,8 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A64" s="117"/>
-      <c r="B64" s="118"/>
+      <c r="A64" s="110"/>
+      <c r="B64" s="111"/>
       <c r="C64" s="66"/>
       <c r="D64" s="67" t="s">
         <v>128</v>
@@ -3488,8 +3585,8 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A65" s="117"/>
-      <c r="B65" s="118"/>
+      <c r="A65" s="110"/>
+      <c r="B65" s="111"/>
       <c r="C65" s="66"/>
       <c r="D65" s="67" t="s">
         <v>129</v>
@@ -3502,8 +3599,8 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="117"/>
-      <c r="B66" s="118"/>
+      <c r="A66" s="110"/>
+      <c r="B66" s="111"/>
       <c r="C66" s="66"/>
       <c r="D66" s="67" t="s">
         <v>130</v>
@@ -3516,8 +3613,8 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="117"/>
-      <c r="B67" s="118" t="s">
+      <c r="A67" s="110"/>
+      <c r="B67" s="111" t="s">
         <v>122</v>
       </c>
       <c r="C67" s="66"/>
@@ -3532,8 +3629,8 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="117"/>
-      <c r="B68" s="118"/>
+      <c r="A68" s="110"/>
+      <c r="B68" s="111"/>
       <c r="C68" s="66"/>
       <c r="D68" s="67" t="s">
         <v>133</v>
@@ -3546,8 +3643,8 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A69" s="117"/>
-      <c r="B69" s="118"/>
+      <c r="A69" s="110"/>
+      <c r="B69" s="111"/>
       <c r="C69" s="66"/>
       <c r="D69" s="67" t="s">
         <v>132</v>
@@ -3560,8 +3657,8 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="117"/>
-      <c r="B70" s="118"/>
+      <c r="A70" s="110"/>
+      <c r="B70" s="111"/>
       <c r="C70" s="66"/>
       <c r="D70" s="68" t="s">
         <v>135</v>
@@ -3574,8 +3671,8 @@
       </c>
     </row>
     <row r="71" spans="1:8" s="16" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="117"/>
-      <c r="B71" s="119" t="s">
+      <c r="A71" s="110"/>
+      <c r="B71" s="112" t="s">
         <v>123</v>
       </c>
       <c r="C71" s="64"/>
@@ -3591,8 +3688,8 @@
       <c r="H71" s="71"/>
     </row>
     <row r="72" spans="1:8" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="117"/>
-      <c r="B72" s="119"/>
+      <c r="A72" s="110"/>
+      <c r="B72" s="112"/>
       <c r="C72" s="64"/>
       <c r="D72" s="69" t="s">
         <v>141</v>
@@ -3606,8 +3703,8 @@
       <c r="H72" s="71"/>
     </row>
     <row r="73" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="117"/>
-      <c r="B73" s="118" t="s">
+      <c r="A73" s="110"/>
+      <c r="B73" s="111" t="s">
         <v>124</v>
       </c>
       <c r="C73" s="66"/>
@@ -3622,8 +3719,8 @@
       </c>
     </row>
     <row r="74" spans="1:8" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.25">
-      <c r="A74" s="117"/>
-      <c r="B74" s="118"/>
+      <c r="A74" s="110"/>
+      <c r="B74" s="111"/>
       <c r="C74" s="64"/>
       <c r="D74" s="69" t="s">
         <v>134</v>
@@ -3646,13 +3743,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A55:E58"/>
-    <mergeCell ref="A59:A74"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="B59:B61"/>
     <mergeCell ref="A51:B54"/>
     <mergeCell ref="B16:B21"/>
     <mergeCell ref="H10:H11"/>
@@ -3667,6 +3757,13 @@
     <mergeCell ref="B22:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B32"/>
+    <mergeCell ref="A55:E58"/>
+    <mergeCell ref="A59:A74"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="B59:B61"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E53" location="_ftn2" display="_ftn2" xr:uid="{FFC9BABA-D715-48D2-801D-3C2A2DB136EB}"/>
@@ -3755,13 +3852,13 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="125" t="s">
+      <c r="D4" s="123" t="s">
         <v>161</v>
       </c>
-      <c r="E4" s="123" t="s">
+      <c r="E4" s="121" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="123" t="s">
+      <c r="F4" s="121" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3775,9 +3872,9 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="125"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
@@ -3789,11 +3886,11 @@
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="125" t="s">
+      <c r="D6" s="123" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
@@ -3805,9 +3902,9 @@
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="125"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
     </row>
     <row r="8" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="74" t="s">
@@ -3819,11 +3916,11 @@
       <c r="C8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="123" t="s">
+      <c r="D8" s="121" t="s">
         <v>164</v>
       </c>
-      <c r="E8" s="123"/>
-      <c r="F8" s="123"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="121"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
@@ -3835,9 +3932,9 @@
       <c r="C9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="123"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
+      <c r="D9" s="121"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="121"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
@@ -3849,11 +3946,11 @@
       <c r="C10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="123" t="s">
+      <c r="D10" s="121" t="s">
         <v>165</v>
       </c>
-      <c r="E10" s="123"/>
-      <c r="F10" s="123"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="121"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="74" t="s">
@@ -3865,9 +3962,9 @@
       <c r="C11" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="123"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="123"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
@@ -3879,9 +3976,9 @@
       <c r="C12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="123"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="123"/>
+      <c r="D12" s="121"/>
+      <c r="E12" s="121"/>
+      <c r="F12" s="121"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="78" t="s">
@@ -3893,11 +3990,11 @@
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="123" t="s">
+      <c r="D13" s="121" t="s">
         <v>166</v>
       </c>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
+      <c r="E13" s="121"/>
+      <c r="F13" s="121"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="78" t="s">
@@ -3909,9 +4006,9 @@
       <c r="C14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="123"/>
-      <c r="E14" s="123"/>
-      <c r="F14" s="123"/>
+      <c r="D14" s="121"/>
+      <c r="E14" s="121"/>
+      <c r="F14" s="121"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="78" t="s">
@@ -3923,9 +4020,9 @@
       <c r="C15" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="123"/>
-      <c r="E15" s="123"/>
-      <c r="F15" s="123"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="121"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="78" t="s">
@@ -3937,9 +4034,9 @@
       <c r="C16" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="123"/>
-      <c r="E16" s="123"/>
-      <c r="F16" s="123"/>
+      <c r="D16" s="121"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="121"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="78" t="s">
@@ -3951,9 +4048,9 @@
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="123"/>
-      <c r="E17" s="123"/>
-      <c r="F17" s="123"/>
+      <c r="D17" s="121"/>
+      <c r="E17" s="121"/>
+      <c r="F17" s="121"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
@@ -3968,8 +4065,8 @@
       <c r="D18" s="79" t="s">
         <v>167</v>
       </c>
-      <c r="E18" s="123"/>
-      <c r="F18" s="123"/>
+      <c r="E18" s="121"/>
+      <c r="F18" s="121"/>
     </row>
     <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
@@ -3981,13 +4078,13 @@
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="123" t="s">
+      <c r="D19" s="121" t="s">
         <v>168</v>
       </c>
-      <c r="E19" s="123" t="s">
+      <c r="E19" s="121" t="s">
         <v>197</v>
       </c>
-      <c r="F19" s="123" t="s">
+      <c r="F19" s="121" t="s">
         <v>169</v>
       </c>
     </row>
@@ -4001,9 +4098,9 @@
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="123"/>
-      <c r="E20" s="123"/>
-      <c r="F20" s="123"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="121"/>
+      <c r="F20" s="121"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
@@ -4015,13 +4112,13 @@
       <c r="C21" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="123" t="s">
+      <c r="D21" s="121" t="s">
         <v>170</v>
       </c>
-      <c r="E21" s="123" t="s">
+      <c r="E21" s="121" t="s">
         <v>172</v>
       </c>
-      <c r="F21" s="124" t="s">
+      <c r="F21" s="122" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4035,9 +4132,9 @@
       <c r="C22" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="123"/>
-      <c r="E22" s="123"/>
-      <c r="F22" s="124"/>
+      <c r="D22" s="121"/>
+      <c r="E22" s="121"/>
+      <c r="F22" s="122"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="74" t="s">
@@ -4049,9 +4146,9 @@
       <c r="C23" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="124"/>
+      <c r="D23" s="121"/>
+      <c r="E23" s="121"/>
+      <c r="F23" s="122"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="74" t="s">
@@ -4063,9 +4160,9 @@
       <c r="C24" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="123"/>
-      <c r="E24" s="123"/>
-      <c r="F24" s="124"/>
+      <c r="D24" s="121"/>
+      <c r="E24" s="121"/>
+      <c r="F24" s="122"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="74" t="s">
@@ -4077,9 +4174,9 @@
       <c r="C25" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="123"/>
-      <c r="E25" s="123"/>
-      <c r="F25" s="124"/>
+      <c r="D25" s="121"/>
+      <c r="E25" s="121"/>
+      <c r="F25" s="122"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="74" t="s">
@@ -4091,9 +4188,9 @@
       <c r="C26" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="123"/>
-      <c r="E26" s="123"/>
-      <c r="F26" s="124"/>
+      <c r="D26" s="121"/>
+      <c r="E26" s="121"/>
+      <c r="F26" s="122"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="74" t="s">
@@ -4105,13 +4202,13 @@
       <c r="C27" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="123" t="s">
+      <c r="D27" s="121" t="s">
         <v>174</v>
       </c>
-      <c r="E27" s="123" t="s">
+      <c r="E27" s="121" t="s">
         <v>175</v>
       </c>
-      <c r="F27" s="123" t="s">
+      <c r="F27" s="121" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4125,9 +4222,9 @@
       <c r="C28" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="123"/>
-      <c r="E28" s="123"/>
-      <c r="F28" s="123"/>
+      <c r="D28" s="121"/>
+      <c r="E28" s="121"/>
+      <c r="F28" s="121"/>
     </row>
     <row r="29" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="74" t="s">
@@ -4139,9 +4236,9 @@
       <c r="C29" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D29" s="123"/>
-      <c r="E29" s="123"/>
-      <c r="F29" s="123"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="121"/>
+      <c r="F29" s="121"/>
     </row>
     <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="74" t="s">
@@ -4153,9 +4250,9 @@
       <c r="C30" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="123"/>
-      <c r="E30" s="123"/>
-      <c r="F30" s="123"/>
+      <c r="D30" s="121"/>
+      <c r="E30" s="121"/>
+      <c r="F30" s="121"/>
     </row>
     <row r="31" spans="1:6" ht="409.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="74" t="s">
@@ -4187,13 +4284,13 @@
       <c r="C32" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="123" t="s">
+      <c r="D32" s="121" t="s">
         <v>176</v>
       </c>
-      <c r="E32" s="123" t="s">
+      <c r="E32" s="121" t="s">
         <v>177</v>
       </c>
-      <c r="F32" s="124" t="s">
+      <c r="F32" s="122" t="s">
         <v>178</v>
       </c>
     </row>
@@ -4207,9 +4304,9 @@
       <c r="C33" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="124"/>
-      <c r="E33" s="123"/>
-      <c r="F33" s="124"/>
+      <c r="D33" s="122"/>
+      <c r="E33" s="121"/>
+      <c r="F33" s="122"/>
     </row>
     <row r="34" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="74" t="s">
@@ -4221,9 +4318,9 @@
       <c r="C34" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="124"/>
-      <c r="E34" s="123"/>
-      <c r="F34" s="124"/>
+      <c r="D34" s="122"/>
+      <c r="E34" s="121"/>
+      <c r="F34" s="122"/>
     </row>
     <row r="35" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="80" t="s">
@@ -4235,13 +4332,13 @@
       <c r="C35" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="123" t="s">
+      <c r="D35" s="121" t="s">
         <v>179</v>
       </c>
-      <c r="E35" s="123" t="s">
+      <c r="E35" s="121" t="s">
         <v>180</v>
       </c>
-      <c r="F35" s="123" t="s">
+      <c r="F35" s="121" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4255,9 +4352,9 @@
       <c r="C36" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="123"/>
-      <c r="E36" s="123"/>
-      <c r="F36" s="123"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="121"/>
+      <c r="F36" s="121"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="81" t="s">
@@ -4309,13 +4406,13 @@
       <c r="C39" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D39" s="123" t="s">
+      <c r="D39" s="121" t="s">
         <v>187</v>
       </c>
-      <c r="E39" s="123" t="s">
+      <c r="E39" s="121" t="s">
         <v>188</v>
       </c>
-      <c r="F39" s="123" t="s">
+      <c r="F39" s="121" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4329,9 +4426,9 @@
       <c r="C40" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="123"/>
-      <c r="E40" s="123"/>
-      <c r="F40" s="123"/>
+      <c r="D40" s="121"/>
+      <c r="E40" s="121"/>
+      <c r="F40" s="121"/>
     </row>
     <row r="41" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A41" s="78" t="s">
@@ -4343,9 +4440,9 @@
       <c r="C41" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="123"/>
-      <c r="E41" s="123"/>
-      <c r="F41" s="123"/>
+      <c r="D41" s="121"/>
+      <c r="E41" s="121"/>
+      <c r="F41" s="121"/>
     </row>
     <row r="42" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="78" t="s">
@@ -4357,13 +4454,13 @@
       <c r="C42" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="123" t="s">
+      <c r="D42" s="121" t="s">
         <v>189</v>
       </c>
-      <c r="E42" s="123" t="s">
+      <c r="E42" s="121" t="s">
         <v>190</v>
       </c>
-      <c r="F42" s="123" t="s">
+      <c r="F42" s="121" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4377,9 +4474,9 @@
       <c r="C43" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="123"/>
-      <c r="E43" s="123"/>
-      <c r="F43" s="123"/>
+      <c r="D43" s="121"/>
+      <c r="E43" s="121"/>
+      <c r="F43" s="121"/>
     </row>
     <row r="44" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A44" s="78" t="s">
@@ -4391,9 +4488,9 @@
       <c r="C44" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D44" s="123"/>
-      <c r="E44" s="123"/>
-      <c r="F44" s="123"/>
+      <c r="D44" s="121"/>
+      <c r="E44" s="121"/>
+      <c r="F44" s="121"/>
     </row>
     <row r="45" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A45" s="78" t="s">
@@ -4405,9 +4502,9 @@
       <c r="C45" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="123"/>
-      <c r="E45" s="123"/>
-      <c r="F45" s="123"/>
+      <c r="D45" s="121"/>
+      <c r="E45" s="121"/>
+      <c r="F45" s="121"/>
     </row>
     <row r="46" spans="1:6" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="78" t="s">
@@ -4419,9 +4516,9 @@
       <c r="C46" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D46" s="123"/>
-      <c r="E46" s="123"/>
-      <c r="F46" s="123"/>
+      <c r="D46" s="121"/>
+      <c r="E46" s="121"/>
+      <c r="F46" s="121"/>
     </row>
     <row r="47" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A47" s="78" t="s">
@@ -4433,9 +4530,9 @@
       <c r="C47" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D47" s="123"/>
-      <c r="E47" s="123"/>
-      <c r="F47" s="123"/>
+      <c r="D47" s="121"/>
+      <c r="E47" s="121"/>
+      <c r="F47" s="121"/>
     </row>
     <row r="48" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A48" s="78" t="s">
@@ -4447,9 +4544,9 @@
       <c r="C48" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D48" s="123"/>
-      <c r="E48" s="123"/>
-      <c r="F48" s="123"/>
+      <c r="D48" s="121"/>
+      <c r="E48" s="121"/>
+      <c r="F48" s="121"/>
     </row>
     <row r="49" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" s="78" t="s">
@@ -4461,9 +4558,9 @@
       <c r="C49" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D49" s="123"/>
-      <c r="E49" s="123"/>
-      <c r="F49" s="123"/>
+      <c r="D49" s="121"/>
+      <c r="E49" s="121"/>
+      <c r="F49" s="121"/>
     </row>
     <row r="50" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A50" s="78" t="s">
@@ -4475,9 +4572,9 @@
       <c r="C50" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D50" s="123"/>
-      <c r="E50" s="123"/>
-      <c r="F50" s="123"/>
+      <c r="D50" s="121"/>
+      <c r="E50" s="121"/>
+      <c r="F50" s="121"/>
     </row>
     <row r="51" spans="1:6" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="78" t="s">
@@ -4489,9 +4586,9 @@
       <c r="C51" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D51" s="123"/>
-      <c r="E51" s="123"/>
-      <c r="F51" s="123"/>
+      <c r="D51" s="121"/>
+      <c r="E51" s="121"/>
+      <c r="F51" s="121"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="78" t="s">
@@ -4503,13 +4600,13 @@
       <c r="C52" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D52" s="123" t="s">
+      <c r="D52" s="121" t="s">
         <v>191</v>
       </c>
-      <c r="E52" s="123" t="s">
+      <c r="E52" s="121" t="s">
         <v>192</v>
       </c>
-      <c r="F52" s="123" t="s">
+      <c r="F52" s="121" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4523,9 +4620,9 @@
       <c r="C53" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D53" s="123"/>
-      <c r="E53" s="123"/>
-      <c r="F53" s="123"/>
+      <c r="D53" s="121"/>
+      <c r="E53" s="121"/>
+      <c r="F53" s="121"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="78" t="s">
@@ -4537,9 +4634,9 @@
       <c r="C54" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="123"/>
-      <c r="E54" s="123"/>
-      <c r="F54" s="123"/>
+      <c r="D54" s="121"/>
+      <c r="E54" s="121"/>
+      <c r="F54" s="121"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="78" t="s">
@@ -4551,12 +4648,30 @@
       <c r="C55" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D55" s="123"/>
-      <c r="E55" s="123"/>
-      <c r="F55" s="123"/>
+      <c r="D55" s="121"/>
+      <c r="E55" s="121"/>
+      <c r="F55" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="F52:F55"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="D42:D51"/>
+    <mergeCell ref="E42:E51"/>
+    <mergeCell ref="F42:F51"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="F32:F34"/>
     <mergeCell ref="D13:D17"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
@@ -4570,24 +4685,6 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="F52:F55"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="D42:D51"/>
-    <mergeCell ref="E42:E51"/>
-    <mergeCell ref="F42:F51"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C37" location="_ftn2" display="_ftn2" xr:uid="{25CB2AF1-E91C-4F96-A745-EB04437048A9}"/>
@@ -4679,16 +4776,16 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="125" t="s">
+      <c r="D4" s="123" t="s">
         <v>215</v>
       </c>
-      <c r="E4" s="123" t="s">
+      <c r="E4" s="121" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="123" t="s">
+      <c r="F4" s="121" t="s">
         <v>158</v>
       </c>
-      <c r="G4" s="125"/>
+      <c r="G4" s="123"/>
       <c r="H4" s="87"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4701,10 +4798,10 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="125"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="125"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="123"/>
       <c r="H5" s="87"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4717,12 +4814,12 @@
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="125" t="s">
+      <c r="D6" s="123" t="s">
         <v>216</v>
       </c>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="125"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="123"/>
       <c r="H6" s="87"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4735,10 +4832,10 @@
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="125"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="125"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="123"/>
       <c r="H7" s="87"/>
     </row>
     <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4751,12 +4848,12 @@
       <c r="C8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="125" t="s">
+      <c r="D8" s="123" t="s">
         <v>164</v>
       </c>
-      <c r="E8" s="123"/>
-      <c r="F8" s="123"/>
-      <c r="G8" s="125"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="121"/>
+      <c r="G8" s="123"/>
       <c r="H8" s="87"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4769,10 +4866,10 @@
       <c r="C9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="125"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="125"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="121"/>
+      <c r="G9" s="123"/>
       <c r="H9" s="87"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4785,12 +4882,12 @@
       <c r="C10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="125" t="s">
+      <c r="D10" s="123" t="s">
         <v>217</v>
       </c>
-      <c r="E10" s="123"/>
-      <c r="F10" s="123"/>
-      <c r="G10" s="125"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="121"/>
+      <c r="G10" s="123"/>
       <c r="H10" s="87"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4803,10 +4900,10 @@
       <c r="C11" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="125"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="123"/>
-      <c r="G11" s="125"/>
+      <c r="D11" s="123"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
+      <c r="G11" s="123"/>
       <c r="H11" s="87"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4819,10 +4916,10 @@
       <c r="C12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="125"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="125"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="121"/>
+      <c r="F12" s="121"/>
+      <c r="G12" s="123"/>
       <c r="H12" s="87"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4835,12 +4932,12 @@
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="125" t="s">
+      <c r="D13" s="123" t="s">
         <v>218</v>
       </c>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="125"/>
+      <c r="E13" s="121"/>
+      <c r="F13" s="121"/>
+      <c r="G13" s="123"/>
       <c r="H13" s="87"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4853,10 +4950,10 @@
       <c r="C14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="125"/>
-      <c r="E14" s="123"/>
-      <c r="F14" s="123"/>
-      <c r="G14" s="125"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="121"/>
+      <c r="F14" s="121"/>
+      <c r="G14" s="123"/>
       <c r="H14" s="87"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4869,10 +4966,10 @@
       <c r="C15" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="125"/>
-      <c r="E15" s="123"/>
-      <c r="F15" s="123"/>
-      <c r="G15" s="125"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="123"/>
       <c r="H15" s="87"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4885,10 +4982,10 @@
       <c r="C16" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="125"/>
-      <c r="E16" s="123"/>
-      <c r="F16" s="123"/>
-      <c r="G16" s="125"/>
+      <c r="D16" s="123"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="123"/>
       <c r="H16" s="87"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -4901,10 +4998,10 @@
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="125"/>
-      <c r="E17" s="123"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="125"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="121"/>
+      <c r="F17" s="121"/>
+      <c r="G17" s="123"/>
       <c r="H17" s="87"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -4920,9 +5017,9 @@
       <c r="D18" s="83" t="s">
         <v>219</v>
       </c>
-      <c r="E18" s="123"/>
-      <c r="F18" s="123"/>
-      <c r="G18" s="125"/>
+      <c r="E18" s="121"/>
+      <c r="F18" s="121"/>
+      <c r="G18" s="123"/>
       <c r="H18" s="87"/>
     </row>
     <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -4935,19 +5032,19 @@
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="125" t="s">
+      <c r="D19" s="123" t="s">
         <v>220</v>
       </c>
-      <c r="E19" s="123" t="s">
+      <c r="E19" s="121" t="s">
         <v>197</v>
       </c>
-      <c r="F19" s="123" t="s">
+      <c r="F19" s="121" t="s">
         <v>169</v>
       </c>
-      <c r="G19" s="125" t="s">
+      <c r="G19" s="123" t="s">
         <v>235</v>
       </c>
-      <c r="H19" s="126" t="s">
+      <c r="H19" s="125" t="s">
         <v>234</v>
       </c>
     </row>
@@ -4961,11 +5058,11 @@
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="125"/>
-      <c r="E20" s="123"/>
-      <c r="F20" s="123"/>
-      <c r="G20" s="125"/>
-      <c r="H20" s="126"/>
+      <c r="D20" s="123"/>
+      <c r="E20" s="121"/>
+      <c r="F20" s="121"/>
+      <c r="G20" s="123"/>
+      <c r="H20" s="125"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
@@ -4977,16 +5074,16 @@
       <c r="C21" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="125" t="s">
+      <c r="D21" s="123" t="s">
         <v>221</v>
       </c>
-      <c r="E21" s="123" t="s">
+      <c r="E21" s="121" t="s">
         <v>172</v>
       </c>
-      <c r="F21" s="124" t="s">
+      <c r="F21" s="122" t="s">
         <v>173</v>
       </c>
-      <c r="G21" s="128"/>
+      <c r="G21" s="126"/>
       <c r="H21" s="87"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -4999,10 +5096,10 @@
       <c r="C22" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="125"/>
-      <c r="E22" s="123"/>
-      <c r="F22" s="124"/>
-      <c r="G22" s="128"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="121"/>
+      <c r="F22" s="122"/>
+      <c r="G22" s="126"/>
       <c r="H22" s="87"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -5015,10 +5112,10 @@
       <c r="C23" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="125"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="124"/>
-      <c r="G23" s="128"/>
+      <c r="D23" s="123"/>
+      <c r="E23" s="121"/>
+      <c r="F23" s="122"/>
+      <c r="G23" s="126"/>
       <c r="H23" s="87"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -5031,10 +5128,10 @@
       <c r="C24" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="125"/>
-      <c r="E24" s="123"/>
-      <c r="F24" s="124"/>
-      <c r="G24" s="128"/>
+      <c r="D24" s="123"/>
+      <c r="E24" s="121"/>
+      <c r="F24" s="122"/>
+      <c r="G24" s="126"/>
       <c r="H24" s="87"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -5047,10 +5144,10 @@
       <c r="C25" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="125"/>
-      <c r="E25" s="123"/>
-      <c r="F25" s="124"/>
-      <c r="G25" s="128"/>
+      <c r="D25" s="123"/>
+      <c r="E25" s="121"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="126"/>
       <c r="H25" s="87"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -5063,10 +5160,10 @@
       <c r="C26" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="125"/>
-      <c r="E26" s="123"/>
-      <c r="F26" s="124"/>
-      <c r="G26" s="128"/>
+      <c r="D26" s="123"/>
+      <c r="E26" s="121"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="126"/>
       <c r="H26" s="87"/>
     </row>
     <row r="27" spans="1:8" ht="374.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5105,19 +5202,19 @@
       <c r="C28" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="125" t="s">
+      <c r="D28" s="123" t="s">
         <v>224</v>
       </c>
-      <c r="E28" s="123" t="s">
+      <c r="E28" s="121" t="s">
         <v>229</v>
       </c>
-      <c r="F28" s="124" t="s">
+      <c r="F28" s="122" t="s">
         <v>178</v>
       </c>
-      <c r="G28" s="128" t="s">
+      <c r="G28" s="126" t="s">
         <v>243</v>
       </c>
-      <c r="H28" s="127" t="s">
+      <c r="H28" s="124" t="s">
         <v>242</v>
       </c>
     </row>
@@ -5131,11 +5228,11 @@
       <c r="C29" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="128"/>
-      <c r="E29" s="123"/>
-      <c r="F29" s="124"/>
-      <c r="G29" s="128"/>
-      <c r="H29" s="127"/>
+      <c r="D29" s="126"/>
+      <c r="E29" s="121"/>
+      <c r="F29" s="122"/>
+      <c r="G29" s="126"/>
+      <c r="H29" s="124"/>
     </row>
     <row r="30" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="74" t="s">
@@ -5147,11 +5244,11 @@
       <c r="C30" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="128"/>
-      <c r="E30" s="123"/>
-      <c r="F30" s="124"/>
-      <c r="G30" s="128"/>
-      <c r="H30" s="127"/>
+      <c r="D30" s="126"/>
+      <c r="E30" s="121"/>
+      <c r="F30" s="122"/>
+      <c r="G30" s="126"/>
+      <c r="H30" s="124"/>
     </row>
     <row r="31" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="80" t="s">
@@ -5163,17 +5260,17 @@
       <c r="C31" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="125" t="s">
+      <c r="D31" s="123" t="s">
         <v>179</v>
       </c>
-      <c r="E31" s="123" t="s">
+      <c r="E31" s="121" t="s">
         <v>180</v>
       </c>
-      <c r="F31" s="123" t="s">
+      <c r="F31" s="121" t="s">
         <v>181</v>
       </c>
-      <c r="G31" s="125"/>
-      <c r="H31" s="127"/>
+      <c r="G31" s="123"/>
+      <c r="H31" s="124"/>
     </row>
     <row r="32" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="80" t="s">
@@ -5185,11 +5282,11 @@
       <c r="C32" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="125"/>
-      <c r="E32" s="123"/>
-      <c r="F32" s="123"/>
-      <c r="G32" s="125"/>
-      <c r="H32" s="127"/>
+      <c r="D32" s="123"/>
+      <c r="E32" s="121"/>
+      <c r="F32" s="121"/>
+      <c r="G32" s="123"/>
+      <c r="H32" s="124"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="81" t="s">
@@ -5249,19 +5346,19 @@
       <c r="C35" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="125" t="s">
+      <c r="D35" s="123" t="s">
         <v>231</v>
       </c>
-      <c r="E35" s="123" t="s">
+      <c r="E35" s="121" t="s">
         <v>188</v>
       </c>
-      <c r="F35" s="123" t="s">
+      <c r="F35" s="121" t="s">
         <v>144</v>
       </c>
-      <c r="G35" s="125" t="s">
+      <c r="G35" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="H35" s="126" t="s">
+      <c r="H35" s="125" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5275,11 +5372,11 @@
       <c r="C36" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D36" s="125"/>
-      <c r="E36" s="123"/>
-      <c r="F36" s="123"/>
-      <c r="G36" s="125"/>
-      <c r="H36" s="126"/>
+      <c r="D36" s="123"/>
+      <c r="E36" s="121"/>
+      <c r="F36" s="121"/>
+      <c r="G36" s="123"/>
+      <c r="H36" s="125"/>
     </row>
     <row r="37" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A37" s="78" t="s">
@@ -5291,11 +5388,11 @@
       <c r="C37" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D37" s="125"/>
-      <c r="E37" s="123"/>
-      <c r="F37" s="123"/>
-      <c r="G37" s="125"/>
-      <c r="H37" s="126"/>
+      <c r="D37" s="123"/>
+      <c r="E37" s="121"/>
+      <c r="F37" s="121"/>
+      <c r="G37" s="123"/>
+      <c r="H37" s="125"/>
     </row>
     <row r="38" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="78" t="s">
@@ -5307,19 +5404,19 @@
       <c r="C38" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D38" s="125" t="s">
+      <c r="D38" s="123" t="s">
         <v>226</v>
       </c>
-      <c r="E38" s="123" t="s">
+      <c r="E38" s="121" t="s">
         <v>190</v>
       </c>
-      <c r="F38" s="123" t="s">
+      <c r="F38" s="121" t="s">
         <v>244</v>
       </c>
-      <c r="G38" s="125" t="s">
+      <c r="G38" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="H38" s="127" t="s">
+      <c r="H38" s="124" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5333,11 +5430,11 @@
       <c r="C39" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="125"/>
-      <c r="E39" s="123"/>
-      <c r="F39" s="123"/>
-      <c r="G39" s="125"/>
-      <c r="H39" s="127"/>
+      <c r="D39" s="123"/>
+      <c r="E39" s="121"/>
+      <c r="F39" s="121"/>
+      <c r="G39" s="123"/>
+      <c r="H39" s="124"/>
     </row>
     <row r="40" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A40" s="78" t="s">
@@ -5349,11 +5446,11 @@
       <c r="C40" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D40" s="125"/>
-      <c r="E40" s="123"/>
-      <c r="F40" s="123"/>
-      <c r="G40" s="125"/>
-      <c r="H40" s="127"/>
+      <c r="D40" s="123"/>
+      <c r="E40" s="121"/>
+      <c r="F40" s="121"/>
+      <c r="G40" s="123"/>
+      <c r="H40" s="124"/>
     </row>
     <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A41" s="78" t="s">
@@ -5365,11 +5462,11 @@
       <c r="C41" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="125"/>
-      <c r="E41" s="123"/>
-      <c r="F41" s="123"/>
-      <c r="G41" s="125"/>
-      <c r="H41" s="127"/>
+      <c r="D41" s="123"/>
+      <c r="E41" s="121"/>
+      <c r="F41" s="121"/>
+      <c r="G41" s="123"/>
+      <c r="H41" s="124"/>
     </row>
     <row r="42" spans="1:8" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="78" t="s">
@@ -5381,11 +5478,11 @@
       <c r="C42" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="125"/>
-      <c r="E42" s="123"/>
-      <c r="F42" s="123"/>
-      <c r="G42" s="125"/>
-      <c r="H42" s="127"/>
+      <c r="D42" s="123"/>
+      <c r="E42" s="121"/>
+      <c r="F42" s="121"/>
+      <c r="G42" s="123"/>
+      <c r="H42" s="124"/>
     </row>
     <row r="43" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A43" s="78" t="s">
@@ -5397,11 +5494,11 @@
       <c r="C43" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="125"/>
-      <c r="E43" s="123"/>
-      <c r="F43" s="123"/>
-      <c r="G43" s="125"/>
-      <c r="H43" s="127"/>
+      <c r="D43" s="123"/>
+      <c r="E43" s="121"/>
+      <c r="F43" s="121"/>
+      <c r="G43" s="123"/>
+      <c r="H43" s="124"/>
     </row>
     <row r="44" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A44" s="78" t="s">
@@ -5413,11 +5510,11 @@
       <c r="C44" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D44" s="125"/>
-      <c r="E44" s="123"/>
-      <c r="F44" s="123"/>
-      <c r="G44" s="125"/>
-      <c r="H44" s="127"/>
+      <c r="D44" s="123"/>
+      <c r="E44" s="121"/>
+      <c r="F44" s="121"/>
+      <c r="G44" s="123"/>
+      <c r="H44" s="124"/>
     </row>
     <row r="45" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A45" s="78" t="s">
@@ -5429,11 +5526,11 @@
       <c r="C45" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="125"/>
-      <c r="E45" s="123"/>
-      <c r="F45" s="123"/>
-      <c r="G45" s="125"/>
-      <c r="H45" s="127"/>
+      <c r="D45" s="123"/>
+      <c r="E45" s="121"/>
+      <c r="F45" s="121"/>
+      <c r="G45" s="123"/>
+      <c r="H45" s="124"/>
     </row>
     <row r="46" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A46" s="78" t="s">
@@ -5445,11 +5542,11 @@
       <c r="C46" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D46" s="125"/>
-      <c r="E46" s="123"/>
-      <c r="F46" s="123"/>
-      <c r="G46" s="125"/>
-      <c r="H46" s="127"/>
+      <c r="D46" s="123"/>
+      <c r="E46" s="121"/>
+      <c r="F46" s="121"/>
+      <c r="G46" s="123"/>
+      <c r="H46" s="124"/>
     </row>
     <row r="47" spans="1:8" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="78" t="s">
@@ -5461,11 +5558,11 @@
       <c r="C47" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D47" s="125"/>
-      <c r="E47" s="123"/>
-      <c r="F47" s="123"/>
-      <c r="G47" s="125"/>
-      <c r="H47" s="127"/>
+      <c r="D47" s="123"/>
+      <c r="E47" s="121"/>
+      <c r="F47" s="121"/>
+      <c r="G47" s="123"/>
+      <c r="H47" s="124"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="78" t="s">
@@ -5477,19 +5574,19 @@
       <c r="C48" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D48" s="125" t="s">
+      <c r="D48" s="123" t="s">
         <v>227</v>
       </c>
-      <c r="E48" s="123" t="s">
+      <c r="E48" s="121" t="s">
         <v>192</v>
       </c>
-      <c r="F48" s="123" t="s">
+      <c r="F48" s="121" t="s">
         <v>144</v>
       </c>
-      <c r="G48" s="125" t="s">
+      <c r="G48" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="H48" s="127" t="s">
+      <c r="H48" s="124" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5503,11 +5600,11 @@
       <c r="C49" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D49" s="125"/>
-      <c r="E49" s="123"/>
-      <c r="F49" s="123"/>
-      <c r="G49" s="125"/>
-      <c r="H49" s="127"/>
+      <c r="D49" s="123"/>
+      <c r="E49" s="121"/>
+      <c r="F49" s="121"/>
+      <c r="G49" s="123"/>
+      <c r="H49" s="124"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="78" t="s">
@@ -5519,11 +5616,11 @@
       <c r="C50" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D50" s="125"/>
-      <c r="E50" s="123"/>
-      <c r="F50" s="123"/>
-      <c r="G50" s="125"/>
-      <c r="H50" s="127"/>
+      <c r="D50" s="123"/>
+      <c r="E50" s="121"/>
+      <c r="F50" s="121"/>
+      <c r="G50" s="123"/>
+      <c r="H50" s="124"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="78" t="s">
@@ -5535,29 +5632,25 @@
       <c r="C51" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D51" s="125"/>
-      <c r="E51" s="123"/>
-      <c r="F51" s="123"/>
-      <c r="G51" s="125"/>
-      <c r="H51" s="127"/>
+      <c r="D51" s="123"/>
+      <c r="E51" s="121"/>
+      <c r="F51" s="121"/>
+      <c r="G51" s="123"/>
+      <c r="H51" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="F48:F51"/>
-    <mergeCell ref="G48:G51"/>
-    <mergeCell ref="H48:H51"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="D38:D47"/>
-    <mergeCell ref="E38:E47"/>
-    <mergeCell ref="F38:F47"/>
-    <mergeCell ref="G38:G47"/>
-    <mergeCell ref="H38:H47"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E18"/>
+    <mergeCell ref="F4:F18"/>
+    <mergeCell ref="G4:G18"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D17"/>
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="H28:H30"/>
     <mergeCell ref="D31:D32"/>
@@ -5574,17 +5667,21 @@
     <mergeCell ref="F21:F26"/>
     <mergeCell ref="G21:G26"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E18"/>
-    <mergeCell ref="F4:F18"/>
-    <mergeCell ref="G4:G18"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="D38:D47"/>
+    <mergeCell ref="E38:E47"/>
+    <mergeCell ref="F38:F47"/>
+    <mergeCell ref="G38:G47"/>
+    <mergeCell ref="H38:H47"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="F48:F51"/>
+    <mergeCell ref="G48:G51"/>
+    <mergeCell ref="H48:H51"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C33" location="_ftn2" display="_ftn2" xr:uid="{E50DF5A1-13E6-4004-9692-0F820274B734}"/>
@@ -5595,19 +5692,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE037D9D-4E45-4C5B-8392-AE943DD18A55}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE037D9D-4E45-4C5B-8392-AE943DD18A55}">
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" style="88" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" style="88" customWidth="1"/>
-    <col min="3" max="3" width="57.140625" style="92" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="88" customWidth="1"/>
+    <col min="3" max="3" width="61.42578125" style="92" customWidth="1"/>
+    <col min="4" max="4" width="22" style="88" customWidth="1"/>
     <col min="5" max="16384" width="29.7109375" style="88"/>
   </cols>
   <sheetData>
@@ -5629,11 +5729,11 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="127" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="106" t="s">
-        <v>319</v>
+      <c r="B2" s="103" t="s">
+        <v>306</v>
       </c>
       <c r="C2" s="94" t="s">
         <v>273</v>
@@ -5649,9 +5749,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="130"/>
-      <c r="B3" s="107" t="s">
-        <v>320</v>
+      <c r="A3" s="128"/>
+      <c r="B3" s="104" t="s">
+        <v>307</v>
       </c>
       <c r="C3" s="94" t="s">
         <v>249</v>
@@ -5664,9 +5764,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="131"/>
-      <c r="B4" s="107" t="s">
-        <v>321</v>
+      <c r="A4" s="129"/>
+      <c r="B4" s="104" t="s">
+        <v>308</v>
       </c>
       <c r="C4" s="94" t="s">
         <v>288</v>
@@ -5680,11 +5780,11 @@
       <c r="F4" s="100"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="129" t="s">
+      <c r="A5" s="127" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="107" t="s">
-        <v>322</v>
+      <c r="B5" s="104" t="s">
+        <v>309</v>
       </c>
       <c r="C5" s="94" t="s">
         <v>250</v>
@@ -5700,9 +5800,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="131"/>
-      <c r="B6" s="107" t="s">
-        <v>323</v>
+      <c r="A6" s="129"/>
+      <c r="B6" s="104" t="s">
+        <v>310</v>
       </c>
       <c r="C6" s="94" t="s">
         <v>251</v>
@@ -5718,11 +5818,11 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="132" t="s">
+      <c r="A7" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="108" t="s">
-        <v>335</v>
+      <c r="B7" s="105" t="s">
+        <v>322</v>
       </c>
       <c r="C7" s="94" t="s">
         <v>252</v>
@@ -5736,9 +5836,9 @@
       <c r="F7" s="101"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="133"/>
-      <c r="B8" s="108" t="s">
-        <v>336</v>
+      <c r="A8" s="131"/>
+      <c r="B8" s="105" t="s">
+        <v>323</v>
       </c>
       <c r="C8" s="94" t="s">
         <v>253</v>
@@ -5751,9 +5851,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="133"/>
-      <c r="B9" s="108" t="s">
-        <v>337</v>
+      <c r="A9" s="131"/>
+      <c r="B9" s="105" t="s">
+        <v>324</v>
       </c>
       <c r="C9" s="94" t="s">
         <v>254</v>
@@ -5766,9 +5866,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="133"/>
-      <c r="B10" s="108" t="s">
-        <v>338</v>
+      <c r="A10" s="131"/>
+      <c r="B10" s="105" t="s">
+        <v>325</v>
       </c>
       <c r="C10" s="94" t="s">
         <v>289</v>
@@ -5782,70 +5882,70 @@
       <c r="F10" s="100"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="133"/>
-      <c r="B11" s="142" t="s">
+      <c r="A11" s="131"/>
+      <c r="B11" s="106" t="s">
+        <v>331</v>
+      </c>
+      <c r="C11" s="94" t="s">
+        <v>255</v>
+      </c>
+      <c r="D11" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="96" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+      <c r="A12" s="131"/>
+      <c r="B12" s="106" t="s">
         <v>292</v>
       </c>
-      <c r="C11" s="139" t="s">
-        <v>255</v>
-      </c>
-      <c r="D11" s="140" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="141" t="s">
+      <c r="C12" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="D12" s="95" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" s="96" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.25">
-      <c r="A12" s="133"/>
-      <c r="B12" s="107" t="s">
+    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="131"/>
+      <c r="B13" s="106" t="s">
+        <v>333</v>
+      </c>
+      <c r="C13" s="94" t="s">
+        <v>274</v>
+      </c>
+      <c r="D13" s="95" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="96" t="s">
+        <v>283</v>
+      </c>
+      <c r="F13" s="100"/>
+    </row>
+    <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="131"/>
+      <c r="B14" s="106" t="s">
+        <v>332</v>
+      </c>
+      <c r="C14" s="94" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" s="95" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="96" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="131"/>
+      <c r="B15" s="104" t="s">
         <v>293</v>
-      </c>
-      <c r="C12" s="103" t="s">
-        <v>285</v>
-      </c>
-      <c r="D12" s="104" t="s">
-        <v>119</v>
-      </c>
-      <c r="E12" s="105" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="133"/>
-      <c r="B13" s="107" t="s">
-        <v>294</v>
-      </c>
-      <c r="C13" s="90" t="s">
-        <v>274</v>
-      </c>
-      <c r="D13" s="89" t="s">
-        <v>119</v>
-      </c>
-      <c r="E13" s="93" t="s">
-        <v>283</v>
-      </c>
-      <c r="F13" s="100"/>
-    </row>
-    <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="133"/>
-      <c r="B14" s="107" t="s">
-        <v>295</v>
-      </c>
-      <c r="C14" s="90" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" s="89" t="s">
-        <v>119</v>
-      </c>
-      <c r="E14" s="93" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="133"/>
-      <c r="B15" s="107" t="s">
-        <v>296</v>
       </c>
       <c r="C15" s="91" t="s">
         <v>127</v>
@@ -5857,145 +5957,145 @@
         <v>284</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="133"/>
-      <c r="B16" s="107" t="s">
-        <v>297</v>
-      </c>
-      <c r="C16" s="90" t="s">
+    <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="131"/>
+      <c r="B16" s="106" t="s">
+        <v>330</v>
+      </c>
+      <c r="C16" s="94" t="s">
         <v>139</v>
       </c>
-      <c r="D16" s="89" t="s">
+      <c r="D16" s="95" t="s">
         <v>246</v>
       </c>
-      <c r="E16" s="93" t="s">
+      <c r="E16" s="96" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="133"/>
-      <c r="B17" s="107" t="s">
-        <v>298</v>
-      </c>
-      <c r="C17" s="90" t="s">
+      <c r="A17" s="131"/>
+      <c r="B17" s="106" t="s">
+        <v>334</v>
+      </c>
+      <c r="C17" s="94" t="s">
         <v>286</v>
       </c>
-      <c r="D17" s="89" t="s">
+      <c r="D17" s="95" t="s">
         <v>246</v>
       </c>
-      <c r="E17" s="93" t="s">
+      <c r="E17" s="96" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="133"/>
-      <c r="B18" s="107" t="s">
-        <v>299</v>
-      </c>
-      <c r="C18" s="90" t="s">
+      <c r="A18" s="131"/>
+      <c r="B18" s="106" t="s">
+        <v>335</v>
+      </c>
+      <c r="C18" s="94" t="s">
         <v>276</v>
       </c>
-      <c r="D18" s="89" t="s">
+      <c r="D18" s="95" t="s">
         <v>246</v>
       </c>
-      <c r="E18" s="93" t="s">
+      <c r="E18" s="96" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A19" s="133"/>
-      <c r="B19" s="107" t="s">
-        <v>300</v>
-      </c>
-      <c r="C19" s="90" t="s">
+      <c r="A19" s="131"/>
+      <c r="B19" s="106" t="s">
+        <v>336</v>
+      </c>
+      <c r="C19" s="94" t="s">
         <v>277</v>
       </c>
-      <c r="D19" s="89" t="s">
+      <c r="D19" s="95" t="s">
         <v>246</v>
       </c>
-      <c r="E19" s="93" t="s">
+      <c r="E19" s="96" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A20" s="133"/>
-      <c r="B20" s="107" t="s">
-        <v>301</v>
-      </c>
-      <c r="C20" s="90" t="s">
+      <c r="A20" s="131"/>
+      <c r="B20" s="106" t="s">
+        <v>327</v>
+      </c>
+      <c r="C20" s="94" t="s">
         <v>279</v>
       </c>
-      <c r="D20" s="89" t="s">
+      <c r="D20" s="95" t="s">
         <v>246</v>
       </c>
-      <c r="E20" s="93" t="s">
+      <c r="E20" s="96" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A21" s="133"/>
-      <c r="B21" s="107" t="s">
-        <v>302</v>
-      </c>
-      <c r="C21" s="90" t="s">
+      <c r="A21" s="131"/>
+      <c r="B21" s="106" t="s">
+        <v>328</v>
+      </c>
+      <c r="C21" s="94" t="s">
         <v>275</v>
       </c>
-      <c r="D21" s="89" t="s">
+      <c r="D21" s="95" t="s">
         <v>246</v>
       </c>
-      <c r="E21" s="93" t="s">
+      <c r="E21" s="96" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="133"/>
-      <c r="B22" s="107" t="s">
-        <v>303</v>
-      </c>
-      <c r="C22" s="90" t="s">
+      <c r="A22" s="131"/>
+      <c r="B22" s="106" t="s">
+        <v>329</v>
+      </c>
+      <c r="C22" s="94" t="s">
         <v>278</v>
       </c>
-      <c r="D22" s="89" t="s">
+      <c r="D22" s="95" t="s">
         <v>246</v>
       </c>
-      <c r="E22" s="93" t="s">
+      <c r="E22" s="96" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="133"/>
-      <c r="B23" s="107" t="s">
-        <v>304</v>
-      </c>
-      <c r="C23" s="90" t="s">
+      <c r="A23" s="131"/>
+      <c r="B23" s="106" t="s">
+        <v>337</v>
+      </c>
+      <c r="C23" s="94" t="s">
         <v>280</v>
       </c>
-      <c r="D23" s="89" t="s">
+      <c r="D23" s="95" t="s">
         <v>246</v>
       </c>
-      <c r="E23" s="93" t="s">
+      <c r="E23" s="96" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="133"/>
-      <c r="B24" s="107" t="s">
-        <v>305</v>
-      </c>
-      <c r="C24" s="90" t="s">
+      <c r="A24" s="131"/>
+      <c r="B24" s="104" t="s">
+        <v>338</v>
+      </c>
+      <c r="C24" s="94" t="s">
         <v>272</v>
       </c>
-      <c r="D24" s="89" t="s">
+      <c r="D24" s="95" t="s">
         <v>246</v>
       </c>
-      <c r="E24" s="93" t="s">
+      <c r="E24" s="96" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="133"/>
-      <c r="B25" s="107" t="s">
-        <v>306</v>
+      <c r="A25" s="131"/>
+      <c r="B25" s="104" t="s">
+        <v>294</v>
       </c>
       <c r="C25" s="90" t="s">
         <v>281</v>
@@ -6008,9 +6108,9 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="133"/>
-      <c r="B26" s="107" t="s">
-        <v>307</v>
+      <c r="A26" s="131"/>
+      <c r="B26" s="104" t="s">
+        <v>295</v>
       </c>
       <c r="C26" s="90" t="s">
         <v>256</v>
@@ -6023,9 +6123,9 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="133"/>
-      <c r="B27" s="107" t="s">
-        <v>308</v>
+      <c r="A27" s="131"/>
+      <c r="B27" s="104" t="s">
+        <v>296</v>
       </c>
       <c r="C27" s="90" t="s">
         <v>257</v>
@@ -6038,9 +6138,9 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="134"/>
-      <c r="B28" s="107" t="s">
-        <v>309</v>
+      <c r="A28" s="132"/>
+      <c r="B28" s="104" t="s">
+        <v>297</v>
       </c>
       <c r="C28" s="90" t="s">
         <v>258</v>
@@ -6053,11 +6153,11 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="132" t="s">
+      <c r="A29" s="130" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="107" t="s">
-        <v>310</v>
+      <c r="B29" s="104" t="s">
+        <v>298</v>
       </c>
       <c r="C29" s="90" t="s">
         <v>259</v>
@@ -6070,9 +6170,9 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="133"/>
-      <c r="B30" s="107" t="s">
-        <v>311</v>
+      <c r="A30" s="131"/>
+      <c r="B30" s="104" t="s">
+        <v>299</v>
       </c>
       <c r="C30" s="90" t="s">
         <v>260</v>
@@ -6085,9 +6185,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="133"/>
-      <c r="B31" s="107" t="s">
-        <v>312</v>
+      <c r="A31" s="131"/>
+      <c r="B31" s="104" t="s">
+        <v>300</v>
       </c>
       <c r="C31" s="90" t="s">
         <v>261</v>
@@ -6100,9 +6200,9 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="133"/>
-      <c r="B32" s="107" t="s">
-        <v>313</v>
+      <c r="A32" s="131"/>
+      <c r="B32" s="104" t="s">
+        <v>301</v>
       </c>
       <c r="C32" s="90" t="s">
         <v>262</v>
@@ -6115,9 +6215,9 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="133"/>
-      <c r="B33" s="107" t="s">
-        <v>314</v>
+      <c r="A33" s="131"/>
+      <c r="B33" s="104" t="s">
+        <v>302</v>
       </c>
       <c r="C33" s="90" t="s">
         <v>263</v>
@@ -6130,9 +6230,9 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="134"/>
-      <c r="B34" s="107" t="s">
-        <v>315</v>
+      <c r="A34" s="132"/>
+      <c r="B34" s="104" t="s">
+        <v>303</v>
       </c>
       <c r="C34" s="90" t="s">
         <v>264</v>
@@ -6145,11 +6245,11 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="129" t="s">
+      <c r="A35" s="127" t="s">
         <v>287</v>
       </c>
-      <c r="B35" s="107" t="s">
-        <v>324</v>
+      <c r="B35" s="104" t="s">
+        <v>311</v>
       </c>
       <c r="C35" s="97" t="s">
         <v>265</v>
@@ -6162,9 +6262,9 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="131"/>
-      <c r="B36" s="107" t="s">
-        <v>325</v>
+      <c r="A36" s="129"/>
+      <c r="B36" s="104" t="s">
+        <v>312</v>
       </c>
       <c r="C36" s="97" t="s">
         <v>266</v>
@@ -6177,11 +6277,11 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="129" t="s">
+      <c r="A37" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="107" t="s">
-        <v>326</v>
+      <c r="B37" s="104" t="s">
+        <v>313</v>
       </c>
       <c r="C37" s="97" t="s">
         <v>267</v>
@@ -6194,9 +6294,9 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="131"/>
-      <c r="B38" s="107" t="s">
-        <v>327</v>
+      <c r="A38" s="129"/>
+      <c r="B38" s="104" t="s">
+        <v>314</v>
       </c>
       <c r="C38" s="97" t="s">
         <v>268</v>
@@ -6209,11 +6309,11 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="129" t="s">
+      <c r="A39" s="127" t="s">
         <v>199</v>
       </c>
-      <c r="B39" s="107" t="s">
-        <v>328</v>
+      <c r="B39" s="104" t="s">
+        <v>315</v>
       </c>
       <c r="C39" s="97" t="s">
         <v>269</v>
@@ -6226,9 +6326,9 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="130"/>
-      <c r="B40" s="107" t="s">
-        <v>329</v>
+      <c r="A40" s="128"/>
+      <c r="B40" s="104" t="s">
+        <v>316</v>
       </c>
       <c r="C40" s="97" t="s">
         <v>270</v>
@@ -6241,9 +6341,9 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="130"/>
-      <c r="B41" s="107" t="s">
-        <v>330</v>
+      <c r="A41" s="128"/>
+      <c r="B41" s="104" t="s">
+        <v>317</v>
       </c>
       <c r="C41" s="97" t="s">
         <v>271</v>
@@ -6256,9 +6356,9 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="131"/>
-      <c r="B42" s="107" t="s">
-        <v>331</v>
+      <c r="A42" s="129"/>
+      <c r="B42" s="104" t="s">
+        <v>318</v>
       </c>
       <c r="C42" s="97" t="s">
         <v>245</v>
@@ -6271,26 +6371,26 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="132" t="s">
+      <c r="A43" s="130" t="s">
         <v>198</v>
       </c>
-      <c r="B43" s="142" t="s">
-        <v>316</v>
-      </c>
-      <c r="C43" s="139" t="s">
+      <c r="B43" s="106" t="s">
+        <v>326</v>
+      </c>
+      <c r="C43" s="97" t="s">
         <v>248</v>
       </c>
-      <c r="D43" s="140" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" s="141" t="s">
+      <c r="D43" s="98" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="99" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="133"/>
-      <c r="B44" s="107" t="s">
-        <v>334</v>
+      <c r="A44" s="131"/>
+      <c r="B44" s="104" t="s">
+        <v>321</v>
       </c>
       <c r="C44" s="97" t="s">
         <v>86</v>
@@ -6306,9 +6406,9 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="133"/>
-      <c r="B45" s="107" t="s">
-        <v>332</v>
+      <c r="A45" s="131"/>
+      <c r="B45" s="104" t="s">
+        <v>319</v>
       </c>
       <c r="C45" s="97" t="s">
         <v>87</v>
@@ -6324,9 +6424,9 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="134"/>
-      <c r="B46" s="107" t="s">
-        <v>333</v>
+      <c r="A46" s="132"/>
+      <c r="B46" s="104" t="s">
+        <v>320</v>
       </c>
       <c r="C46" s="97" t="s">
         <v>100</v>
@@ -6342,11 +6442,11 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="132" t="s">
+      <c r="A47" s="130" t="s">
         <v>151</v>
       </c>
-      <c r="B47" s="107" t="s">
-        <v>317</v>
+      <c r="B47" s="104" t="s">
+        <v>304</v>
       </c>
       <c r="C47" s="90" t="s">
         <v>209</v>
@@ -6359,9 +6459,9 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="134"/>
-      <c r="B48" s="107" t="s">
-        <v>318</v>
+      <c r="A48" s="132"/>
+      <c r="B48" s="104" t="s">
+        <v>305</v>
       </c>
       <c r="C48" s="90" t="s">
         <v>247</v>
@@ -6387,6 +6487,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6472,16 +6573,16 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="125" t="s">
+      <c r="D4" s="123" t="s">
         <v>215</v>
       </c>
-      <c r="E4" s="123" t="s">
+      <c r="E4" s="121" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="123" t="s">
+      <c r="F4" s="121" t="s">
         <v>158</v>
       </c>
-      <c r="G4" s="125"/>
+      <c r="G4" s="123"/>
       <c r="H4" s="87"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6494,10 +6595,10 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="125"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="125"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="123"/>
       <c r="H5" s="87"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6510,12 +6611,12 @@
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="125" t="s">
+      <c r="D6" s="123" t="s">
         <v>216</v>
       </c>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="125"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="123"/>
       <c r="H6" s="87"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6528,10 +6629,10 @@
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="125"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="125"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="123"/>
       <c r="H7" s="87"/>
     </row>
     <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6544,12 +6645,12 @@
       <c r="C8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="125" t="s">
+      <c r="D8" s="123" t="s">
         <v>164</v>
       </c>
-      <c r="E8" s="123"/>
-      <c r="F8" s="123"/>
-      <c r="G8" s="125"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="121"/>
+      <c r="G8" s="123"/>
       <c r="H8" s="87"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6562,10 +6663,10 @@
       <c r="C9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="125"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="125"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="121"/>
+      <c r="G9" s="123"/>
       <c r="H9" s="87"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -6578,12 +6679,12 @@
       <c r="C10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="125" t="s">
+      <c r="D10" s="123" t="s">
         <v>217</v>
       </c>
-      <c r="E10" s="123"/>
-      <c r="F10" s="123"/>
-      <c r="G10" s="125"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="121"/>
+      <c r="G10" s="123"/>
       <c r="H10" s="87"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -6596,10 +6697,10 @@
       <c r="C11" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="125"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="123"/>
-      <c r="G11" s="125"/>
+      <c r="D11" s="123"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
+      <c r="G11" s="123"/>
       <c r="H11" s="87"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6612,10 +6713,10 @@
       <c r="C12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="125"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="125"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="121"/>
+      <c r="F12" s="121"/>
+      <c r="G12" s="123"/>
       <c r="H12" s="87"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6628,12 +6729,12 @@
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="125" t="s">
+      <c r="D13" s="123" t="s">
         <v>218</v>
       </c>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="125"/>
+      <c r="E13" s="121"/>
+      <c r="F13" s="121"/>
+      <c r="G13" s="123"/>
       <c r="H13" s="87"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -6646,10 +6747,10 @@
       <c r="C14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="125"/>
-      <c r="E14" s="123"/>
-      <c r="F14" s="123"/>
-      <c r="G14" s="125"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="121"/>
+      <c r="F14" s="121"/>
+      <c r="G14" s="123"/>
       <c r="H14" s="87"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6662,10 +6763,10 @@
       <c r="C15" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="125"/>
-      <c r="E15" s="123"/>
-      <c r="F15" s="123"/>
-      <c r="G15" s="125"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="123"/>
       <c r="H15" s="87"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -6678,10 +6779,10 @@
       <c r="C16" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="125"/>
-      <c r="E16" s="123"/>
-      <c r="F16" s="123"/>
-      <c r="G16" s="125"/>
+      <c r="D16" s="123"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="123"/>
       <c r="H16" s="87"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -6694,10 +6795,10 @@
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="125"/>
-      <c r="E17" s="123"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="125"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="121"/>
+      <c r="F17" s="121"/>
+      <c r="G17" s="123"/>
       <c r="H17" s="87"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -6713,9 +6814,9 @@
       <c r="D18" s="83" t="s">
         <v>219</v>
       </c>
-      <c r="E18" s="123"/>
-      <c r="F18" s="123"/>
-      <c r="G18" s="125"/>
+      <c r="E18" s="121"/>
+      <c r="F18" s="121"/>
+      <c r="G18" s="123"/>
       <c r="H18" s="87"/>
     </row>
     <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -6728,19 +6829,19 @@
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="125" t="s">
+      <c r="D19" s="123" t="s">
         <v>220</v>
       </c>
-      <c r="E19" s="123" t="s">
+      <c r="E19" s="121" t="s">
         <v>197</v>
       </c>
-      <c r="F19" s="123" t="s">
+      <c r="F19" s="121" t="s">
         <v>169</v>
       </c>
-      <c r="G19" s="125" t="s">
+      <c r="G19" s="123" t="s">
         <v>235</v>
       </c>
-      <c r="H19" s="126" t="s">
+      <c r="H19" s="125" t="s">
         <v>234</v>
       </c>
     </row>
@@ -6754,11 +6855,11 @@
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="125"/>
-      <c r="E20" s="123"/>
-      <c r="F20" s="123"/>
-      <c r="G20" s="125"/>
-      <c r="H20" s="126"/>
+      <c r="D20" s="123"/>
+      <c r="E20" s="121"/>
+      <c r="F20" s="121"/>
+      <c r="G20" s="123"/>
+      <c r="H20" s="125"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
@@ -6770,16 +6871,16 @@
       <c r="C21" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="125" t="s">
+      <c r="D21" s="123" t="s">
         <v>221</v>
       </c>
-      <c r="E21" s="123" t="s">
+      <c r="E21" s="121" t="s">
         <v>172</v>
       </c>
-      <c r="F21" s="124" t="s">
+      <c r="F21" s="122" t="s">
         <v>173</v>
       </c>
-      <c r="G21" s="128"/>
+      <c r="G21" s="126"/>
       <c r="H21" s="87"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -6792,10 +6893,10 @@
       <c r="C22" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="125"/>
-      <c r="E22" s="123"/>
-      <c r="F22" s="124"/>
-      <c r="G22" s="128"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="121"/>
+      <c r="F22" s="122"/>
+      <c r="G22" s="126"/>
       <c r="H22" s="87"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -6808,10 +6909,10 @@
       <c r="C23" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="125"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="124"/>
-      <c r="G23" s="128"/>
+      <c r="D23" s="123"/>
+      <c r="E23" s="121"/>
+      <c r="F23" s="122"/>
+      <c r="G23" s="126"/>
       <c r="H23" s="87"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -6824,10 +6925,10 @@
       <c r="C24" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="125"/>
-      <c r="E24" s="123"/>
-      <c r="F24" s="124"/>
-      <c r="G24" s="128"/>
+      <c r="D24" s="123"/>
+      <c r="E24" s="121"/>
+      <c r="F24" s="122"/>
+      <c r="G24" s="126"/>
       <c r="H24" s="87"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -6840,10 +6941,10 @@
       <c r="C25" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="125"/>
-      <c r="E25" s="123"/>
-      <c r="F25" s="124"/>
-      <c r="G25" s="128"/>
+      <c r="D25" s="123"/>
+      <c r="E25" s="121"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="126"/>
       <c r="H25" s="87"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -6856,10 +6957,10 @@
       <c r="C26" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="125"/>
-      <c r="E26" s="123"/>
-      <c r="F26" s="124"/>
-      <c r="G26" s="128"/>
+      <c r="D26" s="123"/>
+      <c r="E26" s="121"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="126"/>
       <c r="H26" s="87"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -6872,16 +6973,16 @@
       <c r="C27" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="125" t="s">
+      <c r="D27" s="123" t="s">
         <v>222</v>
       </c>
-      <c r="E27" s="123" t="s">
+      <c r="E27" s="121" t="s">
         <v>175</v>
       </c>
-      <c r="F27" s="123" t="s">
+      <c r="F27" s="121" t="s">
         <v>158</v>
       </c>
-      <c r="G27" s="125"/>
+      <c r="G27" s="123"/>
       <c r="H27" s="87"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -6894,10 +6995,10 @@
       <c r="C28" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="125"/>
-      <c r="E28" s="123"/>
-      <c r="F28" s="123"/>
-      <c r="G28" s="125"/>
+      <c r="D28" s="123"/>
+      <c r="E28" s="121"/>
+      <c r="F28" s="121"/>
+      <c r="G28" s="123"/>
       <c r="H28" s="87"/>
     </row>
     <row r="29" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -6910,10 +7011,10 @@
       <c r="C29" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D29" s="125"/>
-      <c r="E29" s="123"/>
-      <c r="F29" s="123"/>
-      <c r="G29" s="125"/>
+      <c r="D29" s="123"/>
+      <c r="E29" s="121"/>
+      <c r="F29" s="121"/>
+      <c r="G29" s="123"/>
       <c r="H29" s="87"/>
     </row>
     <row r="30" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -6926,10 +7027,10 @@
       <c r="C30" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="125"/>
-      <c r="E30" s="123"/>
-      <c r="F30" s="123"/>
-      <c r="G30" s="125"/>
+      <c r="D30" s="123"/>
+      <c r="E30" s="121"/>
+      <c r="F30" s="121"/>
+      <c r="G30" s="123"/>
       <c r="H30" s="87"/>
     </row>
     <row r="31" spans="1:8" ht="374.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6968,19 +7069,19 @@
       <c r="C32" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="125" t="s">
+      <c r="D32" s="123" t="s">
         <v>224</v>
       </c>
-      <c r="E32" s="123" t="s">
+      <c r="E32" s="121" t="s">
         <v>229</v>
       </c>
-      <c r="F32" s="124" t="s">
+      <c r="F32" s="122" t="s">
         <v>178</v>
       </c>
-      <c r="G32" s="128" t="s">
+      <c r="G32" s="126" t="s">
         <v>243</v>
       </c>
-      <c r="H32" s="127" t="s">
+      <c r="H32" s="124" t="s">
         <v>242</v>
       </c>
     </row>
@@ -6994,11 +7095,11 @@
       <c r="C33" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="128"/>
-      <c r="E33" s="123"/>
-      <c r="F33" s="124"/>
-      <c r="G33" s="128"/>
-      <c r="H33" s="127"/>
+      <c r="D33" s="126"/>
+      <c r="E33" s="121"/>
+      <c r="F33" s="122"/>
+      <c r="G33" s="126"/>
+      <c r="H33" s="124"/>
     </row>
     <row r="34" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="74" t="s">
@@ -7010,11 +7111,11 @@
       <c r="C34" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="128"/>
-      <c r="E34" s="123"/>
-      <c r="F34" s="124"/>
-      <c r="G34" s="128"/>
-      <c r="H34" s="127"/>
+      <c r="D34" s="126"/>
+      <c r="E34" s="121"/>
+      <c r="F34" s="122"/>
+      <c r="G34" s="126"/>
+      <c r="H34" s="124"/>
     </row>
     <row r="35" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="80" t="s">
@@ -7026,17 +7127,17 @@
       <c r="C35" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="125" t="s">
+      <c r="D35" s="123" t="s">
         <v>179</v>
       </c>
-      <c r="E35" s="123" t="s">
+      <c r="E35" s="121" t="s">
         <v>180</v>
       </c>
-      <c r="F35" s="123" t="s">
+      <c r="F35" s="121" t="s">
         <v>181</v>
       </c>
-      <c r="G35" s="125"/>
-      <c r="H35" s="127"/>
+      <c r="G35" s="123"/>
+      <c r="H35" s="124"/>
     </row>
     <row r="36" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="80" t="s">
@@ -7048,11 +7149,11 @@
       <c r="C36" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="125"/>
-      <c r="E36" s="123"/>
-      <c r="F36" s="123"/>
-      <c r="G36" s="125"/>
-      <c r="H36" s="127"/>
+      <c r="D36" s="123"/>
+      <c r="E36" s="121"/>
+      <c r="F36" s="121"/>
+      <c r="G36" s="123"/>
+      <c r="H36" s="124"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="81" t="s">
@@ -7112,19 +7213,19 @@
       <c r="C39" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D39" s="125" t="s">
+      <c r="D39" s="123" t="s">
         <v>231</v>
       </c>
-      <c r="E39" s="123" t="s">
+      <c r="E39" s="121" t="s">
         <v>188</v>
       </c>
-      <c r="F39" s="123" t="s">
+      <c r="F39" s="121" t="s">
         <v>144</v>
       </c>
-      <c r="G39" s="125" t="s">
+      <c r="G39" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="H39" s="126" t="s">
+      <c r="H39" s="125" t="s">
         <v>236</v>
       </c>
     </row>
@@ -7138,11 +7239,11 @@
       <c r="C40" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="125"/>
-      <c r="E40" s="123"/>
-      <c r="F40" s="123"/>
-      <c r="G40" s="125"/>
-      <c r="H40" s="126"/>
+      <c r="D40" s="123"/>
+      <c r="E40" s="121"/>
+      <c r="F40" s="121"/>
+      <c r="G40" s="123"/>
+      <c r="H40" s="125"/>
     </row>
     <row r="41" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A41" s="78" t="s">
@@ -7154,11 +7255,11 @@
       <c r="C41" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="125"/>
-      <c r="E41" s="123"/>
-      <c r="F41" s="123"/>
-      <c r="G41" s="125"/>
-      <c r="H41" s="126"/>
+      <c r="D41" s="123"/>
+      <c r="E41" s="121"/>
+      <c r="F41" s="121"/>
+      <c r="G41" s="123"/>
+      <c r="H41" s="125"/>
     </row>
     <row r="42" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="78" t="s">
@@ -7170,19 +7271,19 @@
       <c r="C42" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="125" t="s">
+      <c r="D42" s="123" t="s">
         <v>226</v>
       </c>
-      <c r="E42" s="123" t="s">
+      <c r="E42" s="121" t="s">
         <v>190</v>
       </c>
-      <c r="F42" s="123" t="s">
+      <c r="F42" s="121" t="s">
         <v>244</v>
       </c>
-      <c r="G42" s="125" t="s">
+      <c r="G42" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="H42" s="127" t="s">
+      <c r="H42" s="124" t="s">
         <v>236</v>
       </c>
     </row>
@@ -7196,11 +7297,11 @@
       <c r="C43" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="125"/>
-      <c r="E43" s="123"/>
-      <c r="F43" s="123"/>
-      <c r="G43" s="125"/>
-      <c r="H43" s="127"/>
+      <c r="D43" s="123"/>
+      <c r="E43" s="121"/>
+      <c r="F43" s="121"/>
+      <c r="G43" s="123"/>
+      <c r="H43" s="124"/>
     </row>
     <row r="44" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A44" s="78" t="s">
@@ -7212,11 +7313,11 @@
       <c r="C44" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D44" s="125"/>
-      <c r="E44" s="123"/>
-      <c r="F44" s="123"/>
-      <c r="G44" s="125"/>
-      <c r="H44" s="127"/>
+      <c r="D44" s="123"/>
+      <c r="E44" s="121"/>
+      <c r="F44" s="121"/>
+      <c r="G44" s="123"/>
+      <c r="H44" s="124"/>
     </row>
     <row r="45" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A45" s="78" t="s">
@@ -7228,11 +7329,11 @@
       <c r="C45" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="125"/>
-      <c r="E45" s="123"/>
-      <c r="F45" s="123"/>
-      <c r="G45" s="125"/>
-      <c r="H45" s="127"/>
+      <c r="D45" s="123"/>
+      <c r="E45" s="121"/>
+      <c r="F45" s="121"/>
+      <c r="G45" s="123"/>
+      <c r="H45" s="124"/>
     </row>
     <row r="46" spans="1:8" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="78" t="s">
@@ -7244,11 +7345,11 @@
       <c r="C46" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D46" s="125"/>
-      <c r="E46" s="123"/>
-      <c r="F46" s="123"/>
-      <c r="G46" s="125"/>
-      <c r="H46" s="127"/>
+      <c r="D46" s="123"/>
+      <c r="E46" s="121"/>
+      <c r="F46" s="121"/>
+      <c r="G46" s="123"/>
+      <c r="H46" s="124"/>
     </row>
     <row r="47" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A47" s="78" t="s">
@@ -7260,11 +7361,11 @@
       <c r="C47" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D47" s="125"/>
-      <c r="E47" s="123"/>
-      <c r="F47" s="123"/>
-      <c r="G47" s="125"/>
-      <c r="H47" s="127"/>
+      <c r="D47" s="123"/>
+      <c r="E47" s="121"/>
+      <c r="F47" s="121"/>
+      <c r="G47" s="123"/>
+      <c r="H47" s="124"/>
     </row>
     <row r="48" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A48" s="78" t="s">
@@ -7276,11 +7377,11 @@
       <c r="C48" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D48" s="125"/>
-      <c r="E48" s="123"/>
-      <c r="F48" s="123"/>
-      <c r="G48" s="125"/>
-      <c r="H48" s="127"/>
+      <c r="D48" s="123"/>
+      <c r="E48" s="121"/>
+      <c r="F48" s="121"/>
+      <c r="G48" s="123"/>
+      <c r="H48" s="124"/>
     </row>
     <row r="49" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" s="78" t="s">
@@ -7292,11 +7393,11 @@
       <c r="C49" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D49" s="125"/>
-      <c r="E49" s="123"/>
-      <c r="F49" s="123"/>
-      <c r="G49" s="125"/>
-      <c r="H49" s="127"/>
+      <c r="D49" s="123"/>
+      <c r="E49" s="121"/>
+      <c r="F49" s="121"/>
+      <c r="G49" s="123"/>
+      <c r="H49" s="124"/>
     </row>
     <row r="50" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A50" s="78" t="s">
@@ -7308,11 +7409,11 @@
       <c r="C50" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D50" s="125"/>
-      <c r="E50" s="123"/>
-      <c r="F50" s="123"/>
-      <c r="G50" s="125"/>
-      <c r="H50" s="127"/>
+      <c r="D50" s="123"/>
+      <c r="E50" s="121"/>
+      <c r="F50" s="121"/>
+      <c r="G50" s="123"/>
+      <c r="H50" s="124"/>
     </row>
     <row r="51" spans="1:8" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="78" t="s">
@@ -7324,11 +7425,11 @@
       <c r="C51" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D51" s="125"/>
-      <c r="E51" s="123"/>
-      <c r="F51" s="123"/>
-      <c r="G51" s="125"/>
-      <c r="H51" s="127"/>
+      <c r="D51" s="123"/>
+      <c r="E51" s="121"/>
+      <c r="F51" s="121"/>
+      <c r="G51" s="123"/>
+      <c r="H51" s="124"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="78" t="s">
@@ -7340,19 +7441,19 @@
       <c r="C52" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D52" s="125" t="s">
+      <c r="D52" s="123" t="s">
         <v>227</v>
       </c>
-      <c r="E52" s="123" t="s">
+      <c r="E52" s="121" t="s">
         <v>192</v>
       </c>
-      <c r="F52" s="123" t="s">
+      <c r="F52" s="121" t="s">
         <v>144</v>
       </c>
-      <c r="G52" s="125" t="s">
+      <c r="G52" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="H52" s="127" t="s">
+      <c r="H52" s="124" t="s">
         <v>236</v>
       </c>
     </row>
@@ -7366,11 +7467,11 @@
       <c r="C53" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D53" s="125"/>
-      <c r="E53" s="123"/>
-      <c r="F53" s="123"/>
-      <c r="G53" s="125"/>
-      <c r="H53" s="127"/>
+      <c r="D53" s="123"/>
+      <c r="E53" s="121"/>
+      <c r="F53" s="121"/>
+      <c r="G53" s="123"/>
+      <c r="H53" s="124"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="78" t="s">
@@ -7382,11 +7483,11 @@
       <c r="C54" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="125"/>
-      <c r="E54" s="123"/>
-      <c r="F54" s="123"/>
-      <c r="G54" s="125"/>
-      <c r="H54" s="127"/>
+      <c r="D54" s="123"/>
+      <c r="E54" s="121"/>
+      <c r="F54" s="121"/>
+      <c r="G54" s="123"/>
+      <c r="H54" s="124"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="78" t="s">
@@ -7398,14 +7499,50 @@
       <c r="C55" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D55" s="125"/>
-      <c r="E55" s="123"/>
-      <c r="F55" s="123"/>
-      <c r="G55" s="125"/>
-      <c r="H55" s="127"/>
+      <c r="D55" s="123"/>
+      <c r="E55" s="121"/>
+      <c r="F55" s="121"/>
+      <c r="G55" s="123"/>
+      <c r="H55" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E18"/>
+    <mergeCell ref="F4:F18"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="D21:D26"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="F21:F26"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="D42:D51"/>
+    <mergeCell ref="E42:E51"/>
+    <mergeCell ref="F42:F51"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="F52:F55"/>
+    <mergeCell ref="G4:G18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G21:G26"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="G32:G34"/>
     <mergeCell ref="G39:G41"/>
     <mergeCell ref="G42:G51"/>
     <mergeCell ref="G52:G55"/>
@@ -7416,42 +7553,6 @@
     <mergeCell ref="H35:H36"/>
     <mergeCell ref="H42:H51"/>
     <mergeCell ref="G35:G36"/>
-    <mergeCell ref="G4:G18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G21:G26"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G32:G34"/>
-    <mergeCell ref="D42:D51"/>
-    <mergeCell ref="E42:E51"/>
-    <mergeCell ref="F42:F51"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="F52:F55"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="D21:D26"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="F21:F26"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E18"/>
-    <mergeCell ref="F4:F18"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C37" location="_ftn2" display="_ftn2" xr:uid="{74DB3199-791E-4FED-9C20-E93C69505EA4}"/>
@@ -7501,7 +7602,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="135" t="s">
+      <c r="A3" s="133" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2"/>
@@ -7515,7 +7616,7 @@
       <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="135"/>
+      <c r="A4" s="133"/>
       <c r="B4" s="2"/>
       <c r="C4" s="23" t="s">
         <v>65</v>
@@ -7527,7 +7628,7 @@
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="135"/>
+      <c r="A5" s="133"/>
       <c r="B5" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -7545,7 +7646,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="136" t="s">
+      <c r="A6" s="134" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2">
@@ -7563,7 +7664,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="136"/>
+      <c r="A7" s="134"/>
       <c r="B7" s="2">
         <v>2.2000000000000002</v>
       </c>
@@ -7579,7 +7680,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="136" t="s">
+      <c r="A8" s="134" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2">
@@ -7599,7 +7700,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="136"/>
+      <c r="A9" s="134"/>
       <c r="B9" s="2"/>
       <c r="C9" s="23" t="s">
         <v>64</v>
@@ -7611,7 +7712,7 @@
       <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="136"/>
+      <c r="A10" s="134"/>
       <c r="B10" s="2"/>
       <c r="C10" s="23" t="s">
         <v>55</v>
@@ -7623,7 +7724,7 @@
       <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="136"/>
+      <c r="A11" s="134"/>
       <c r="B11" s="2"/>
       <c r="C11" s="23" t="s">
         <v>50</v>
@@ -7635,7 +7736,7 @@
       <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="136"/>
+      <c r="A12" s="134"/>
       <c r="B12" s="2">
         <v>3.2</v>
       </c>
@@ -7653,7 +7754,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="136"/>
+      <c r="A13" s="134"/>
       <c r="B13" s="2">
         <v>12.1</v>
       </c>
@@ -7669,7 +7770,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="136"/>
+      <c r="A14" s="134"/>
       <c r="B14" s="2">
         <v>12.2</v>
       </c>
@@ -7685,7 +7786,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="136"/>
+      <c r="A15" s="134"/>
       <c r="B15" s="2">
         <v>12.3</v>
       </c>
@@ -7701,7 +7802,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="135" t="s">
+      <c r="A16" s="133" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="18">
@@ -7721,7 +7822,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="135"/>
+      <c r="A17" s="133"/>
       <c r="B17" s="18">
         <v>5.2</v>
       </c>
@@ -7739,7 +7840,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="135"/>
+      <c r="A18" s="133"/>
       <c r="B18" s="2">
         <v>5.3</v>
       </c>
@@ -7757,7 +7858,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="135"/>
+      <c r="A19" s="133"/>
       <c r="B19" s="18">
         <v>5.4</v>
       </c>
@@ -7775,7 +7876,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="135"/>
+      <c r="A20" s="133"/>
       <c r="B20" s="18"/>
       <c r="C20" s="22" t="s">
         <v>53</v>
@@ -7787,7 +7888,7 @@
       <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="135"/>
+      <c r="A21" s="133"/>
       <c r="B21" s="18"/>
       <c r="C21" s="22" t="s">
         <v>54</v>
@@ -7799,7 +7900,7 @@
       <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="135" t="s">
+      <c r="A22" s="133" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="18">
@@ -7819,7 +7920,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="135"/>
+      <c r="A23" s="133"/>
       <c r="B23" s="2"/>
       <c r="C23" s="22" t="s">
         <v>52</v>
@@ -7831,7 +7932,7 @@
       <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="135"/>
+      <c r="A24" s="133"/>
       <c r="B24" s="2"/>
       <c r="C24" s="22" t="s">
         <v>51</v>
@@ -7843,7 +7944,7 @@
       <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="136" t="s">
+      <c r="A25" s="134" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="2">
@@ -7861,7 +7962,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="136"/>
+      <c r="A26" s="134"/>
       <c r="B26" s="2">
         <v>7.2</v>
       </c>
@@ -7877,7 +7978,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="138" t="s">
+      <c r="A27" s="136" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="18">
@@ -7897,7 +7998,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="138"/>
+      <c r="A28" s="136"/>
       <c r="B28" s="18">
         <v>8.1999999999999993</v>
       </c>
@@ -7915,7 +8016,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="138"/>
+      <c r="A29" s="136"/>
       <c r="B29" s="18">
         <v>8.3000000000000007</v>
       </c>
@@ -7933,7 +8034,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="138"/>
+      <c r="A30" s="136"/>
       <c r="B30" s="24">
         <v>8.1</v>
       </c>
@@ -7951,7 +8052,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="138"/>
+      <c r="A31" s="136"/>
       <c r="B31" s="24">
         <v>8.1999999999999993</v>
       </c>
@@ -7969,7 +8070,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="138"/>
+      <c r="A32" s="136"/>
       <c r="B32" s="24">
         <v>8.3000000000000007</v>
       </c>
@@ -7987,7 +8088,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="135" t="s">
+      <c r="A33" s="133" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="2">
@@ -8005,7 +8106,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="135"/>
+      <c r="A34" s="133"/>
       <c r="B34" s="2">
         <v>9.1999999999999993</v>
       </c>
@@ -8021,7 +8122,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="135"/>
+      <c r="A35" s="133"/>
       <c r="B35" s="2"/>
       <c r="C35" s="23" t="s">
         <v>59</v>
@@ -8051,7 +8152,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="137" t="s">
+      <c r="A37" s="135" t="s">
         <v>39</v>
       </c>
       <c r="B37" s="4">
@@ -8069,7 +8170,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="137"/>
+      <c r="A38" s="135"/>
       <c r="B38" s="4">
         <v>11.2</v>
       </c>
@@ -8085,7 +8186,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" s="16" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="137"/>
+      <c r="A39" s="135"/>
       <c r="B39" s="4">
         <v>11.3</v>
       </c>
@@ -8101,7 +8202,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" s="16" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="137"/>
+      <c r="A40" s="135"/>
       <c r="B40" s="4"/>
       <c r="C40" s="22" t="s">
         <v>66</v>
@@ -8113,7 +8214,7 @@
       <c r="F40" s="28"/>
     </row>
     <row r="41" spans="1:6" s="16" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="137"/>
+      <c r="A41" s="135"/>
       <c r="B41" s="4"/>
       <c r="C41" s="22" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Automatic update of 18/05/2024 at 16:55
</commit_message>
<xml_diff>
--- a/Indicadores OPI-CETG rev 28.04.24 v3.xlsx
+++ b/Indicadores OPI-CETG rev 28.04.24 v3.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\03. Job\05. CONSULTORIAS\13. MEF\FIDT_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56C0AF8-AC83-42A1-B475-DA6777E9499C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AF265B-56AB-4952-91FE-B66325786BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{A4291CEF-37A6-4732-90F4-77F55B4FD4D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="3" xr2:uid="{A4291CEF-37A6-4732-90F4-77F55B4FD4D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="2" state="hidden" r:id="rId1"/>
     <sheet name="Indicadores_V2" sheetId="3" state="hidden" r:id="rId2"/>
-    <sheet name="Indicadores_v4" sheetId="5" state="hidden" r:id="rId3"/>
+    <sheet name="Indicadores_v4" sheetId="5" r:id="rId3"/>
     <sheet name="Hoja3" sheetId="6" r:id="rId4"/>
-    <sheet name="Indicadores_v3" sheetId="4" state="hidden" r:id="rId5"/>
+    <sheet name="Indicadores_v3" sheetId="4" r:id="rId5"/>
     <sheet name="Hoja1" sheetId="1" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Hoja3!$A$1:$D$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Hoja3!$A$1:$D$46</definedName>
     <definedName name="_ftn1" localSheetId="5">Hoja1!$D$44</definedName>
     <definedName name="_ftn1" localSheetId="0">Indicadores!$E$52</definedName>
     <definedName name="_ftn1" localSheetId="1">Indicadores_V2!#REF!</definedName>
@@ -179,7 +179,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="348">
   <si>
     <t>SERVICIOS</t>
   </si>
@@ -1180,9 +1180,6 @@
     <t>Encuesta Nacional a Instituciones Educativas</t>
   </si>
   <si>
-    <t>Pocentaje  de Ejecución anual</t>
-  </si>
-  <si>
     <t>Porcentaje de PEA ocupada agrícola</t>
   </si>
   <si>
@@ -1267,18 +1264,6 @@
     <t>Porcentaje de locales educativos con eliminación de excretas del local educativo  a traves de Red pública de desagüe dentro del local educativo y Red pública de desagüe fuera del local educativo, pero dentro de la edificación</t>
   </si>
   <si>
-    <t xml:space="preserve">Porcentaje de locales educativos con el material predominante en el piso del local educativo de Parquet o madera pulida, Láminas asfálticas, vinílicos o similares, Losetas, terrazos, cerámicos o similares, Madera (pona, tornillo, etc.) y Cemento
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porcentaje de locales educativos con el material predominante en el techo del local educativo de Concreto armado, Madera, Tejas y Planchas de calamina, fibra de cemento o similares
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porcentaje de locales educativos con acceso al servicio de energía eléctrica del local educativo por Red pública de electricidad dentro del local educativo y Red pública de electricidad fuera del local educativo, pero dentro de la edificación
-</t>
-  </si>
-  <si>
     <t>Porcentaje de locales educativos con abastecimiento de agua del local educativo por Red pública, Red pública dentro de la vivienda, Red pública fuera de la vivienda, pero dentro de la edificación y Pilón o pileta de uso público</t>
   </si>
   <si>
@@ -1352,12 +1337,6 @@
   </si>
   <si>
     <t>v33_</t>
-  </si>
-  <si>
-    <t>v46_</t>
-  </si>
-  <si>
-    <t>v47_</t>
   </si>
   <si>
     <t>v01_Establecimientos_salud_SP</t>
@@ -1461,13 +1440,58 @@
     <t>v23_Cerco_perimétrico_total
 v23_Cerco_perimétrico_parcial
 v23_Cerco_perimétrico_no_tiene</t>
+  </si>
+  <si>
+    <t>Porcentaje de locales educativos con el material predominante en el techo del local educativo de Concreto armado, Madera, Tejas y Planchas de calamina, fibra de cemento o similares</t>
+  </si>
+  <si>
+    <t>Porcentaje de locales educativos con acceso al servicio de energía eléctrica del local educativo por Red pública de electricidad dentro del local educativo y Red pública de electricidad fuera del local educativo, pero dentro de la edificación</t>
+  </si>
+  <si>
+    <t>Porcentaje de locales educativos con el material predominante en el piso del local educativo de Parquet o madera pulida, Láminas asfálticas, vinílicos o similares, Losetas, terrazos, cerámicos o similares, Madera (pona, tornillo, etc.) y Cemento</t>
+  </si>
+  <si>
+    <t>PIM promedio total</t>
+  </si>
+  <si>
+    <t>PIM promedio de inversiones cuya función es subvencionada por el FIDT</t>
+  </si>
+  <si>
+    <t>PIM promedio por donaciones y Transferencia</t>
+  </si>
+  <si>
+    <t>Porcentaje de ejecución promedio de donaciones y transferencia</t>
+  </si>
+  <si>
+    <t>Porcentaje de ejecución promedio total</t>
+  </si>
+  <si>
+    <t>Porcentaje de ejecución promedio de inversiones cuya función es subvencionada FIDT</t>
+  </si>
+  <si>
+    <t>v51_Ejecución_promedio_donaciones</t>
+  </si>
+  <si>
+    <t>v50_Ejecución_FIDT</t>
+  </si>
+  <si>
+    <t>v49_Ejecución_total</t>
+  </si>
+  <si>
+    <t>v48_PIM_promedio_donaciones</t>
+  </si>
+  <si>
+    <t>v47_PIM_promedio_FIDT</t>
+  </si>
+  <si>
+    <t>v46_PIM_promedio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1635,8 +1659,21 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1670,6 +1707,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1779,7 +1828,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -2043,9 +2092,6 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2091,6 +2137,24 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2118,21 +2182,6 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2142,12 +2191,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2180,6 +2229,39 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2555,8 +2637,8 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="120"/>
-      <c r="B3" s="117" t="s">
+      <c r="A3" s="111"/>
+      <c r="B3" s="108" t="s">
         <v>99</v>
       </c>
       <c r="C3" s="31"/>
@@ -2573,8 +2655,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="120"/>
-      <c r="B4" s="117"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="108"/>
       <c r="C4" s="31"/>
       <c r="D4" s="23" t="s">
         <v>65</v>
@@ -2586,8 +2668,8 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="120"/>
-      <c r="B5" s="117"/>
+      <c r="A5" s="111"/>
+      <c r="B5" s="108"/>
       <c r="C5" s="31">
         <v>1.1000000000000001</v>
       </c>
@@ -2605,8 +2687,8 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="120"/>
-      <c r="B6" s="117" t="s">
+      <c r="A6" s="111"/>
+      <c r="B6" s="108" t="s">
         <v>68</v>
       </c>
       <c r="C6" s="31">
@@ -2624,8 +2706,8 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="120"/>
-      <c r="B7" s="117"/>
+      <c r="A7" s="111"/>
+      <c r="B7" s="108"/>
       <c r="C7" s="31">
         <v>2.2000000000000002</v>
       </c>
@@ -2641,8 +2723,8 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="120"/>
-      <c r="B8" s="117" t="s">
+      <c r="A8" s="111"/>
+      <c r="B8" s="108" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="31">
@@ -2662,8 +2744,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="120"/>
-      <c r="B9" s="117"/>
+      <c r="A9" s="111"/>
+      <c r="B9" s="108"/>
       <c r="C9" s="31"/>
       <c r="D9" s="23" t="s">
         <v>117</v>
@@ -2678,8 +2760,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="120"/>
-      <c r="B10" s="117"/>
+      <c r="A10" s="111"/>
+      <c r="B10" s="108"/>
       <c r="C10" s="31"/>
       <c r="D10" s="23" t="s">
         <v>105</v>
@@ -2689,13 +2771,13 @@
       </c>
       <c r="F10" s="56"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="118" t="s">
+      <c r="H10" s="109" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="120"/>
-      <c r="B11" s="117"/>
+      <c r="A11" s="111"/>
+      <c r="B11" s="108"/>
       <c r="C11" s="31"/>
       <c r="D11" s="23" t="s">
         <v>50</v>
@@ -2705,11 +2787,11 @@
       </c>
       <c r="F11" s="56"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="118"/>
+      <c r="H11" s="109"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="120"/>
-      <c r="B12" s="117"/>
+      <c r="A12" s="111"/>
+      <c r="B12" s="108"/>
       <c r="C12" s="31">
         <v>3.2</v>
       </c>
@@ -2727,8 +2809,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="120"/>
-      <c r="B13" s="117"/>
+      <c r="A13" s="111"/>
+      <c r="B13" s="108"/>
       <c r="C13" s="31">
         <v>12.1</v>
       </c>
@@ -2744,8 +2826,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="120"/>
-      <c r="B14" s="117"/>
+      <c r="A14" s="111"/>
+      <c r="B14" s="108"/>
       <c r="C14" s="31">
         <v>12.2</v>
       </c>
@@ -2761,8 +2843,8 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="120"/>
-      <c r="B15" s="117"/>
+      <c r="A15" s="111"/>
+      <c r="B15" s="108"/>
       <c r="C15" s="31">
         <v>12.3</v>
       </c>
@@ -2778,8 +2860,8 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="120"/>
-      <c r="B16" s="117" t="s">
+      <c r="A16" s="111"/>
+      <c r="B16" s="108" t="s">
         <v>67</v>
       </c>
       <c r="C16" s="31"/>
@@ -2793,8 +2875,8 @@
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="120"/>
-      <c r="B17" s="117"/>
+      <c r="A17" s="111"/>
+      <c r="B17" s="108"/>
       <c r="C17" s="31"/>
       <c r="D17" s="23" t="s">
         <v>108</v>
@@ -2806,8 +2888,8 @@
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="120"/>
-      <c r="B18" s="117"/>
+      <c r="A18" s="111"/>
+      <c r="B18" s="108"/>
       <c r="C18" s="31"/>
       <c r="D18" s="23" t="s">
         <v>109</v>
@@ -2819,8 +2901,8 @@
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="120"/>
-      <c r="B19" s="117"/>
+      <c r="A19" s="111"/>
+      <c r="B19" s="108"/>
       <c r="C19" s="31"/>
       <c r="D19" s="23" t="s">
         <v>110</v>
@@ -2832,8 +2914,8 @@
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="120"/>
-      <c r="B20" s="117"/>
+      <c r="A20" s="111"/>
+      <c r="B20" s="108"/>
       <c r="C20" s="31"/>
       <c r="D20" s="23" t="s">
         <v>111</v>
@@ -2845,8 +2927,8 @@
       <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="120"/>
-      <c r="B21" s="117"/>
+      <c r="A21" s="111"/>
+      <c r="B21" s="108"/>
       <c r="C21" s="31"/>
       <c r="D21" s="23" t="s">
         <v>112</v>
@@ -2861,8 +2943,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="120"/>
-      <c r="B22" s="117" t="s">
+      <c r="A22" s="111"/>
+      <c r="B22" s="108" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="35">
@@ -2885,8 +2967,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="120"/>
-      <c r="B23" s="117"/>
+      <c r="A23" s="111"/>
+      <c r="B23" s="108"/>
       <c r="C23" s="35">
         <v>5.2</v>
       </c>
@@ -2907,8 +2989,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="120"/>
-      <c r="B24" s="117"/>
+      <c r="A24" s="111"/>
+      <c r="B24" s="108"/>
       <c r="C24" s="31">
         <v>5.3</v>
       </c>
@@ -2926,8 +3008,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="120"/>
-      <c r="B25" s="117"/>
+      <c r="A25" s="111"/>
+      <c r="B25" s="108"/>
       <c r="C25" s="35">
         <v>5.4</v>
       </c>
@@ -2948,8 +3030,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="120"/>
-      <c r="B26" s="117"/>
+      <c r="A26" s="111"/>
+      <c r="B26" s="108"/>
       <c r="C26" s="35"/>
       <c r="D26" s="41" t="s">
         <v>53</v>
@@ -2964,8 +3046,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="120"/>
-      <c r="B27" s="117"/>
+      <c r="A27" s="111"/>
+      <c r="B27" s="108"/>
       <c r="C27" s="35"/>
       <c r="D27" s="41" t="s">
         <v>54</v>
@@ -2980,8 +3062,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="120"/>
-      <c r="B28" s="117" t="s">
+      <c r="A28" s="111"/>
+      <c r="B28" s="108" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="35">
@@ -3004,8 +3086,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="120"/>
-      <c r="B29" s="117"/>
+      <c r="A29" s="111"/>
+      <c r="B29" s="108"/>
       <c r="C29" s="31"/>
       <c r="D29" s="41" t="s">
         <v>51</v>
@@ -3020,8 +3102,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="120"/>
-      <c r="B30" s="117"/>
+      <c r="A30" s="111"/>
+      <c r="B30" s="108"/>
       <c r="C30" s="31"/>
       <c r="D30" s="41" t="s">
         <v>52</v>
@@ -3036,8 +3118,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="120"/>
-      <c r="B31" s="117" t="s">
+      <c r="A31" s="111"/>
+      <c r="B31" s="108" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="31">
@@ -3055,8 +3137,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="120"/>
-      <c r="B32" s="117"/>
+      <c r="A32" s="111"/>
+      <c r="B32" s="108"/>
       <c r="C32" s="31">
         <v>7.2</v>
       </c>
@@ -3072,8 +3154,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="120"/>
-      <c r="B33" s="117" t="s">
+      <c r="A33" s="111"/>
+      <c r="B33" s="108" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="35">
@@ -3096,8 +3178,8 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="120"/>
-      <c r="B34" s="117"/>
+      <c r="A34" s="111"/>
+      <c r="B34" s="108"/>
       <c r="C34" s="35">
         <v>8.1999999999999993</v>
       </c>
@@ -3118,8 +3200,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="120"/>
-      <c r="B35" s="117"/>
+      <c r="A35" s="111"/>
+      <c r="B35" s="108"/>
       <c r="C35" s="35">
         <v>8.3000000000000007</v>
       </c>
@@ -3140,8 +3222,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="120"/>
-      <c r="B36" s="117"/>
+      <c r="A36" s="111"/>
+      <c r="B36" s="108"/>
       <c r="C36" s="32">
         <v>8.1</v>
       </c>
@@ -3162,8 +3244,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="120"/>
-      <c r="B37" s="117"/>
+      <c r="A37" s="111"/>
+      <c r="B37" s="108"/>
       <c r="C37" s="32">
         <v>8.1999999999999993</v>
       </c>
@@ -3184,8 +3266,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="120"/>
-      <c r="B38" s="117"/>
+      <c r="A38" s="111"/>
+      <c r="B38" s="108"/>
       <c r="C38" s="32">
         <v>8.3000000000000007</v>
       </c>
@@ -3206,8 +3288,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="120"/>
-      <c r="B39" s="117"/>
+      <c r="A39" s="111"/>
+      <c r="B39" s="108"/>
       <c r="C39" s="32"/>
       <c r="D39" s="22" t="s">
         <v>72</v>
@@ -3219,8 +3301,8 @@
       <c r="G39" s="43"/>
     </row>
     <row r="40" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="120"/>
-      <c r="B40" s="117" t="s">
+      <c r="A40" s="111"/>
+      <c r="B40" s="108" t="s">
         <v>34</v>
       </c>
       <c r="C40" s="31">
@@ -3238,8 +3320,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="120"/>
-      <c r="B41" s="117"/>
+      <c r="A41" s="111"/>
+      <c r="B41" s="108"/>
       <c r="C41" s="31">
         <v>9.1999999999999993</v>
       </c>
@@ -3255,8 +3337,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="120"/>
-      <c r="B42" s="117"/>
+      <c r="A42" s="111"/>
+      <c r="B42" s="108"/>
       <c r="C42" s="31"/>
       <c r="D42" s="23" t="s">
         <v>59</v>
@@ -3268,8 +3350,8 @@
       <c r="G42" s="12"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="120"/>
-      <c r="B43" s="117"/>
+      <c r="A43" s="111"/>
+      <c r="B43" s="108"/>
       <c r="C43" s="31"/>
       <c r="D43" s="22" t="s">
         <v>86</v>
@@ -3284,8 +3366,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="120"/>
-      <c r="B44" s="117"/>
+      <c r="A44" s="111"/>
+      <c r="B44" s="108"/>
       <c r="C44" s="31"/>
       <c r="D44" s="22" t="s">
         <v>87</v>
@@ -3300,8 +3382,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="120"/>
-      <c r="B45" s="117"/>
+      <c r="A45" s="111"/>
+      <c r="B45" s="108"/>
       <c r="C45" s="31"/>
       <c r="D45" s="22" t="s">
         <v>100</v>
@@ -3316,10 +3398,10 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="120" t="s">
+      <c r="A46" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="119" t="s">
+      <c r="B46" s="110" t="s">
         <v>114</v>
       </c>
       <c r="C46" s="34">
@@ -3340,8 +3422,8 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="120"/>
-      <c r="B47" s="119"/>
+      <c r="A47" s="111"/>
+      <c r="B47" s="110"/>
       <c r="C47" s="34">
         <v>11.2</v>
       </c>
@@ -3360,8 +3442,8 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="120"/>
-      <c r="B48" s="119"/>
+      <c r="A48" s="111"/>
+      <c r="B48" s="110"/>
       <c r="C48" s="34">
         <v>11.3</v>
       </c>
@@ -3380,8 +3462,8 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="120"/>
-      <c r="B49" s="119"/>
+      <c r="A49" s="111"/>
+      <c r="B49" s="110"/>
       <c r="C49" s="34"/>
       <c r="D49" s="22" t="s">
         <v>66</v>
@@ -3396,8 +3478,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="120"/>
-      <c r="B50" s="119"/>
+      <c r="A50" s="111"/>
+      <c r="B50" s="110"/>
       <c r="C50" s="34"/>
       <c r="D50" s="22" t="s">
         <v>63</v>
@@ -3412,10 +3494,10 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="116" t="s">
+      <c r="A51" s="107" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="116"/>
+      <c r="B51" s="107"/>
       <c r="C51" s="62"/>
       <c r="D51" s="52" t="s">
         <v>115</v>
@@ -3428,8 +3510,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="116"/>
-      <c r="B52" s="116"/>
+      <c r="A52" s="107"/>
+      <c r="B52" s="107"/>
       <c r="C52" s="62"/>
       <c r="D52" s="52" t="s">
         <v>89</v>
@@ -3440,8 +3522,8 @@
       <c r="F52" s="47"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="116"/>
-      <c r="B53" s="116"/>
+      <c r="A53" s="107"/>
+      <c r="B53" s="107"/>
       <c r="C53" s="62"/>
       <c r="D53" s="54" t="s">
         <v>38</v>
@@ -3452,8 +3534,8 @@
       <c r="F53" s="47"/>
     </row>
     <row r="54" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="116"/>
-      <c r="B54" s="116"/>
+      <c r="A54" s="107"/>
+      <c r="B54" s="107"/>
       <c r="C54" s="62"/>
       <c r="D54" s="52" t="s">
         <v>81</v>
@@ -3464,41 +3546,41 @@
       <c r="F54" s="47"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="107" t="s">
+      <c r="A55" s="112" t="s">
         <v>126</v>
       </c>
-      <c r="B55" s="107"/>
-      <c r="C55" s="107"/>
-      <c r="D55" s="107"/>
-      <c r="E55" s="107"/>
+      <c r="B55" s="112"/>
+      <c r="C55" s="112"/>
+      <c r="D55" s="112"/>
+      <c r="E55" s="112"/>
       <c r="F55" s="47"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="108"/>
-      <c r="B56" s="108"/>
-      <c r="C56" s="108"/>
-      <c r="D56" s="108"/>
-      <c r="E56" s="108"/>
+      <c r="A56" s="113"/>
+      <c r="B56" s="113"/>
+      <c r="C56" s="113"/>
+      <c r="D56" s="113"/>
+      <c r="E56" s="113"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="108"/>
-      <c r="B57" s="108"/>
-      <c r="C57" s="108"/>
-      <c r="D57" s="108"/>
-      <c r="E57" s="108"/>
+      <c r="A57" s="113"/>
+      <c r="B57" s="113"/>
+      <c r="C57" s="113"/>
+      <c r="D57" s="113"/>
+      <c r="E57" s="113"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="109"/>
-      <c r="B58" s="109"/>
-      <c r="C58" s="109"/>
-      <c r="D58" s="109"/>
-      <c r="E58" s="109"/>
+      <c r="A58" s="114"/>
+      <c r="B58" s="114"/>
+      <c r="C58" s="114"/>
+      <c r="D58" s="114"/>
+      <c r="E58" s="114"/>
     </row>
     <row r="59" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A59" s="110" t="s">
+      <c r="A59" s="115" t="s">
         <v>118</v>
       </c>
-      <c r="B59" s="113" t="s">
+      <c r="B59" s="118" t="s">
         <v>125</v>
       </c>
       <c r="C59" s="64"/>
@@ -3513,8 +3595,8 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="110"/>
-      <c r="B60" s="114"/>
+      <c r="A60" s="115"/>
+      <c r="B60" s="119"/>
       <c r="C60" s="64"/>
       <c r="D60" s="69" t="s">
         <v>137</v>
@@ -3527,8 +3609,8 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="110"/>
-      <c r="B61" s="115"/>
+      <c r="A61" s="115"/>
+      <c r="B61" s="120"/>
       <c r="C61" s="64"/>
       <c r="D61" s="69" t="s">
         <v>138</v>
@@ -3541,8 +3623,8 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="110"/>
-      <c r="B62" s="111" t="s">
+      <c r="A62" s="115"/>
+      <c r="B62" s="116" t="s">
         <v>120</v>
       </c>
       <c r="C62" s="66"/>
@@ -3557,8 +3639,8 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="110"/>
-      <c r="B63" s="111"/>
+      <c r="A63" s="115"/>
+      <c r="B63" s="116"/>
       <c r="C63" s="66"/>
       <c r="D63" s="67" t="s">
         <v>139</v>
@@ -3571,8 +3653,8 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A64" s="110"/>
-      <c r="B64" s="111"/>
+      <c r="A64" s="115"/>
+      <c r="B64" s="116"/>
       <c r="C64" s="66"/>
       <c r="D64" s="67" t="s">
         <v>128</v>
@@ -3585,8 +3667,8 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A65" s="110"/>
-      <c r="B65" s="111"/>
+      <c r="A65" s="115"/>
+      <c r="B65" s="116"/>
       <c r="C65" s="66"/>
       <c r="D65" s="67" t="s">
         <v>129</v>
@@ -3599,8 +3681,8 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="110"/>
-      <c r="B66" s="111"/>
+      <c r="A66" s="115"/>
+      <c r="B66" s="116"/>
       <c r="C66" s="66"/>
       <c r="D66" s="67" t="s">
         <v>130</v>
@@ -3613,8 +3695,8 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="110"/>
-      <c r="B67" s="111" t="s">
+      <c r="A67" s="115"/>
+      <c r="B67" s="116" t="s">
         <v>122</v>
       </c>
       <c r="C67" s="66"/>
@@ -3629,8 +3711,8 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="110"/>
-      <c r="B68" s="111"/>
+      <c r="A68" s="115"/>
+      <c r="B68" s="116"/>
       <c r="C68" s="66"/>
       <c r="D68" s="67" t="s">
         <v>133</v>
@@ -3643,8 +3725,8 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A69" s="110"/>
-      <c r="B69" s="111"/>
+      <c r="A69" s="115"/>
+      <c r="B69" s="116"/>
       <c r="C69" s="66"/>
       <c r="D69" s="67" t="s">
         <v>132</v>
@@ -3657,8 +3739,8 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="110"/>
-      <c r="B70" s="111"/>
+      <c r="A70" s="115"/>
+      <c r="B70" s="116"/>
       <c r="C70" s="66"/>
       <c r="D70" s="68" t="s">
         <v>135</v>
@@ -3671,8 +3753,8 @@
       </c>
     </row>
     <row r="71" spans="1:8" s="16" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="110"/>
-      <c r="B71" s="112" t="s">
+      <c r="A71" s="115"/>
+      <c r="B71" s="117" t="s">
         <v>123</v>
       </c>
       <c r="C71" s="64"/>
@@ -3688,8 +3770,8 @@
       <c r="H71" s="71"/>
     </row>
     <row r="72" spans="1:8" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="110"/>
-      <c r="B72" s="112"/>
+      <c r="A72" s="115"/>
+      <c r="B72" s="117"/>
       <c r="C72" s="64"/>
       <c r="D72" s="69" t="s">
         <v>141</v>
@@ -3703,8 +3785,8 @@
       <c r="H72" s="71"/>
     </row>
     <row r="73" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="110"/>
-      <c r="B73" s="111" t="s">
+      <c r="A73" s="115"/>
+      <c r="B73" s="116" t="s">
         <v>124</v>
       </c>
       <c r="C73" s="66"/>
@@ -3719,8 +3801,8 @@
       </c>
     </row>
     <row r="74" spans="1:8" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.25">
-      <c r="A74" s="110"/>
-      <c r="B74" s="111"/>
+      <c r="A74" s="115"/>
+      <c r="B74" s="116"/>
       <c r="C74" s="64"/>
       <c r="D74" s="69" t="s">
         <v>134</v>
@@ -3743,6 +3825,13 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A55:E58"/>
+    <mergeCell ref="A59:A74"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="B59:B61"/>
     <mergeCell ref="A51:B54"/>
     <mergeCell ref="B16:B21"/>
     <mergeCell ref="H10:H11"/>
@@ -3757,13 +3846,6 @@
     <mergeCell ref="B22:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B32"/>
-    <mergeCell ref="A55:E58"/>
-    <mergeCell ref="A59:A74"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="B59:B61"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E53" location="_ftn2" display="_ftn2" xr:uid="{FFC9BABA-D715-48D2-801D-3C2A2DB136EB}"/>
@@ -4654,24 +4736,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="F52:F55"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="D42:D51"/>
-    <mergeCell ref="E42:E51"/>
-    <mergeCell ref="F42:F51"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="F32:F34"/>
     <mergeCell ref="D13:D17"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
@@ -4685,6 +4749,24 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="F52:F55"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="D42:D51"/>
+    <mergeCell ref="E42:E51"/>
+    <mergeCell ref="F42:F51"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C37" location="_ftn2" display="_ftn2" xr:uid="{25CB2AF1-E91C-4F96-A745-EB04437048A9}"/>
@@ -4699,7 +4781,7 @@
   <dimension ref="A2:H51"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
@@ -5044,7 +5126,7 @@
       <c r="G19" s="123" t="s">
         <v>235</v>
       </c>
-      <c r="H19" s="125" t="s">
+      <c r="H19" s="124" t="s">
         <v>234</v>
       </c>
     </row>
@@ -5062,7 +5144,7 @@
       <c r="E20" s="121"/>
       <c r="F20" s="121"/>
       <c r="G20" s="123"/>
-      <c r="H20" s="125"/>
+      <c r="H20" s="124"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
@@ -5214,7 +5296,7 @@
       <c r="G28" s="126" t="s">
         <v>243</v>
       </c>
-      <c r="H28" s="124" t="s">
+      <c r="H28" s="125" t="s">
         <v>242</v>
       </c>
     </row>
@@ -5232,7 +5314,7 @@
       <c r="E29" s="121"/>
       <c r="F29" s="122"/>
       <c r="G29" s="126"/>
-      <c r="H29" s="124"/>
+      <c r="H29" s="125"/>
     </row>
     <row r="30" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="74" t="s">
@@ -5248,7 +5330,7 @@
       <c r="E30" s="121"/>
       <c r="F30" s="122"/>
       <c r="G30" s="126"/>
-      <c r="H30" s="124"/>
+      <c r="H30" s="125"/>
     </row>
     <row r="31" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="80" t="s">
@@ -5270,7 +5352,7 @@
         <v>181</v>
       </c>
       <c r="G31" s="123"/>
-      <c r="H31" s="124"/>
+      <c r="H31" s="125"/>
     </row>
     <row r="32" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="80" t="s">
@@ -5286,7 +5368,7 @@
       <c r="E32" s="121"/>
       <c r="F32" s="121"/>
       <c r="G32" s="123"/>
-      <c r="H32" s="124"/>
+      <c r="H32" s="125"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="81" t="s">
@@ -5358,7 +5440,7 @@
       <c r="G35" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="H35" s="125" t="s">
+      <c r="H35" s="124" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5376,7 +5458,7 @@
       <c r="E36" s="121"/>
       <c r="F36" s="121"/>
       <c r="G36" s="123"/>
-      <c r="H36" s="125"/>
+      <c r="H36" s="124"/>
     </row>
     <row r="37" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A37" s="78" t="s">
@@ -5392,7 +5474,7 @@
       <c r="E37" s="121"/>
       <c r="F37" s="121"/>
       <c r="G37" s="123"/>
-      <c r="H37" s="125"/>
+      <c r="H37" s="124"/>
     </row>
     <row r="38" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="78" t="s">
@@ -5416,7 +5498,7 @@
       <c r="G38" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="H38" s="124" t="s">
+      <c r="H38" s="125" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5434,7 +5516,7 @@
       <c r="E39" s="121"/>
       <c r="F39" s="121"/>
       <c r="G39" s="123"/>
-      <c r="H39" s="124"/>
+      <c r="H39" s="125"/>
     </row>
     <row r="40" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A40" s="78" t="s">
@@ -5450,7 +5532,7 @@
       <c r="E40" s="121"/>
       <c r="F40" s="121"/>
       <c r="G40" s="123"/>
-      <c r="H40" s="124"/>
+      <c r="H40" s="125"/>
     </row>
     <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A41" s="78" t="s">
@@ -5466,7 +5548,7 @@
       <c r="E41" s="121"/>
       <c r="F41" s="121"/>
       <c r="G41" s="123"/>
-      <c r="H41" s="124"/>
+      <c r="H41" s="125"/>
     </row>
     <row r="42" spans="1:8" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="78" t="s">
@@ -5482,7 +5564,7 @@
       <c r="E42" s="121"/>
       <c r="F42" s="121"/>
       <c r="G42" s="123"/>
-      <c r="H42" s="124"/>
+      <c r="H42" s="125"/>
     </row>
     <row r="43" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A43" s="78" t="s">
@@ -5498,7 +5580,7 @@
       <c r="E43" s="121"/>
       <c r="F43" s="121"/>
       <c r="G43" s="123"/>
-      <c r="H43" s="124"/>
+      <c r="H43" s="125"/>
     </row>
     <row r="44" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A44" s="78" t="s">
@@ -5514,7 +5596,7 @@
       <c r="E44" s="121"/>
       <c r="F44" s="121"/>
       <c r="G44" s="123"/>
-      <c r="H44" s="124"/>
+      <c r="H44" s="125"/>
     </row>
     <row r="45" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A45" s="78" t="s">
@@ -5530,7 +5612,7 @@
       <c r="E45" s="121"/>
       <c r="F45" s="121"/>
       <c r="G45" s="123"/>
-      <c r="H45" s="124"/>
+      <c r="H45" s="125"/>
     </row>
     <row r="46" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A46" s="78" t="s">
@@ -5546,7 +5628,7 @@
       <c r="E46" s="121"/>
       <c r="F46" s="121"/>
       <c r="G46" s="123"/>
-      <c r="H46" s="124"/>
+      <c r="H46" s="125"/>
     </row>
     <row r="47" spans="1:8" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="78" t="s">
@@ -5562,7 +5644,7 @@
       <c r="E47" s="121"/>
       <c r="F47" s="121"/>
       <c r="G47" s="123"/>
-      <c r="H47" s="124"/>
+      <c r="H47" s="125"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="78" t="s">
@@ -5586,7 +5668,7 @@
       <c r="G48" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="H48" s="124" t="s">
+      <c r="H48" s="125" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5604,7 +5686,7 @@
       <c r="E49" s="121"/>
       <c r="F49" s="121"/>
       <c r="G49" s="123"/>
-      <c r="H49" s="124"/>
+      <c r="H49" s="125"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="78" t="s">
@@ -5620,7 +5702,7 @@
       <c r="E50" s="121"/>
       <c r="F50" s="121"/>
       <c r="G50" s="123"/>
-      <c r="H50" s="124"/>
+      <c r="H50" s="125"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="78" t="s">
@@ -5636,21 +5718,25 @@
       <c r="E51" s="121"/>
       <c r="F51" s="121"/>
       <c r="G51" s="123"/>
-      <c r="H51" s="124"/>
+      <c r="H51" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E18"/>
-    <mergeCell ref="F4:F18"/>
-    <mergeCell ref="G4:G18"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="F48:F51"/>
+    <mergeCell ref="G48:G51"/>
+    <mergeCell ref="H48:H51"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="D38:D47"/>
+    <mergeCell ref="E38:E47"/>
+    <mergeCell ref="F38:F47"/>
+    <mergeCell ref="G38:G47"/>
+    <mergeCell ref="H38:H47"/>
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="H28:H30"/>
     <mergeCell ref="D31:D32"/>
@@ -5667,21 +5753,17 @@
     <mergeCell ref="F21:F26"/>
     <mergeCell ref="G21:G26"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D38:D47"/>
-    <mergeCell ref="E38:E47"/>
-    <mergeCell ref="F38:F47"/>
-    <mergeCell ref="G38:G47"/>
-    <mergeCell ref="H38:H47"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="F48:F51"/>
-    <mergeCell ref="G48:G51"/>
-    <mergeCell ref="H48:H51"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E18"/>
+    <mergeCell ref="F4:F18"/>
+    <mergeCell ref="G4:G18"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C33" location="_ftn2" display="_ftn2" xr:uid="{E50DF5A1-13E6-4004-9692-0F820274B734}"/>
@@ -5693,20 +5775,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE037D9D-4E45-4C5B-8392-AE943DD18A55}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="B47" sqref="B47:E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" style="88" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" style="88" customWidth="1"/>
-    <col min="3" max="3" width="61.42578125" style="92" customWidth="1"/>
+    <col min="3" max="3" width="61.42578125" style="91" customWidth="1"/>
     <col min="4" max="4" width="22" style="88" customWidth="1"/>
     <col min="5" max="16384" width="29.7109375" style="88"/>
   </cols>
@@ -5716,7 +5798,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="73" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C1" s="73" t="s">
         <v>2</v>
@@ -5725,759 +5807,822 @@
         <v>3</v>
       </c>
       <c r="E1" s="63" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="127" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="103" t="s">
-        <v>306</v>
-      </c>
-      <c r="C2" s="94" t="s">
-        <v>273</v>
-      </c>
-      <c r="D2" s="95" t="s">
+      <c r="B2" s="102" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" s="93" t="s">
+        <v>272</v>
+      </c>
+      <c r="D2" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="96" t="s">
-        <v>283</v>
-      </c>
-      <c r="F2" s="102" t="s">
-        <v>290</v>
+      <c r="E2" s="95" t="s">
+        <v>279</v>
+      </c>
+      <c r="F2" s="101" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="128"/>
-      <c r="B3" s="104" t="s">
-        <v>307</v>
-      </c>
-      <c r="C3" s="94" t="s">
-        <v>249</v>
-      </c>
-      <c r="D3" s="95" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="96" t="s">
-        <v>283</v>
+      <c r="B3" s="103" t="s">
+        <v>301</v>
+      </c>
+      <c r="C3" s="93" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" s="94" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="95" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="129"/>
-      <c r="B4" s="104" t="s">
-        <v>308</v>
-      </c>
-      <c r="C4" s="94" t="s">
-        <v>288</v>
-      </c>
-      <c r="D4" s="95" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="96" t="s">
-        <v>283</v>
-      </c>
-      <c r="F4" s="100"/>
+      <c r="B4" s="103" t="s">
+        <v>302</v>
+      </c>
+      <c r="C4" s="93" t="s">
+        <v>284</v>
+      </c>
+      <c r="D4" s="94" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="95" t="s">
+        <v>279</v>
+      </c>
+      <c r="F4" s="99"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="127" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="104" t="s">
-        <v>309</v>
-      </c>
-      <c r="C5" s="94" t="s">
-        <v>250</v>
-      </c>
-      <c r="D5" s="95" t="s">
+      <c r="B5" s="103" t="s">
+        <v>303</v>
+      </c>
+      <c r="C5" s="93" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="96" t="s">
-        <v>283</v>
-      </c>
-      <c r="F5" s="102" t="s">
-        <v>290</v>
+      <c r="E5" s="95" t="s">
+        <v>279</v>
+      </c>
+      <c r="F5" s="101" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="129"/>
-      <c r="B6" s="104" t="s">
-        <v>310</v>
-      </c>
-      <c r="C6" s="94" t="s">
-        <v>251</v>
-      </c>
-      <c r="D6" s="95" t="s">
+      <c r="B6" s="103" t="s">
+        <v>304</v>
+      </c>
+      <c r="C6" s="93" t="s">
+        <v>250</v>
+      </c>
+      <c r="D6" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="96" t="s">
-        <v>283</v>
-      </c>
-      <c r="F6" s="102" t="s">
-        <v>290</v>
+      <c r="E6" s="95" t="s">
+        <v>279</v>
+      </c>
+      <c r="F6" s="101" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="105" t="s">
-        <v>322</v>
-      </c>
-      <c r="C7" s="94" t="s">
-        <v>252</v>
-      </c>
-      <c r="D7" s="95" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="96" t="s">
-        <v>283</v>
-      </c>
-      <c r="F7" s="101"/>
+      <c r="B7" s="104" t="s">
+        <v>316</v>
+      </c>
+      <c r="C7" s="93" t="s">
+        <v>251</v>
+      </c>
+      <c r="D7" s="94" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="95" t="s">
+        <v>279</v>
+      </c>
+      <c r="F7" s="100"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="131"/>
-      <c r="B8" s="105" t="s">
-        <v>323</v>
-      </c>
-      <c r="C8" s="94" t="s">
-        <v>253</v>
-      </c>
-      <c r="D8" s="95" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="96" t="s">
-        <v>283</v>
+      <c r="B8" s="104" t="s">
+        <v>317</v>
+      </c>
+      <c r="C8" s="93" t="s">
+        <v>252</v>
+      </c>
+      <c r="D8" s="94" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="95" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="131"/>
-      <c r="B9" s="105" t="s">
-        <v>324</v>
-      </c>
-      <c r="C9" s="94" t="s">
-        <v>254</v>
-      </c>
-      <c r="D9" s="95" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="96" t="s">
-        <v>283</v>
+      <c r="B9" s="104" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9" s="93" t="s">
+        <v>253</v>
+      </c>
+      <c r="D9" s="94" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="95" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="131"/>
-      <c r="B10" s="105" t="s">
-        <v>325</v>
-      </c>
-      <c r="C10" s="94" t="s">
-        <v>289</v>
-      </c>
-      <c r="D10" s="95" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="96" t="s">
-        <v>283</v>
-      </c>
-      <c r="F10" s="100"/>
+      <c r="B10" s="104" t="s">
+        <v>319</v>
+      </c>
+      <c r="C10" s="93" t="s">
+        <v>285</v>
+      </c>
+      <c r="D10" s="94" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="95" t="s">
+        <v>279</v>
+      </c>
+      <c r="F10" s="99"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="131"/>
-      <c r="B11" s="106" t="s">
-        <v>331</v>
-      </c>
-      <c r="C11" s="94" t="s">
-        <v>255</v>
-      </c>
-      <c r="D11" s="95" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="96" t="s">
-        <v>283</v>
+      <c r="B11" s="105" t="s">
+        <v>325</v>
+      </c>
+      <c r="C11" s="93" t="s">
+        <v>254</v>
+      </c>
+      <c r="D11" s="94" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="95" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A12" s="131"/>
-      <c r="B12" s="106" t="s">
-        <v>292</v>
-      </c>
-      <c r="C12" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="D12" s="95" t="s">
+      <c r="B12" s="105" t="s">
+        <v>288</v>
+      </c>
+      <c r="C12" s="93" t="s">
+        <v>281</v>
+      </c>
+      <c r="D12" s="94" t="s">
         <v>119</v>
       </c>
-      <c r="E12" s="96" t="s">
-        <v>283</v>
+      <c r="E12" s="95" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="131"/>
-      <c r="B13" s="106" t="s">
-        <v>333</v>
-      </c>
-      <c r="C13" s="94" t="s">
-        <v>274</v>
-      </c>
-      <c r="D13" s="95" t="s">
+      <c r="B13" s="105" t="s">
+        <v>327</v>
+      </c>
+      <c r="C13" s="93" t="s">
+        <v>273</v>
+      </c>
+      <c r="D13" s="94" t="s">
         <v>119</v>
       </c>
-      <c r="E13" s="96" t="s">
-        <v>283</v>
-      </c>
-      <c r="F13" s="100"/>
+      <c r="E13" s="95" t="s">
+        <v>279</v>
+      </c>
+      <c r="F13" s="99"/>
     </row>
     <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A14" s="131"/>
-      <c r="B14" s="106" t="s">
-        <v>332</v>
-      </c>
-      <c r="C14" s="94" t="s">
+      <c r="B14" s="105" t="s">
+        <v>326</v>
+      </c>
+      <c r="C14" s="93" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="95" t="s">
+      <c r="D14" s="94" t="s">
         <v>119</v>
       </c>
-      <c r="E14" s="96" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="E14" s="95" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="131"/>
-      <c r="B15" s="104" t="s">
-        <v>293</v>
-      </c>
-      <c r="C15" s="91" t="s">
+      <c r="B15" s="141" t="s">
+        <v>289</v>
+      </c>
+      <c r="C15" s="142" t="s">
         <v>127</v>
       </c>
-      <c r="D15" s="89" t="s">
+      <c r="D15" s="143" t="s">
         <v>246</v>
       </c>
-      <c r="E15" s="93" t="s">
-        <v>284</v>
+      <c r="E15" s="144" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="131"/>
-      <c r="B16" s="106" t="s">
-        <v>330</v>
-      </c>
-      <c r="C16" s="94" t="s">
+      <c r="B16" s="105" t="s">
+        <v>324</v>
+      </c>
+      <c r="C16" s="93" t="s">
         <v>139</v>
       </c>
-      <c r="D16" s="95" t="s">
+      <c r="D16" s="94" t="s">
         <v>246</v>
       </c>
-      <c r="E16" s="96" t="s">
-        <v>284</v>
+      <c r="E16" s="95" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A17" s="131"/>
-      <c r="B17" s="106" t="s">
-        <v>334</v>
-      </c>
-      <c r="C17" s="94" t="s">
-        <v>286</v>
-      </c>
-      <c r="D17" s="95" t="s">
+      <c r="B17" s="105" t="s">
+        <v>328</v>
+      </c>
+      <c r="C17" s="93" t="s">
+        <v>282</v>
+      </c>
+      <c r="D17" s="94" t="s">
         <v>246</v>
       </c>
-      <c r="E17" s="96" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="E17" s="95" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A18" s="131"/>
-      <c r="B18" s="106" t="s">
+      <c r="B18" s="105" t="s">
+        <v>329</v>
+      </c>
+      <c r="C18" s="93" t="s">
         <v>335</v>
       </c>
-      <c r="C18" s="94" t="s">
-        <v>276</v>
-      </c>
-      <c r="D18" s="95" t="s">
+      <c r="D18" s="94" t="s">
         <v>246</v>
       </c>
-      <c r="E18" s="96" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="E18" s="95" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A19" s="131"/>
-      <c r="B19" s="106" t="s">
-        <v>336</v>
-      </c>
-      <c r="C19" s="94" t="s">
-        <v>277</v>
-      </c>
-      <c r="D19" s="95" t="s">
+      <c r="B19" s="105" t="s">
+        <v>330</v>
+      </c>
+      <c r="C19" s="93" t="s">
+        <v>333</v>
+      </c>
+      <c r="D19" s="94" t="s">
         <v>246</v>
       </c>
-      <c r="E19" s="96" t="s">
-        <v>284</v>
+      <c r="E19" s="95" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A20" s="131"/>
-      <c r="B20" s="106" t="s">
-        <v>327</v>
-      </c>
-      <c r="C20" s="94" t="s">
-        <v>279</v>
-      </c>
-      <c r="D20" s="95" t="s">
+      <c r="B20" s="105" t="s">
+        <v>321</v>
+      </c>
+      <c r="C20" s="93" t="s">
+        <v>275</v>
+      </c>
+      <c r="D20" s="94" t="s">
         <v>246</v>
       </c>
-      <c r="E20" s="96" t="s">
-        <v>284</v>
+      <c r="E20" s="95" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A21" s="131"/>
-      <c r="B21" s="106" t="s">
-        <v>328</v>
-      </c>
-      <c r="C21" s="94" t="s">
-        <v>275</v>
-      </c>
-      <c r="D21" s="95" t="s">
+      <c r="B21" s="105" t="s">
+        <v>322</v>
+      </c>
+      <c r="C21" s="93" t="s">
+        <v>274</v>
+      </c>
+      <c r="D21" s="94" t="s">
         <v>246</v>
       </c>
-      <c r="E21" s="96" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="E21" s="95" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A22" s="131"/>
-      <c r="B22" s="106" t="s">
-        <v>329</v>
-      </c>
-      <c r="C22" s="94" t="s">
-        <v>278</v>
-      </c>
-      <c r="D22" s="95" t="s">
+      <c r="B22" s="105" t="s">
+        <v>323</v>
+      </c>
+      <c r="C22" s="93" t="s">
+        <v>334</v>
+      </c>
+      <c r="D22" s="94" t="s">
         <v>246</v>
       </c>
-      <c r="E22" s="96" t="s">
-        <v>284</v>
+      <c r="E22" s="95" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A23" s="131"/>
-      <c r="B23" s="106" t="s">
-        <v>337</v>
-      </c>
-      <c r="C23" s="94" t="s">
+      <c r="B23" s="105" t="s">
+        <v>331</v>
+      </c>
+      <c r="C23" s="93" t="s">
+        <v>276</v>
+      </c>
+      <c r="D23" s="94" t="s">
+        <v>246</v>
+      </c>
+      <c r="E23" s="95" t="s">
         <v>280</v>
-      </c>
-      <c r="D23" s="95" t="s">
-        <v>246</v>
-      </c>
-      <c r="E23" s="96" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A24" s="131"/>
-      <c r="B24" s="104" t="s">
-        <v>338</v>
-      </c>
-      <c r="C24" s="94" t="s">
-        <v>272</v>
-      </c>
-      <c r="D24" s="95" t="s">
+      <c r="B24" s="103" t="s">
+        <v>332</v>
+      </c>
+      <c r="C24" s="93" t="s">
+        <v>271</v>
+      </c>
+      <c r="D24" s="94" t="s">
         <v>246</v>
       </c>
-      <c r="E24" s="96" t="s">
-        <v>284</v>
+      <c r="E24" s="95" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="131"/>
-      <c r="B25" s="104" t="s">
-        <v>294</v>
-      </c>
-      <c r="C25" s="90" t="s">
-        <v>281</v>
-      </c>
-      <c r="D25" s="89" t="s">
+      <c r="B25" s="137" t="s">
+        <v>290</v>
+      </c>
+      <c r="C25" s="138" t="s">
+        <v>277</v>
+      </c>
+      <c r="D25" s="139" t="s">
         <v>144</v>
       </c>
-      <c r="E25" s="93" t="s">
-        <v>283</v>
+      <c r="E25" s="140" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="131"/>
-      <c r="B26" s="104" t="s">
-        <v>295</v>
+      <c r="B26" s="103" t="s">
+        <v>291</v>
       </c>
       <c r="C26" s="90" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D26" s="89" t="s">
         <v>144</v>
       </c>
-      <c r="E26" s="93" t="s">
-        <v>283</v>
+      <c r="E26" s="92" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="131"/>
-      <c r="B27" s="104" t="s">
-        <v>296</v>
+      <c r="B27" s="103" t="s">
+        <v>292</v>
       </c>
       <c r="C27" s="90" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D27" s="89" t="s">
         <v>144</v>
       </c>
-      <c r="E27" s="93" t="s">
-        <v>283</v>
+      <c r="E27" s="92" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" s="132"/>
-      <c r="B28" s="104" t="s">
-        <v>297</v>
+      <c r="B28" s="103" t="s">
+        <v>293</v>
       </c>
       <c r="C28" s="90" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D28" s="89" t="s">
         <v>144</v>
       </c>
-      <c r="E28" s="93" t="s">
-        <v>283</v>
+      <c r="E28" s="92" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="130" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="104" t="s">
-        <v>298</v>
+      <c r="B29" s="103" t="s">
+        <v>294</v>
       </c>
       <c r="C29" s="90" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D29" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="E29" s="93" t="s">
-        <v>284</v>
+      <c r="E29" s="92" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="131"/>
-      <c r="B30" s="104" t="s">
-        <v>299</v>
+      <c r="B30" s="103" t="s">
+        <v>295</v>
       </c>
       <c r="C30" s="90" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D30" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="E30" s="93" t="s">
-        <v>284</v>
+      <c r="E30" s="92" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="131"/>
-      <c r="B31" s="104" t="s">
-        <v>300</v>
+      <c r="B31" s="103" t="s">
+        <v>296</v>
       </c>
       <c r="C31" s="90" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D31" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="E31" s="93" t="s">
-        <v>284</v>
+      <c r="E31" s="92" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="131"/>
-      <c r="B32" s="104" t="s">
-        <v>301</v>
+      <c r="B32" s="103" t="s">
+        <v>297</v>
       </c>
       <c r="C32" s="90" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D32" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="E32" s="93" t="s">
-        <v>284</v>
+      <c r="E32" s="92" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="131"/>
-      <c r="B33" s="104" t="s">
-        <v>302</v>
+      <c r="B33" s="103" t="s">
+        <v>298</v>
       </c>
       <c r="C33" s="90" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D33" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="E33" s="93" t="s">
-        <v>284</v>
+      <c r="E33" s="92" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="132"/>
-      <c r="B34" s="104" t="s">
-        <v>303</v>
+      <c r="B34" s="103" t="s">
+        <v>299</v>
       </c>
       <c r="C34" s="90" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D34" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="E34" s="93" t="s">
-        <v>284</v>
+      <c r="E34" s="92" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="127" t="s">
-        <v>287</v>
-      </c>
-      <c r="B35" s="104" t="s">
-        <v>311</v>
-      </c>
-      <c r="C35" s="97" t="s">
-        <v>265</v>
-      </c>
-      <c r="D35" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="99" t="s">
         <v>283</v>
+      </c>
+      <c r="B35" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="C35" s="96" t="s">
+        <v>264</v>
+      </c>
+      <c r="D35" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="98" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="129"/>
-      <c r="B36" s="104" t="s">
-        <v>312</v>
-      </c>
-      <c r="C36" s="97" t="s">
-        <v>266</v>
-      </c>
-      <c r="D36" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" s="99" t="s">
-        <v>283</v>
+      <c r="B36" s="103" t="s">
+        <v>306</v>
+      </c>
+      <c r="C36" s="96" t="s">
+        <v>265</v>
+      </c>
+      <c r="D36" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="98" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="104" t="s">
-        <v>313</v>
-      </c>
-      <c r="C37" s="97" t="s">
-        <v>267</v>
-      </c>
-      <c r="D37" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="99" t="s">
-        <v>283</v>
+      <c r="B37" s="103" t="s">
+        <v>307</v>
+      </c>
+      <c r="C37" s="96" t="s">
+        <v>266</v>
+      </c>
+      <c r="D37" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="98" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="129"/>
-      <c r="B38" s="104" t="s">
-        <v>314</v>
-      </c>
-      <c r="C38" s="97" t="s">
-        <v>268</v>
-      </c>
-      <c r="D38" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="99" t="s">
-        <v>283</v>
+      <c r="B38" s="103" t="s">
+        <v>308</v>
+      </c>
+      <c r="C38" s="96" t="s">
+        <v>267</v>
+      </c>
+      <c r="D38" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="98" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="127" t="s">
         <v>199</v>
       </c>
-      <c r="B39" s="104" t="s">
-        <v>315</v>
-      </c>
-      <c r="C39" s="97" t="s">
-        <v>269</v>
-      </c>
-      <c r="D39" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" s="99" t="s">
-        <v>283</v>
+      <c r="B39" s="103" t="s">
+        <v>309</v>
+      </c>
+      <c r="C39" s="96" t="s">
+        <v>268</v>
+      </c>
+      <c r="D39" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="98" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="128"/>
-      <c r="B40" s="104" t="s">
-        <v>316</v>
-      </c>
-      <c r="C40" s="97" t="s">
-        <v>270</v>
-      </c>
-      <c r="D40" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" s="99" t="s">
-        <v>283</v>
+      <c r="B40" s="103" t="s">
+        <v>310</v>
+      </c>
+      <c r="C40" s="96" t="s">
+        <v>269</v>
+      </c>
+      <c r="D40" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="98" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="128"/>
-      <c r="B41" s="104" t="s">
-        <v>317</v>
-      </c>
-      <c r="C41" s="97" t="s">
-        <v>271</v>
-      </c>
-      <c r="D41" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" s="99" t="s">
-        <v>283</v>
+      <c r="B41" s="103" t="s">
+        <v>311</v>
+      </c>
+      <c r="C41" s="96" t="s">
+        <v>270</v>
+      </c>
+      <c r="D41" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="98" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A42" s="129"/>
-      <c r="B42" s="104" t="s">
-        <v>318</v>
-      </c>
-      <c r="C42" s="97" t="s">
+      <c r="B42" s="103" t="s">
+        <v>312</v>
+      </c>
+      <c r="C42" s="96" t="s">
         <v>245</v>
       </c>
-      <c r="D42" s="98" t="s">
+      <c r="D42" s="97" t="s">
         <v>73</v>
       </c>
-      <c r="E42" s="99" t="s">
-        <v>283</v>
+      <c r="E42" s="98" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="130" t="s">
         <v>198</v>
       </c>
-      <c r="B43" s="106" t="s">
-        <v>326</v>
-      </c>
-      <c r="C43" s="97" t="s">
-        <v>248</v>
-      </c>
-      <c r="D43" s="98" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" s="99" t="s">
-        <v>283</v>
+      <c r="B43" s="105" t="s">
+        <v>320</v>
+      </c>
+      <c r="C43" s="96" t="s">
+        <v>247</v>
+      </c>
+      <c r="D43" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="98" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A44" s="131"/>
-      <c r="B44" s="104" t="s">
-        <v>321</v>
-      </c>
-      <c r="C44" s="97" t="s">
+      <c r="B44" s="103" t="s">
+        <v>315</v>
+      </c>
+      <c r="C44" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="D44" s="98" t="s">
+      <c r="D44" s="97" t="s">
         <v>88</v>
       </c>
-      <c r="E44" s="99" t="s">
-        <v>283</v>
-      </c>
-      <c r="F44" s="102" t="s">
-        <v>290</v>
+      <c r="E44" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="F44" s="101" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="131"/>
-      <c r="B45" s="104" t="s">
-        <v>319</v>
-      </c>
-      <c r="C45" s="97" t="s">
+      <c r="B45" s="103" t="s">
+        <v>313</v>
+      </c>
+      <c r="C45" s="96" t="s">
         <v>87</v>
       </c>
-      <c r="D45" s="98" t="s">
+      <c r="D45" s="97" t="s">
         <v>88</v>
       </c>
-      <c r="E45" s="99" t="s">
-        <v>283</v>
-      </c>
-      <c r="F45" s="102" t="s">
-        <v>290</v>
+      <c r="E45" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="F45" s="101" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="132"/>
-      <c r="B46" s="104" t="s">
-        <v>320</v>
-      </c>
-      <c r="C46" s="97" t="s">
+      <c r="B46" s="103" t="s">
+        <v>314</v>
+      </c>
+      <c r="C46" s="96" t="s">
         <v>100</v>
       </c>
-      <c r="D46" s="98" t="s">
+      <c r="D46" s="97" t="s">
         <v>88</v>
       </c>
-      <c r="E46" s="99" t="s">
-        <v>283</v>
-      </c>
-      <c r="F46" s="102" t="s">
-        <v>290</v>
+      <c r="E46" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="F46" s="101" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="130" t="s">
+      <c r="A47" s="145" t="s">
         <v>151</v>
       </c>
-      <c r="B47" s="104" t="s">
-        <v>304</v>
-      </c>
-      <c r="C47" s="90" t="s">
-        <v>209</v>
-      </c>
-      <c r="D47" s="89" t="s">
+      <c r="B47" s="106" t="s">
+        <v>347</v>
+      </c>
+      <c r="C47" s="96" t="s">
+        <v>336</v>
+      </c>
+      <c r="D47" s="97" t="s">
         <v>62</v>
       </c>
-      <c r="E47" s="93" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="132"/>
-      <c r="B48" s="104" t="s">
-        <v>305</v>
-      </c>
-      <c r="C48" s="90" t="s">
-        <v>247</v>
-      </c>
-      <c r="D48" s="89" t="s">
+      <c r="E47" s="98" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="146"/>
+      <c r="B48" s="106" t="s">
+        <v>346</v>
+      </c>
+      <c r="C48" s="96" t="s">
+        <v>337</v>
+      </c>
+      <c r="D48" s="97" t="s">
         <v>62</v>
       </c>
-      <c r="E48" s="93" t="s">
-        <v>283</v>
-      </c>
+      <c r="E48" s="98" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="146"/>
+      <c r="B49" s="106" t="s">
+        <v>345</v>
+      </c>
+      <c r="C49" s="96" t="s">
+        <v>338</v>
+      </c>
+      <c r="D49" s="97" t="s">
+        <v>62</v>
+      </c>
+      <c r="E49" s="98" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="146"/>
+      <c r="B50" s="106" t="s">
+        <v>344</v>
+      </c>
+      <c r="C50" s="96" t="s">
+        <v>340</v>
+      </c>
+      <c r="D50" s="97" t="s">
+        <v>62</v>
+      </c>
+      <c r="E50" s="98" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="146"/>
+      <c r="B51" s="106" t="s">
+        <v>343</v>
+      </c>
+      <c r="C51" s="96" t="s">
+        <v>341</v>
+      </c>
+      <c r="D51" s="97" t="s">
+        <v>62</v>
+      </c>
+      <c r="E51" s="98" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="147"/>
+      <c r="B52" s="106" t="s">
+        <v>342</v>
+      </c>
+      <c r="C52" s="96" t="s">
+        <v>339</v>
+      </c>
+      <c r="D52" s="97" t="s">
+        <v>62</v>
+      </c>
+      <c r="E52" s="98" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A47:A52"/>
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A47:A48"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A28"/>
@@ -6496,10 +6641,10 @@
   <dimension ref="A2:H55"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomRight" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6841,7 +6986,7 @@
       <c r="G19" s="123" t="s">
         <v>235</v>
       </c>
-      <c r="H19" s="125" t="s">
+      <c r="H19" s="124" t="s">
         <v>234</v>
       </c>
     </row>
@@ -6859,7 +7004,7 @@
       <c r="E20" s="121"/>
       <c r="F20" s="121"/>
       <c r="G20" s="123"/>
-      <c r="H20" s="125"/>
+      <c r="H20" s="124"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
@@ -7081,7 +7226,7 @@
       <c r="G32" s="126" t="s">
         <v>243</v>
       </c>
-      <c r="H32" s="124" t="s">
+      <c r="H32" s="125" t="s">
         <v>242</v>
       </c>
     </row>
@@ -7099,7 +7244,7 @@
       <c r="E33" s="121"/>
       <c r="F33" s="122"/>
       <c r="G33" s="126"/>
-      <c r="H33" s="124"/>
+      <c r="H33" s="125"/>
     </row>
     <row r="34" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="74" t="s">
@@ -7115,7 +7260,7 @@
       <c r="E34" s="121"/>
       <c r="F34" s="122"/>
       <c r="G34" s="126"/>
-      <c r="H34" s="124"/>
+      <c r="H34" s="125"/>
     </row>
     <row r="35" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="80" t="s">
@@ -7137,7 +7282,7 @@
         <v>181</v>
       </c>
       <c r="G35" s="123"/>
-      <c r="H35" s="124"/>
+      <c r="H35" s="125"/>
     </row>
     <row r="36" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="80" t="s">
@@ -7153,7 +7298,7 @@
       <c r="E36" s="121"/>
       <c r="F36" s="121"/>
       <c r="G36" s="123"/>
-      <c r="H36" s="124"/>
+      <c r="H36" s="125"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="81" t="s">
@@ -7225,7 +7370,7 @@
       <c r="G39" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="H39" s="125" t="s">
+      <c r="H39" s="124" t="s">
         <v>236</v>
       </c>
     </row>
@@ -7243,7 +7388,7 @@
       <c r="E40" s="121"/>
       <c r="F40" s="121"/>
       <c r="G40" s="123"/>
-      <c r="H40" s="125"/>
+      <c r="H40" s="124"/>
     </row>
     <row r="41" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A41" s="78" t="s">
@@ -7259,7 +7404,7 @@
       <c r="E41" s="121"/>
       <c r="F41" s="121"/>
       <c r="G41" s="123"/>
-      <c r="H41" s="125"/>
+      <c r="H41" s="124"/>
     </row>
     <row r="42" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="78" t="s">
@@ -7283,7 +7428,7 @@
       <c r="G42" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="H42" s="124" t="s">
+      <c r="H42" s="125" t="s">
         <v>236</v>
       </c>
     </row>
@@ -7301,7 +7446,7 @@
       <c r="E43" s="121"/>
       <c r="F43" s="121"/>
       <c r="G43" s="123"/>
-      <c r="H43" s="124"/>
+      <c r="H43" s="125"/>
     </row>
     <row r="44" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A44" s="78" t="s">
@@ -7317,7 +7462,7 @@
       <c r="E44" s="121"/>
       <c r="F44" s="121"/>
       <c r="G44" s="123"/>
-      <c r="H44" s="124"/>
+      <c r="H44" s="125"/>
     </row>
     <row r="45" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A45" s="78" t="s">
@@ -7333,7 +7478,7 @@
       <c r="E45" s="121"/>
       <c r="F45" s="121"/>
       <c r="G45" s="123"/>
-      <c r="H45" s="124"/>
+      <c r="H45" s="125"/>
     </row>
     <row r="46" spans="1:8" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="78" t="s">
@@ -7349,7 +7494,7 @@
       <c r="E46" s="121"/>
       <c r="F46" s="121"/>
       <c r="G46" s="123"/>
-      <c r="H46" s="124"/>
+      <c r="H46" s="125"/>
     </row>
     <row r="47" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A47" s="78" t="s">
@@ -7365,7 +7510,7 @@
       <c r="E47" s="121"/>
       <c r="F47" s="121"/>
       <c r="G47" s="123"/>
-      <c r="H47" s="124"/>
+      <c r="H47" s="125"/>
     </row>
     <row r="48" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A48" s="78" t="s">
@@ -7381,7 +7526,7 @@
       <c r="E48" s="121"/>
       <c r="F48" s="121"/>
       <c r="G48" s="123"/>
-      <c r="H48" s="124"/>
+      <c r="H48" s="125"/>
     </row>
     <row r="49" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" s="78" t="s">
@@ -7397,7 +7542,7 @@
       <c r="E49" s="121"/>
       <c r="F49" s="121"/>
       <c r="G49" s="123"/>
-      <c r="H49" s="124"/>
+      <c r="H49" s="125"/>
     </row>
     <row r="50" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A50" s="78" t="s">
@@ -7413,7 +7558,7 @@
       <c r="E50" s="121"/>
       <c r="F50" s="121"/>
       <c r="G50" s="123"/>
-      <c r="H50" s="124"/>
+      <c r="H50" s="125"/>
     </row>
     <row r="51" spans="1:8" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="78" t="s">
@@ -7429,7 +7574,7 @@
       <c r="E51" s="121"/>
       <c r="F51" s="121"/>
       <c r="G51" s="123"/>
-      <c r="H51" s="124"/>
+      <c r="H51" s="125"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="78" t="s">
@@ -7453,7 +7598,7 @@
       <c r="G52" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="H52" s="124" t="s">
+      <c r="H52" s="125" t="s">
         <v>236</v>
       </c>
     </row>
@@ -7471,7 +7616,7 @@
       <c r="E53" s="121"/>
       <c r="F53" s="121"/>
       <c r="G53" s="123"/>
-      <c r="H53" s="124"/>
+      <c r="H53" s="125"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="78" t="s">
@@ -7487,7 +7632,7 @@
       <c r="E54" s="121"/>
       <c r="F54" s="121"/>
       <c r="G54" s="123"/>
-      <c r="H54" s="124"/>
+      <c r="H54" s="125"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="78" t="s">
@@ -7503,46 +7648,10 @@
       <c r="E55" s="121"/>
       <c r="F55" s="121"/>
       <c r="G55" s="123"/>
-      <c r="H55" s="124"/>
+      <c r="H55" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E18"/>
-    <mergeCell ref="F4:F18"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="D21:D26"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="F21:F26"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="D42:D51"/>
-    <mergeCell ref="E42:E51"/>
-    <mergeCell ref="F42:F51"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="F52:F55"/>
-    <mergeCell ref="G4:G18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G21:G26"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G32:G34"/>
     <mergeCell ref="G39:G41"/>
     <mergeCell ref="G42:G51"/>
     <mergeCell ref="G52:G55"/>
@@ -7553,6 +7662,42 @@
     <mergeCell ref="H35:H36"/>
     <mergeCell ref="H42:H51"/>
     <mergeCell ref="G35:G36"/>
+    <mergeCell ref="G4:G18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G21:G26"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="D42:D51"/>
+    <mergeCell ref="E42:E51"/>
+    <mergeCell ref="F42:F51"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="F52:F55"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="D21:D26"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="F21:F26"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E18"/>
+    <mergeCell ref="F4:F18"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C37" location="_ftn2" display="_ftn2" xr:uid="{74DB3199-791E-4FED-9C20-E93C69505EA4}"/>

</xml_diff>